<commit_message>
actualización en tabla 16
</commit_message>
<xml_diff>
--- a/data-raw/excel-spreadsheets/table_data.xlsx
+++ b/data-raw/excel-spreadsheets/table_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Documents\GitHub\CNAIM\data-raw\excel-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80A705E-B21F-4FF0-822A-9F168EF402C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97577F23-C057-42F4-B163-FE07A8E84DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" firstSheet="205" activeTab="219" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" firstSheet="16" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -14342,8 +14342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15062,7 +15062,7 @@
         <v>19</v>
       </c>
       <c r="B36">
-        <v>6959</v>
+        <v>8000</v>
       </c>
       <c r="C36">
         <v>4823</v>
@@ -25582,7 +25582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-D000-000000000000}">
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
pasar las demás inputs
se pasaron al español todas las demás entradas
</commit_message>
<xml_diff>
--- a/data-raw/excel-spreadsheets/table_data.xlsx
+++ b/data-raw/excel-spreadsheets/table_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andres\Documents\GitHub\CNAIM\data-raw\excel-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3D0A41-34B6-4A09-984D-B0EC67CEC98F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC97C0B5-480E-43FB-94D8-2228F0A56543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="870" firstSheet="84" activeTab="88" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="870" firstSheet="84" activeTab="93" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -277,7 +277,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6279" uniqueCount="1053">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6315" uniqueCount="1063">
   <si>
     <t>Health Index Asset Category</t>
   </si>
@@ -3504,6 +3504,36 @@
   </si>
   <si>
     <t>Evidencia de corrosión y perforación significativas (por ejemplo, agujeros). Ruptura severa de la pintura con cierta pérdida de galvanizado. Fugas importantes de compuestos. Evidencia de descarga, signos de calentamiento, deterioro/daño del aislamiento.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">por ejemplo, corrosión leve o evidencia de fugas de compuestos (cuando corresponda) </t>
+  </si>
+  <si>
+    <t>por ejemplo, corrosión importante o evidencia de fugas de aceite de bajo nivel (si corresponde)</t>
+  </si>
+  <si>
+    <t>por ejemplo, corrosión leve o evidencia de fugas de aceite de bajo nivel (si corresponde)</t>
+  </si>
+  <si>
+    <t>por ejemplo, defectos observados o potenciales en el mecanismo, aislamiento interno, etc.</t>
+  </si>
+  <si>
+    <t>No hay signos de deterioro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El componente del activo es apto para el servicio continuo. Hay poco deterioro </t>
+  </si>
+  <si>
+    <t>por ejemplo, corrosión o desgaste leve de los componentes</t>
+  </si>
+  <si>
+    <t>por ejemplo, corrosión importante o desgaste excesivo en componentes y rodamientos</t>
+  </si>
+  <si>
+    <t>por ejemplo, corrosión importante o deshilachado de trenzas</t>
+  </si>
+  <si>
+    <t>por ejemplo, corrosión o desgaste leves</t>
   </si>
 </sst>
 </file>
@@ -59806,8 +59836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5800-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60174,10 +60204,10 @@
 
 <file path=xl/worksheets/sheet90.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5900-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="A6" sqref="A6:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60275,6 +60305,57 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C7">
+        <v>1.4</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C8">
+        <v>1.8</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -60283,10 +60364,10 @@
 
 <file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5A00-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60384,6 +60465,57 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C7">
+        <v>1.2</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C8">
+        <v>1.4</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -60392,10 +60524,10 @@
 
 <file path=xl/worksheets/sheet92.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5B00-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B6"/>
+      <selection activeCell="A7" sqref="A7:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60510,6 +60642,74 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C7">
+        <v>0.9</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C9">
+        <v>1.2</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C10">
+        <v>1.4</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>0.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -60518,10 +60718,10 @@
 
 <file path=xl/worksheets/sheet93.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5C00-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="A7" sqref="A7:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60636,6 +60836,74 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C7">
+        <v>0.95</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C10">
+        <v>1.3</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>0.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -60644,10 +60912,10 @@
 
 <file path=xl/worksheets/sheet94.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5D00-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60759,6 +61027,74 @@
         <v>10</v>
       </c>
       <c r="E6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C7">
+        <v>0.95</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C9">
+        <v>1.05</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
tablas 88 y 89
</commit_message>
<xml_diff>
--- a/data-raw/excel-spreadsheets/table_data.xlsx
+++ b/data-raw/excel-spreadsheets/table_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andres\Documents\GitHub\CNAIM\data-raw\excel-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1935ECD2-0D62-4073-93E6-A23170CFEA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D04362EA-7269-4BFE-8B53-00B9692F79BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30345" yWindow="1935" windowWidth="21600" windowHeight="11385" tabRatio="870" firstSheet="84" activeTab="90" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3515,9 +3515,6 @@
     <t>por ejemplo, corrosión leve o evidencia de fugas de aceite de bajo nivel (si corresponde)</t>
   </si>
   <si>
-    <t>por ejemplo, defectos observados o potenciales en el mecanismo, aislamiento interno, etc.</t>
-  </si>
-  <si>
     <t>No hay signos de deterioro</t>
   </si>
   <si>
@@ -3534,6 +3531,9 @@
   </si>
   <si>
     <t>por ejemplo, corrosión o desgaste leves</t>
+  </si>
+  <si>
+    <t>p. ejemplo, defectos observados o potenciales en el mecanismo, aislamiento interno, etc.</t>
   </si>
 </sst>
 </file>
@@ -60207,7 +60207,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60367,7 +60367,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60504,7 +60504,7 @@
         <v>1035</v>
       </c>
       <c r="B8" t="s">
-        <v>1056</v>
+        <v>1062</v>
       </c>
       <c r="C8">
         <v>1.4</v>
@@ -60647,7 +60647,7 @@
         <v>1048</v>
       </c>
       <c r="B7" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="C7">
         <v>0.9</v>
@@ -60664,7 +60664,7 @@
         <v>1033</v>
       </c>
       <c r="B8" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -60681,7 +60681,7 @@
         <v>1034</v>
       </c>
       <c r="B9" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="C9">
         <v>1.2</v>
@@ -60698,7 +60698,7 @@
         <v>1035</v>
       </c>
       <c r="B10" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="C10">
         <v>1.4</v>
@@ -60841,7 +60841,7 @@
         <v>1048</v>
       </c>
       <c r="B7" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="C7">
         <v>0.95</v>
@@ -60858,7 +60858,7 @@
         <v>1033</v>
       </c>
       <c r="B8" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -60875,7 +60875,7 @@
         <v>1034</v>
       </c>
       <c r="B9" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="C9">
         <v>1.1000000000000001</v>
@@ -60892,7 +60892,7 @@
         <v>1035</v>
       </c>
       <c r="B10" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="C10">
         <v>1.3</v>
@@ -61035,7 +61035,7 @@
         <v>1048</v>
       </c>
       <c r="B7" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="C7">
         <v>0.95</v>
@@ -61052,7 +61052,7 @@
         <v>1033</v>
       </c>
       <c r="B8" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -61069,7 +61069,7 @@
         <v>1034</v>
       </c>
       <c r="B9" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C9">
         <v>1.05</v>
@@ -61086,7 +61086,7 @@
         <v>1035</v>
       </c>
       <c r="B10" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="C10">
         <v>1.1000000000000001</v>

</xml_diff>

<commit_message>
Se actualizó table_data.xlsx con nuevos datos
</commit_message>
<xml_diff>
--- a/data-raw/excel-spreadsheets/table_data.xlsx
+++ b/data-raw/excel-spreadsheets/table_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CNAIM\data-raw\excel-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9BCACA-EB8B-4F5D-9936-FE5A4FD88240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5D2EEF-522B-4E6D-864B-2522E22F9693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -277,7 +277,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6335" uniqueCount="1064">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6337" uniqueCount="1066">
   <si>
     <t>Health Index Asset Category</t>
   </si>
@@ -3537,6 +3537,12 @@
   </si>
   <si>
     <t>34,5/13,8kV</t>
+  </si>
+  <si>
+    <t>Generador Convencional</t>
+  </si>
+  <si>
+    <t>Grupo Electrógeno Diésel 13.8kV</t>
   </si>
 </sst>
 </file>
@@ -3643,7 +3649,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3659,6 +3665,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3735,7 +3747,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3801,6 +3813,7 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4183,10 +4196,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B63"/>
+  <dimension ref="A1:B64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64:XFD64"/>
+      <selection activeCell="B64" sqref="A64:B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4698,6 +4711,14 @@
       </c>
       <c r="B63" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="39" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B64" s="39" t="s">
+        <v>1065</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se eliminó archivo .yaml
</commit_message>
<xml_diff>
--- a/data-raw/excel-spreadsheets/table_data.xlsx
+++ b/data-raw/excel-spreadsheets/table_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CNAIM\data-raw\excel-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC860AA-81A2-494E-A822-0CC229761935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3E0831-2C14-4376-8A40-91BA139BC156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -277,7 +277,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6339" uniqueCount="1066">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6342" uniqueCount="1066">
   <si>
     <t>Health Index Asset Category</t>
   </si>
@@ -4198,7 +4198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
@@ -7966,8 +7966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A28" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9548,8 +9548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11323,7 +11323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -12897,7 +12897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C3" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
@@ -52131,7 +52131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
@@ -57356,7 +57356,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -60187,15 +60187,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C15" sqref="B15:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49.33203125" customWidth="1"/>
     <col min="3" max="3" width="30.6640625" customWidth="1"/>
     <col min="4" max="1025" width="8.88671875" customWidth="1"/>
@@ -60352,6 +60352,17 @@
         <v>187</v>
       </c>
       <c r="C14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="39" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B15" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="C15" s="39" t="s">
         <v>177</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización de tablas excel y pof_grupo_electrogeno_13_8kv.R
</commit_message>
<xml_diff>
--- a/data-raw/excel-spreadsheets/table_data.xlsx
+++ b/data-raw/excel-spreadsheets/table_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CNAIM\data-raw\excel-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5EEBAD4-85F2-4D64-8882-10E4AF561EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0C1FC4-990B-47D4-917B-4FEC2CE89130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -3555,12 +3555,6 @@
     <t>Alternador</t>
   </si>
   <si>
-    <t>1. Cubierta de acero, 2. Condición de los rodamientos, 3. Condición del sistema de combustible, 4. Condición del sistema de enfriamiento, 5. Condición del sistema de lubricación, 6. Condición del sistema de inducción de aire, 7. Condición de las culatas de cilíndros, 8. Condición del filtro</t>
-  </si>
-  <si>
-    <t>1. Envolvente, 2. Condición del aislamiento, 3. Condición de los cables y de la caja de terminales, 4. Condición del rotor, 5. Condición del estator</t>
-  </si>
-  <si>
     <t>1. Rendimiento, 2. RPM, 3. Consumo, 4. Freno</t>
   </si>
   <si>
@@ -3589,6 +3583,12 @@
   </si>
   <si>
     <t>Transformador 13.2kV (GM)</t>
+  </si>
+  <si>
+    <t>1. Cubierta de acero, 2. Rodamientos, 3. Sistema de combustible, 4. Sistema de enfriamiento, 5. Sistema de lubricación, 6. Sistema de inducción de aire, 7.Culatas de cilíndros, 8. Filtro</t>
+  </si>
+  <si>
+    <t>1. Cubierta, 2. Aislamiento, 3. Cables y de la caja de terminales, 4. Rotor, 5. Estator</t>
   </si>
 </sst>
 </file>
@@ -4457,7 +4457,7 @@
         <v>26</v>
       </c>
       <c r="B22" s="46" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -8089,8 +8089,8 @@
   </sheetPr>
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:B36"/>
+    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8483,7 +8483,7 @@
         <v>1067</v>
       </c>
       <c r="C35" s="38" t="s">
-        <v>1069</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -8494,7 +8494,7 @@
         <v>1068</v>
       </c>
       <c r="C36" s="38" t="s">
-        <v>1070</v>
+        <v>1080</v>
       </c>
     </row>
   </sheetData>
@@ -11882,7 +11882,7 @@
         <v>1067</v>
       </c>
       <c r="C35" s="38" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -11893,7 +11893,7 @@
         <v>1068</v>
       </c>
       <c r="C36" s="38" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
     </row>
   </sheetData>
@@ -20793,22 +20793,22 @@
         <v>1066</v>
       </c>
       <c r="B19" s="38" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C19" s="38" t="s">
+        <v>1072</v>
+      </c>
+      <c r="D19" s="38" t="s">
         <v>1073</v>
       </c>
-      <c r="C19" s="38" t="s">
+      <c r="E19" s="38" t="s">
         <v>1074</v>
       </c>
-      <c r="D19" s="38" t="s">
+      <c r="F19" s="38" t="s">
         <v>1075</v>
       </c>
-      <c r="E19" s="38" t="s">
+      <c r="G19" s="38" t="s">
         <v>1076</v>
-      </c>
-      <c r="F19" s="38" t="s">
-        <v>1077</v>
-      </c>
-      <c r="G19" s="38" t="s">
-        <v>1078</v>
       </c>
     </row>
   </sheetData>
@@ -51941,8 +51941,8 @@
   </sheetPr>
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView topLeftCell="A52" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -52502,7 +52502,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -53804,7 +53804,7 @@
         <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -53818,7 +53818,7 @@
         <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="D3">
         <v>1.05</v>
@@ -53832,7 +53832,7 @@
         <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="D4">
         <v>1.1000000000000001</v>
@@ -53844,7 +53844,7 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="D5">
         <v>1.4</v>
@@ -53858,7 +53858,7 @@
         <v>400</v>
       </c>
       <c r="C6" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="D6">
         <v>1</v>

</xml_diff>

<commit_message>
Actualización de tabla y pof de grupo electrógeno - Condiciones medidas
</commit_message>
<xml_diff>
--- a/data-raw/excel-spreadsheets/table_data.xlsx
+++ b/data-raw/excel-spreadsheets/table_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CNAIM\data-raw\excel-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0C1FC4-990B-47D4-917B-4FEC2CE89130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DE0A12-364C-4744-B37E-ABF1C095FD67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -259,6 +259,7 @@
     <sheet name="241" sheetId="254" r:id="rId244"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -3555,12 +3556,6 @@
     <t>Alternador</t>
   </si>
   <si>
-    <t>1. Rendimiento, 2. RPM, 3. Consumo, 4. Freno</t>
-  </si>
-  <si>
-    <t>1. Resistencia de aislamiento, 2. Descarga parcial, 3. Secuencia de fases, 4. Vibraciones, 5. Pérdidas, 6. Temperatura del arrollamiento, 7. Xd, Xq, X0, X1, X2, 8. Factor de potencia</t>
-  </si>
-  <si>
     <t>Garantizar el suministro eléctrico como fuente de generación principal, soportando carga continua y variaciones de demanda.</t>
   </si>
   <si>
@@ -3585,10 +3580,16 @@
     <t>Transformador 13.2kV (GM)</t>
   </si>
   <si>
-    <t>1. Cubierta de acero, 2. Rodamientos, 3. Sistema de combustible, 4. Sistema de enfriamiento, 5. Sistema de lubricación, 6. Sistema de inducción de aire, 7.Culatas de cilíndros, 8. Filtro</t>
-  </si>
-  <si>
     <t>1. Cubierta, 2. Aislamiento, 3. Cables y de la caja de terminales, 4. Rotor, 5. Estator</t>
+  </si>
+  <si>
+    <t>1. Cubierta de acero, 2. Rodamientos, 3. Sistema de combustible, 4. Sistema de enfriamiento, 5. Sistema de lubricación, 6. Sistema de inducción de aire, 7. Turbocompresores, 8.Culatas de cilíndros, 9. Filtro</t>
+  </si>
+  <si>
+    <t>1. Rendimiento, 2. Velocidad RPM, 3. Consumo, 4. Freno</t>
+  </si>
+  <si>
+    <t>1. Resistencia de aislamiento, 2. Descargas parciales, 3. Secuencia de fases, 4. Vibraciones, 5. Pérdidas, 6. Temperatura del arrollamiento</t>
   </si>
 </sst>
 </file>
@@ -4457,7 +4458,7 @@
         <v>26</v>
       </c>
       <c r="B22" s="46" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -8089,8 +8090,8 @@
   </sheetPr>
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8483,7 +8484,7 @@
         <v>1067</v>
       </c>
       <c r="C35" s="38" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -8494,7 +8495,7 @@
         <v>1068</v>
       </c>
       <c r="C36" s="38" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
     </row>
   </sheetData>
@@ -9655,7 +9656,7 @@
   </sheetPr>
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A35" sqref="A35:B36"/>
     </sheetView>
   </sheetViews>
@@ -11488,8 +11489,8 @@
   </sheetPr>
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B35" sqref="A35:B36"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11882,7 +11883,7 @@
         <v>1067</v>
       </c>
       <c r="C35" s="38" t="s">
-        <v>1069</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -11893,7 +11894,7 @@
         <v>1068</v>
       </c>
       <c r="C36" s="38" t="s">
-        <v>1070</v>
+        <v>1080</v>
       </c>
     </row>
   </sheetData>
@@ -13087,7 +13088,7 @@
   </sheetPr>
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
@@ -20793,22 +20794,22 @@
         <v>1066</v>
       </c>
       <c r="B19" s="38" t="s">
+        <v>1069</v>
+      </c>
+      <c r="C19" s="38" t="s">
+        <v>1070</v>
+      </c>
+      <c r="D19" s="38" t="s">
         <v>1071</v>
       </c>
-      <c r="C19" s="38" t="s">
+      <c r="E19" s="38" t="s">
         <v>1072</v>
       </c>
-      <c r="D19" s="38" t="s">
+      <c r="F19" s="38" t="s">
         <v>1073</v>
       </c>
-      <c r="E19" s="38" t="s">
+      <c r="G19" s="38" t="s">
         <v>1074</v>
-      </c>
-      <c r="F19" s="38" t="s">
-        <v>1075</v>
-      </c>
-      <c r="G19" s="38" t="s">
-        <v>1076</v>
       </c>
     </row>
   </sheetData>
@@ -53804,7 +53805,7 @@
         <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -53818,7 +53819,7 @@
         <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D3">
         <v>1.05</v>
@@ -53832,7 +53833,7 @@
         <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D4">
         <v>1.1000000000000001</v>
@@ -53844,7 +53845,7 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D5">
         <v>1.4</v>
@@ -53858,7 +53859,7 @@
         <v>400</v>
       </c>
       <c r="C6" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D6">
         <v>1</v>

</xml_diff>

<commit_message>
Actualización table_index con tablas nuevas
</commit_message>
<xml_diff>
--- a/data-raw/excel-spreadsheets/table_data.xlsx
+++ b/data-raw/excel-spreadsheets/table_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CNAIM\data-raw\excel-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DE0A12-364C-4744-B37E-ABF1C095FD67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB1C978-044D-4DFE-8F90-F64B8C4289B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -259,7 +259,6 @@
     <sheet name="241" sheetId="254" r:id="rId244"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -11489,8 +11488,8 @@
   </sheetPr>
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Actualizaciones pof y tablas: Se empieza a agregar transformador de distribución en las tablas
</commit_message>
<xml_diff>
--- a/data-raw/excel-spreadsheets/table_data.xlsx
+++ b/data-raw/excel-spreadsheets/table_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CNAIM\data-raw\excel-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29256C1F-6A77-4E3B-8C09-69228F937CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF7453C-07F1-4DB5-A075-16F1D6466A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" firstSheet="208" activeTab="219" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -302,7 +302,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6615" uniqueCount="1111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6625" uniqueCount="1113">
   <si>
     <t>Health Index Asset Category</t>
   </si>
@@ -3703,6 +3703,12 @@
   </si>
   <si>
     <t>Criterios de Condición: Temperatura</t>
+  </si>
+  <si>
+    <t>1. Condición externa del transformador, 2. Condición de las cajas de cables</t>
+  </si>
+  <si>
+    <t>1. Descargas parciales, 2. Lecturas de temperatura</t>
   </si>
 </sst>
 </file>
@@ -3843,13 +3849,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3926,7 +3932,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4005,10 +4011,13 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4396,8 +4405,8 @@
   </sheetPr>
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4576,10 +4585,10 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="46" t="s">
+      <c r="A22" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="46" t="s">
+      <c r="B22" s="49" t="s">
         <v>1076</v>
       </c>
     </row>
@@ -8210,10 +8219,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="B7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8335,14 +8344,14 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>209</v>
-      </c>
-      <c r="B11" t="s">
-        <v>210</v>
-      </c>
-      <c r="C11" t="s">
-        <v>211</v>
+      <c r="A11" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="49" t="s">
+        <v>177</v>
+      </c>
+      <c r="C11" s="49" t="s">
+        <v>1111</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -8350,21 +8359,21 @@
         <v>209</v>
       </c>
       <c r="B12" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>83</v>
+        <v>209</v>
       </c>
       <c r="B13" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C13" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -8372,37 +8381,37 @@
         <v>83</v>
       </c>
       <c r="B14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>214</v>
+        <v>83</v>
       </c>
       <c r="B15" t="s">
-        <v>177</v>
+        <v>212</v>
       </c>
       <c r="C15" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B16" t="s">
         <v>177</v>
       </c>
       <c r="C16" t="s">
-        <v>862</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B17" t="s">
         <v>177</v>
@@ -8413,29 +8422,29 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B18" t="s">
         <v>177</v>
       </c>
       <c r="C18" t="s">
-        <v>215</v>
+        <v>862</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B19" t="s">
         <v>177</v>
       </c>
       <c r="C19" t="s">
-        <v>862</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B20" t="s">
         <v>177</v>
@@ -8446,29 +8455,29 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B21" t="s">
         <v>177</v>
       </c>
       <c r="C21" t="s">
-        <v>222</v>
+        <v>862</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>3</v>
+        <v>221</v>
       </c>
       <c r="B22" t="s">
         <v>177</v>
       </c>
       <c r="C22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>224</v>
+        <v>3</v>
       </c>
       <c r="B23" t="s">
         <v>177</v>
@@ -8479,7 +8488,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B24" t="s">
         <v>177</v>
@@ -8490,13 +8499,13 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B25" t="s">
-        <v>227</v>
+        <v>177</v>
       </c>
       <c r="C25" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -8504,10 +8513,10 @@
         <v>226</v>
       </c>
       <c r="B26" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C26" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -8515,21 +8524,21 @@
         <v>226</v>
       </c>
       <c r="B27" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C27" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="B28" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C28" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -8537,10 +8546,10 @@
         <v>233</v>
       </c>
       <c r="B29" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C29" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -8548,26 +8557,26 @@
         <v>233</v>
       </c>
       <c r="B30" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C30" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B31" t="s">
-        <v>177</v>
+        <v>231</v>
       </c>
       <c r="C31" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>69</v>
+        <v>234</v>
       </c>
       <c r="B32" t="s">
         <v>177</v>
@@ -8578,18 +8587,18 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>236</v>
+        <v>69</v>
       </c>
       <c r="B33" t="s">
         <v>177</v>
       </c>
       <c r="C33" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B34" t="s">
         <v>177</v>
@@ -8599,14 +8608,14 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="38" t="s">
-        <v>1066</v>
-      </c>
-      <c r="B35" s="38" t="s">
-        <v>1067</v>
-      </c>
-      <c r="C35" s="38" t="s">
-        <v>1078</v>
+      <c r="A35" t="s">
+        <v>238</v>
+      </c>
+      <c r="B35" t="s">
+        <v>177</v>
+      </c>
+      <c r="C35" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -8614,9 +8623,20 @@
         <v>1066</v>
       </c>
       <c r="B36" s="38" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C36" s="38" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="38" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B37" s="38" t="s">
         <v>1068</v>
       </c>
-      <c r="C36" s="38" t="s">
+      <c r="C37" s="38" t="s">
         <v>1077</v>
       </c>
     </row>
@@ -9778,7 +9798,7 @@
   </sheetPr>
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A35" sqref="A35:B36"/>
     </sheetView>
   </sheetViews>
@@ -11634,10 +11654,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11759,14 +11779,14 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>209</v>
-      </c>
-      <c r="B11" t="s">
-        <v>210</v>
-      </c>
-      <c r="C11" t="s">
-        <v>246</v>
+      <c r="A11" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="49" t="s">
+        <v>177</v>
+      </c>
+      <c r="C11" s="49" t="s">
+        <v>1112</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -11774,21 +11794,21 @@
         <v>209</v>
       </c>
       <c r="B12" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>209</v>
       </c>
       <c r="B13" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -11796,37 +11816,37 @@
         <v>82</v>
       </c>
       <c r="B14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C14" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>214</v>
+        <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>177</v>
+        <v>212</v>
       </c>
       <c r="C15" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B16" t="s">
         <v>177</v>
       </c>
       <c r="C16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B17" t="s">
         <v>177</v>
@@ -11837,29 +11857,29 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B18" t="s">
         <v>177</v>
       </c>
       <c r="C18" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B19" t="s">
         <v>177</v>
       </c>
       <c r="C19" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B20" t="s">
         <v>177</v>
@@ -11870,29 +11890,29 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B21" t="s">
         <v>177</v>
       </c>
       <c r="C21" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>3</v>
+        <v>221</v>
       </c>
       <c r="B22" t="s">
         <v>177</v>
       </c>
       <c r="C22" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>224</v>
+        <v>3</v>
       </c>
       <c r="B23" t="s">
         <v>177</v>
@@ -11903,7 +11923,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B24" t="s">
         <v>177</v>
@@ -11914,13 +11934,13 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B25" t="s">
-        <v>227</v>
+        <v>177</v>
       </c>
       <c r="C25" t="s">
-        <v>215</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -11928,7 +11948,7 @@
         <v>226</v>
       </c>
       <c r="B26" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C26" t="s">
         <v>215</v>
@@ -11939,7 +11959,7 @@
         <v>226</v>
       </c>
       <c r="B27" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C27" t="s">
         <v>215</v>
@@ -11947,10 +11967,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="B28" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C28" t="s">
         <v>215</v>
@@ -11961,7 +11981,7 @@
         <v>233</v>
       </c>
       <c r="B29" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C29" t="s">
         <v>215</v>
@@ -11972,7 +11992,7 @@
         <v>233</v>
       </c>
       <c r="B30" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C30" t="s">
         <v>215</v>
@@ -11980,18 +12000,18 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B31" t="s">
-        <v>177</v>
+        <v>231</v>
       </c>
       <c r="C31" t="s">
-        <v>252</v>
+        <v>215</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>69</v>
+        <v>234</v>
       </c>
       <c r="B32" t="s">
         <v>177</v>
@@ -12002,18 +12022,18 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>236</v>
+        <v>69</v>
       </c>
       <c r="B33" t="s">
         <v>177</v>
       </c>
       <c r="C33" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B34" t="s">
         <v>177</v>
@@ -12023,14 +12043,14 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="38" t="s">
-        <v>1066</v>
-      </c>
-      <c r="B35" s="38" t="s">
-        <v>1067</v>
-      </c>
-      <c r="C35" s="38" t="s">
-        <v>1079</v>
+      <c r="A35" t="s">
+        <v>238</v>
+      </c>
+      <c r="B35" t="s">
+        <v>177</v>
+      </c>
+      <c r="C35" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -12038,9 +12058,20 @@
         <v>1066</v>
       </c>
       <c r="B36" s="38" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C36" s="38" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="38" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B37" s="38" t="s">
         <v>1068</v>
       </c>
-      <c r="C36" s="38" t="s">
+      <c r="C37" s="38" t="s">
         <v>1080</v>
       </c>
     </row>
@@ -13137,8 +13168,8 @@
   </sheetPr>
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14894,10 +14925,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView topLeftCell="A49" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16072,122 +16103,142 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>28</v>
-      </c>
-      <c r="B59">
-        <v>10585</v>
-      </c>
-      <c r="C59">
+      <c r="A59" s="49" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B59" s="49">
+        <v>9297</v>
+      </c>
+      <c r="C59" s="49">
         <v>4823</v>
       </c>
-      <c r="D59">
+      <c r="D59" s="49">
         <v>3809</v>
       </c>
-      <c r="E59">
+      <c r="E59" s="49">
         <v>4343</v>
       </c>
-      <c r="F59">
-        <v>23560</v>
+      <c r="F59" s="49">
+        <v>22271</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
+        <v>28</v>
+      </c>
+      <c r="B60">
+        <v>10585</v>
+      </c>
+      <c r="C60">
+        <v>4823</v>
+      </c>
+      <c r="D60">
+        <v>3809</v>
+      </c>
+      <c r="E60">
+        <v>4343</v>
+      </c>
+      <c r="F60">
+        <v>23560</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>66</v>
       </c>
-      <c r="B60" s="41">
+      <c r="B61" s="41">
         <v>134796</v>
       </c>
-      <c r="C60">
+      <c r="C61">
         <v>23502</v>
       </c>
-      <c r="D60">
+      <c r="D61">
         <v>17048</v>
       </c>
-      <c r="E60">
+      <c r="E61">
         <v>28940</v>
       </c>
-      <c r="F60">
+      <c r="F61">
         <v>157188</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="25" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="25" t="s">
         <v>1020</v>
       </c>
-      <c r="B61" s="40">
+      <c r="B62" s="40">
         <v>134796</v>
       </c>
-      <c r="C61" s="25">
+      <c r="C62" s="25">
         <v>23502</v>
       </c>
-      <c r="D61" s="25">
+      <c r="D62" s="25">
         <v>17048</v>
       </c>
-      <c r="E61" s="25">
+      <c r="E62" s="25">
         <v>28940</v>
       </c>
-      <c r="F61" s="25">
+      <c r="F62" s="25">
         <v>157188</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>67</v>
-      </c>
-      <c r="B62">
-        <v>263015</v>
-      </c>
-      <c r="C62">
-        <v>23502</v>
-      </c>
-      <c r="D62">
-        <v>17048</v>
-      </c>
-      <c r="E62">
-        <v>28940</v>
-      </c>
-      <c r="F62">
-        <v>204285</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>67</v>
+      </c>
+      <c r="B63">
+        <v>263015</v>
+      </c>
+      <c r="C63">
+        <v>23502</v>
+      </c>
+      <c r="D63">
+        <v>17048</v>
+      </c>
+      <c r="E63">
+        <v>28940</v>
+      </c>
+      <c r="F63">
+        <v>204285</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>83</v>
       </c>
-      <c r="B63">
+      <c r="B64">
         <v>218932</v>
       </c>
-      <c r="C63">
+      <c r="C64">
         <v>36171</v>
       </c>
-      <c r="D63">
+      <c r="D64">
         <v>35095</v>
       </c>
-      <c r="E63">
+      <c r="E64">
         <v>230441</v>
       </c>
-      <c r="F63">
+      <c r="F64">
         <v>564721</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="38" t="s">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="38" t="s">
         <v>1064</v>
       </c>
-      <c r="B64" s="38">
+      <c r="B65" s="38">
         <v>87698</v>
       </c>
-      <c r="C64" s="38">
+      <c r="C65" s="38">
         <v>23502</v>
       </c>
-      <c r="D64" s="38">
+      <c r="D65" s="38">
         <v>17048</v>
       </c>
-      <c r="E64" s="38">
+      <c r="E65" s="38">
         <v>28940</v>
       </c>
-      <c r="F64" s="38">
+      <c r="F65" s="38">
         <v>157188</v>
       </c>
     </row>
@@ -19962,8 +20013,8 @@
   </sheetPr>
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:C27"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21985,10 +22036,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:C147"/>
+  <dimension ref="A1:C148"/>
   <sheetViews>
-    <sheetView topLeftCell="A136" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A147" sqref="A147"/>
+    <sheetView topLeftCell="A70" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22320,19 +22371,17 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>28</v>
-      </c>
-      <c r="C35">
+      <c r="A35" s="49" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B35" s="49"/>
+      <c r="C35" s="49">
         <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>30</v>
-      </c>
-      <c r="B36" t="s">
-        <v>358</v>
+        <v>28</v>
       </c>
       <c r="C36">
         <v>60</v>
@@ -22343,10 +22392,10 @@
         <v>30</v>
       </c>
       <c r="B37" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C37">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -22354,10 +22403,10 @@
         <v>30</v>
       </c>
       <c r="B38" t="s">
-        <v>866</v>
+        <v>359</v>
       </c>
       <c r="C38">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -22365,10 +22414,10 @@
         <v>30</v>
       </c>
       <c r="B39" t="s">
-        <v>360</v>
+        <v>866</v>
       </c>
       <c r="C39">
-        <v>55</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -22376,21 +22425,21 @@
         <v>30</v>
       </c>
       <c r="B40" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C40">
-        <v>80</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B41" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="C41">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -22398,10 +22447,10 @@
         <v>31</v>
       </c>
       <c r="B42" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C42">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -22409,10 +22458,10 @@
         <v>31</v>
       </c>
       <c r="B43" t="s">
-        <v>866</v>
+        <v>359</v>
       </c>
       <c r="C43">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -22420,10 +22469,10 @@
         <v>31</v>
       </c>
       <c r="B44" t="s">
-        <v>360</v>
+        <v>866</v>
       </c>
       <c r="C44">
-        <v>55</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -22431,21 +22480,21 @@
         <v>31</v>
       </c>
       <c r="B45" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C45">
-        <v>80</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B46" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C46">
-        <v>55</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -22453,10 +22502,10 @@
         <v>36</v>
       </c>
       <c r="B47" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C47">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -22464,10 +22513,10 @@
         <v>36</v>
       </c>
       <c r="B48" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C48">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -22475,10 +22524,10 @@
         <v>36</v>
       </c>
       <c r="B49" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C49">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -22486,10 +22535,10 @@
         <v>36</v>
       </c>
       <c r="B50" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C50">
-        <v>70</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -22497,21 +22546,21 @@
         <v>36</v>
       </c>
       <c r="B51" t="s">
-        <v>141</v>
+        <v>366</v>
       </c>
       <c r="C51">
-        <v>50</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B52" t="s">
-        <v>367</v>
+        <v>141</v>
       </c>
       <c r="C52">
-        <v>80</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -22519,10 +22568,10 @@
         <v>39</v>
       </c>
       <c r="B53" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C53">
-        <v>95</v>
+        <v>80</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
@@ -22530,10 +22579,10 @@
         <v>39</v>
       </c>
       <c r="B54" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C54">
-        <v>60</v>
+        <v>95</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -22541,10 +22590,10 @@
         <v>39</v>
       </c>
       <c r="B55" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C55">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -22552,29 +22601,29 @@
         <v>39</v>
       </c>
       <c r="B56" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C56">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>33</v>
+        <v>39</v>
+      </c>
+      <c r="B57" t="s">
+        <v>371</v>
       </c>
       <c r="C57">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>37</v>
-      </c>
-      <c r="B58" t="s">
-        <v>362</v>
+        <v>33</v>
       </c>
       <c r="C58">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
@@ -22582,10 +22631,10 @@
         <v>37</v>
       </c>
       <c r="B59" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C59">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -22593,10 +22642,10 @@
         <v>37</v>
       </c>
       <c r="B60" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C60">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -22604,10 +22653,10 @@
         <v>37</v>
       </c>
       <c r="B61" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C61">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -22615,10 +22664,10 @@
         <v>37</v>
       </c>
       <c r="B62" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C62">
-        <v>70</v>
+        <v>50</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -22626,21 +22675,21 @@
         <v>37</v>
       </c>
       <c r="B63" t="s">
-        <v>141</v>
+        <v>366</v>
       </c>
       <c r="C63">
-        <v>50</v>
+        <v>70</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B64" t="s">
-        <v>367</v>
+        <v>141</v>
       </c>
       <c r="C64">
-        <v>80</v>
+        <v>50</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -22648,10 +22697,10 @@
         <v>40</v>
       </c>
       <c r="B65" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C65">
-        <v>95</v>
+        <v>80</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -22659,10 +22708,10 @@
         <v>40</v>
       </c>
       <c r="B66" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C66">
-        <v>60</v>
+        <v>95</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -22670,10 +22719,10 @@
         <v>40</v>
       </c>
       <c r="B67" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C67">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
@@ -22681,29 +22730,29 @@
         <v>40</v>
       </c>
       <c r="B68" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C68">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>34</v>
+        <v>40</v>
+      </c>
+      <c r="B69" t="s">
+        <v>371</v>
       </c>
       <c r="C69">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>45</v>
-      </c>
-      <c r="B70" t="s">
-        <v>372</v>
+        <v>34</v>
       </c>
       <c r="C70">
-        <v>100</v>
+        <v>40</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
@@ -22711,7 +22760,7 @@
         <v>45</v>
       </c>
       <c r="B71" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C71">
         <v>100</v>
@@ -22722,7 +22771,7 @@
         <v>45</v>
       </c>
       <c r="B72" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C72">
         <v>100</v>
@@ -22733,7 +22782,7 @@
         <v>45</v>
       </c>
       <c r="B73" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C73">
         <v>100</v>
@@ -22741,13 +22790,13 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B74" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="C74">
-        <v>75</v>
+        <v>100</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
@@ -22755,7 +22804,7 @@
         <v>48</v>
       </c>
       <c r="B75" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C75">
         <v>75</v>
@@ -22766,10 +22815,10 @@
         <v>48</v>
       </c>
       <c r="B76" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C76">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
@@ -22777,7 +22826,7 @@
         <v>48</v>
       </c>
       <c r="B77" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C77">
         <v>80</v>
@@ -22785,13 +22834,13 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B78" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="C78">
-        <v>65</v>
+        <v>80</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
@@ -22799,10 +22848,10 @@
         <v>42</v>
       </c>
       <c r="B79" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C79">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
@@ -22810,10 +22859,10 @@
         <v>42</v>
       </c>
       <c r="B80" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C80">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
@@ -22821,7 +22870,7 @@
         <v>42</v>
       </c>
       <c r="B81" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C81">
         <v>75</v>
@@ -22829,13 +22878,13 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B82" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="C82">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
@@ -22843,7 +22892,7 @@
         <v>46</v>
       </c>
       <c r="B83" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C83">
         <v>100</v>
@@ -22854,7 +22903,7 @@
         <v>46</v>
       </c>
       <c r="B84" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C84">
         <v>100</v>
@@ -22865,7 +22914,7 @@
         <v>46</v>
       </c>
       <c r="B85" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C85">
         <v>100</v>
@@ -22873,13 +22922,13 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B86" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="C86">
-        <v>75</v>
+        <v>100</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
@@ -22887,7 +22936,7 @@
         <v>49</v>
       </c>
       <c r="B87" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C87">
         <v>75</v>
@@ -22898,10 +22947,10 @@
         <v>49</v>
       </c>
       <c r="B88" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C88">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
@@ -22909,7 +22958,7 @@
         <v>49</v>
       </c>
       <c r="B89" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C89">
         <v>80</v>
@@ -22917,13 +22966,13 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B90" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="C90">
-        <v>65</v>
+        <v>80</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
@@ -22931,10 +22980,10 @@
         <v>43</v>
       </c>
       <c r="B91" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C91">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
@@ -22942,10 +22991,10 @@
         <v>43</v>
       </c>
       <c r="B92" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C92">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
@@ -22953,7 +23002,7 @@
         <v>43</v>
       </c>
       <c r="B93" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C93">
         <v>75</v>
@@ -22961,15 +23010,18 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>52</v>
+        <v>43</v>
+      </c>
+      <c r="B94" t="s">
+        <v>375</v>
       </c>
       <c r="C94">
-        <v>60</v>
+        <v>75</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C95">
         <v>60</v>
@@ -22977,39 +23029,39 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C96">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>376</v>
+        <v>56</v>
       </c>
       <c r="C97">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C98">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>60</v>
+        <v>377</v>
       </c>
       <c r="C99">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C100">
         <v>55</v>
@@ -23017,23 +23069,23 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C101">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C102">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>378</v>
+        <v>62</v>
       </c>
       <c r="C103">
         <v>55</v>
@@ -23041,21 +23093,18 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C104">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>66</v>
-      </c>
-      <c r="B105" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C105">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
@@ -23063,21 +23112,21 @@
         <v>66</v>
       </c>
       <c r="B106" t="s">
+        <v>380</v>
+      </c>
+      <c r="C106">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>66</v>
+      </c>
+      <c r="B107" t="s">
         <v>381</v>
       </c>
-      <c r="C106">
+      <c r="C107">
         <v>50</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A107" s="26" t="s">
-        <v>1020</v>
-      </c>
-      <c r="B107" s="25" t="s">
-        <v>380</v>
-      </c>
-      <c r="C107" s="25">
-        <v>60</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
@@ -23085,26 +23134,26 @@
         <v>1020</v>
       </c>
       <c r="B108" s="25" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C108" s="25">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="26" t="s">
         <v>1020</v>
       </c>
-      <c r="B109" t="s">
-        <v>212</v>
-      </c>
-      <c r="C109">
-        <v>60</v>
+      <c r="B109" s="25" t="s">
+        <v>381</v>
+      </c>
+      <c r="C109" s="25">
+        <v>50</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
-        <v>66</v>
+      <c r="A110" s="26" t="s">
+        <v>1020</v>
       </c>
       <c r="B110" t="s">
         <v>212</v>
@@ -23115,10 +23164,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B111" t="s">
-        <v>380</v>
+        <v>212</v>
       </c>
       <c r="C111">
         <v>60</v>
@@ -23129,10 +23178,10 @@
         <v>67</v>
       </c>
       <c r="B112" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C112">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
@@ -23140,21 +23189,21 @@
         <v>67</v>
       </c>
       <c r="B113" t="s">
-        <v>212</v>
+        <v>381</v>
       </c>
       <c r="C113">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B114" t="s">
-        <v>362</v>
+        <v>212</v>
       </c>
       <c r="C114">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
@@ -23162,10 +23211,10 @@
         <v>71</v>
       </c>
       <c r="B115" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C115">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
@@ -23173,10 +23222,10 @@
         <v>71</v>
       </c>
       <c r="B116" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C116">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
@@ -23184,10 +23233,10 @@
         <v>71</v>
       </c>
       <c r="B117" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C117">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
@@ -23195,10 +23244,10 @@
         <v>71</v>
       </c>
       <c r="B118" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C118">
-        <v>70</v>
+        <v>50</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
@@ -23206,21 +23255,21 @@
         <v>71</v>
       </c>
       <c r="B119" t="s">
-        <v>141</v>
+        <v>366</v>
       </c>
       <c r="C119">
-        <v>50</v>
+        <v>70</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B120" t="s">
-        <v>367</v>
+        <v>141</v>
       </c>
       <c r="C120">
-        <v>80</v>
+        <v>50</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
@@ -23228,10 +23277,10 @@
         <v>73</v>
       </c>
       <c r="B121" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C121">
-        <v>95</v>
+        <v>80</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
@@ -23239,10 +23288,10 @@
         <v>73</v>
       </c>
       <c r="B122" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C122">
-        <v>60</v>
+        <v>95</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
@@ -23250,10 +23299,10 @@
         <v>73</v>
       </c>
       <c r="B123" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C123">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
@@ -23261,29 +23310,29 @@
         <v>73</v>
       </c>
       <c r="B124" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C124">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>69</v>
+        <v>73</v>
+      </c>
+      <c r="B125" t="s">
+        <v>371</v>
       </c>
       <c r="C125">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>75</v>
-      </c>
-      <c r="B126" t="s">
-        <v>372</v>
+        <v>69</v>
       </c>
       <c r="C126">
-        <v>100</v>
+        <v>40</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
@@ -23291,7 +23340,7 @@
         <v>75</v>
       </c>
       <c r="B127" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C127">
         <v>100</v>
@@ -23302,7 +23351,7 @@
         <v>75</v>
       </c>
       <c r="B128" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C128">
         <v>100</v>
@@ -23313,7 +23362,7 @@
         <v>75</v>
       </c>
       <c r="B129" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C129">
         <v>100</v>
@@ -23321,13 +23370,13 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B130" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="C130">
-        <v>75</v>
+        <v>100</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
@@ -23335,7 +23384,7 @@
         <v>76</v>
       </c>
       <c r="B131" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C131">
         <v>75</v>
@@ -23346,10 +23395,10 @@
         <v>76</v>
       </c>
       <c r="B132" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C132">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
@@ -23357,7 +23406,7 @@
         <v>76</v>
       </c>
       <c r="B133" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C133">
         <v>80</v>
@@ -23365,13 +23414,13 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B134" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="C134">
-        <v>65</v>
+        <v>80</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
@@ -23379,10 +23428,10 @@
         <v>74</v>
       </c>
       <c r="B135" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C135">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
@@ -23390,10 +23439,10 @@
         <v>74</v>
       </c>
       <c r="B136" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C136">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
@@ -23401,7 +23450,7 @@
         <v>74</v>
       </c>
       <c r="B137" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C137">
         <v>75</v>
@@ -23409,15 +23458,18 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>53</v>
+        <v>74</v>
+      </c>
+      <c r="B138" t="s">
+        <v>375</v>
       </c>
       <c r="C138">
-        <v>60</v>
+        <v>75</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="C139">
         <v>60</v>
@@ -23425,37 +23477,34 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C140">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C141">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C142">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>83</v>
-      </c>
-      <c r="B143" t="s">
-        <v>380</v>
+        <v>81</v>
       </c>
       <c r="C143">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
@@ -23463,10 +23512,10 @@
         <v>83</v>
       </c>
       <c r="B144" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C144">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
@@ -23474,21 +23523,21 @@
         <v>83</v>
       </c>
       <c r="B145" t="s">
+        <v>381</v>
+      </c>
+      <c r="C145">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>83</v>
+      </c>
+      <c r="B146" t="s">
         <v>212</v>
       </c>
-      <c r="C145">
+      <c r="C146">
         <v>60</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A146" s="38" t="s">
-        <v>1064</v>
-      </c>
-      <c r="B146" s="38" t="s">
-        <v>1067</v>
-      </c>
-      <c r="C146" s="38">
-        <v>20</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
@@ -23496,9 +23545,20 @@
         <v>1064</v>
       </c>
       <c r="B147" s="38" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C147" s="38">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A148" s="38" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B148" s="38" t="s">
         <v>1068</v>
       </c>
-      <c r="C147" s="38">
+      <c r="C148" s="38">
         <v>20</v>
       </c>
     </row>
@@ -24973,7 +25033,7 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -24986,79 +25046,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="46" t="s">
         <v>1087</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="46" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="46" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="46" t="s">
         <v>1083</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="46" t="s">
         <v>1084</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="47" t="s">
         <v>1088</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48">
+      <c r="B2" s="47"/>
+      <c r="C2" s="47">
         <v>1</v>
       </c>
-      <c r="D2" s="48">
-        <v>10</v>
-      </c>
-      <c r="E2" s="48">
+      <c r="D2" s="47">
+        <v>10</v>
+      </c>
+      <c r="E2" s="47">
         <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="47" t="s">
         <v>1089</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48">
+      <c r="B3" s="47"/>
+      <c r="C3" s="47">
         <v>1.3</v>
       </c>
-      <c r="D3" s="48">
-        <v>10</v>
-      </c>
-      <c r="E3" s="48">
+      <c r="D3" s="47">
+        <v>10</v>
+      </c>
+      <c r="E3" s="47">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="47" t="s">
         <v>1090</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48">
+      <c r="B4" s="47"/>
+      <c r="C4" s="47">
         <v>1.6</v>
       </c>
-      <c r="D4" s="48">
-        <v>10</v>
-      </c>
-      <c r="E4" s="48">
+      <c r="D4" s="47">
+        <v>10</v>
+      </c>
+      <c r="E4" s="47">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="47" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48">
+      <c r="B5" s="47"/>
+      <c r="C5" s="47">
         <v>1</v>
       </c>
-      <c r="D5" s="48">
-        <v>10</v>
-      </c>
-      <c r="E5" s="48">
+      <c r="D5" s="47">
+        <v>10</v>
+      </c>
+      <c r="E5" s="47">
         <v>0.5</v>
       </c>
     </row>
@@ -25090,79 +25150,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="46" t="s">
         <v>1102</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="46" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="46" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="46" t="s">
         <v>1083</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="46" t="s">
         <v>1084</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="47" t="s">
         <v>1091</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48">
+      <c r="B2" s="47"/>
+      <c r="C2" s="47">
         <v>1</v>
       </c>
-      <c r="D2" s="48">
-        <v>10</v>
-      </c>
-      <c r="E2" s="48">
+      <c r="D2" s="47">
+        <v>10</v>
+      </c>
+      <c r="E2" s="47">
         <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="47" t="s">
         <v>1092</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48">
+      <c r="B3" s="47"/>
+      <c r="C3" s="47">
         <v>1.3</v>
       </c>
-      <c r="D3" s="48">
-        <v>10</v>
-      </c>
-      <c r="E3" s="48">
+      <c r="D3" s="47">
+        <v>10</v>
+      </c>
+      <c r="E3" s="47">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="47" t="s">
         <v>1093</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48">
+      <c r="B4" s="47"/>
+      <c r="C4" s="47">
         <v>1.6</v>
       </c>
-      <c r="D4" s="48">
-        <v>10</v>
-      </c>
-      <c r="E4" s="48">
+      <c r="D4" s="47">
+        <v>10</v>
+      </c>
+      <c r="E4" s="47">
         <v>5.5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="47" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48">
+      <c r="B5" s="47"/>
+      <c r="C5" s="47">
         <v>1</v>
       </c>
-      <c r="D5" s="48">
-        <v>10</v>
-      </c>
-      <c r="E5" s="48">
+      <c r="D5" s="47">
+        <v>10</v>
+      </c>
+      <c r="E5" s="47">
         <v>0.5</v>
       </c>
     </row>
@@ -25194,79 +25254,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="46" t="s">
         <v>1103</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="46" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="46" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="46" t="s">
         <v>1083</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="46" t="s">
         <v>1084</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="47" t="s">
         <v>1088</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48">
+      <c r="B2" s="47"/>
+      <c r="C2" s="47">
         <v>1</v>
       </c>
-      <c r="D2" s="48">
-        <v>10</v>
-      </c>
-      <c r="E2" s="48">
+      <c r="D2" s="47">
+        <v>10</v>
+      </c>
+      <c r="E2" s="47">
         <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="47" t="s">
         <v>1094</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48">
+      <c r="B3" s="47"/>
+      <c r="C3" s="47">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D3" s="48">
-        <v>10</v>
-      </c>
-      <c r="E3" s="48">
+      <c r="D3" s="47">
+        <v>10</v>
+      </c>
+      <c r="E3" s="47">
         <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="47" t="s">
         <v>1095</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48">
+      <c r="B4" s="47"/>
+      <c r="C4" s="47">
         <v>1.5</v>
       </c>
-      <c r="D4" s="48">
-        <v>10</v>
-      </c>
-      <c r="E4" s="48">
+      <c r="D4" s="47">
+        <v>10</v>
+      </c>
+      <c r="E4" s="47">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="47" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48">
+      <c r="B5" s="47"/>
+      <c r="C5" s="47">
         <v>1</v>
       </c>
-      <c r="D5" s="48">
-        <v>10</v>
-      </c>
-      <c r="E5" s="48">
+      <c r="D5" s="47">
+        <v>10</v>
+      </c>
+      <c r="E5" s="47">
         <v>0.5</v>
       </c>
     </row>
@@ -25298,79 +25358,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="46" t="s">
         <v>1104</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="46" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="46" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="46" t="s">
         <v>1083</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="46" t="s">
         <v>1084</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="47" t="s">
         <v>1096</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48">
+      <c r="B2" s="47"/>
+      <c r="C2" s="47">
         <v>1</v>
       </c>
-      <c r="D2" s="48">
-        <v>10</v>
-      </c>
-      <c r="E2" s="48">
+      <c r="D2" s="47">
+        <v>10</v>
+      </c>
+      <c r="E2" s="47">
         <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="47" t="s">
         <v>1097</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48">
+      <c r="B3" s="47"/>
+      <c r="C3" s="47">
         <v>1.3</v>
       </c>
-      <c r="D3" s="48">
-        <v>10</v>
-      </c>
-      <c r="E3" s="48">
+      <c r="D3" s="47">
+        <v>10</v>
+      </c>
+      <c r="E3" s="47">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="47" t="s">
         <v>1098</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48">
+      <c r="B4" s="47"/>
+      <c r="C4" s="47">
         <v>1.6</v>
       </c>
-      <c r="D4" s="48">
-        <v>10</v>
-      </c>
-      <c r="E4" s="48">
+      <c r="D4" s="47">
+        <v>10</v>
+      </c>
+      <c r="E4" s="47">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="47" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48">
+      <c r="B5" s="47"/>
+      <c r="C5" s="47">
         <v>1</v>
       </c>
-      <c r="D5" s="48">
-        <v>10</v>
-      </c>
-      <c r="E5" s="48">
+      <c r="D5" s="47">
+        <v>10</v>
+      </c>
+      <c r="E5" s="47">
         <v>0.5</v>
       </c>
     </row>
@@ -25402,94 +25462,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="46" t="s">
         <v>1105</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="46" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="46" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="46" t="s">
         <v>1083</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="46" t="s">
         <v>1084</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="47" t="s">
         <v>1021</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="49">
+      <c r="B2" s="47"/>
+      <c r="C2" s="48">
         <v>1</v>
       </c>
-      <c r="D2" s="49">
-        <v>10</v>
-      </c>
-      <c r="E2" s="49">
+      <c r="D2" s="48">
+        <v>10</v>
+      </c>
+      <c r="E2" s="48">
         <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="47" t="s">
         <v>1022</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="49">
+      <c r="B3" s="47"/>
+      <c r="C3" s="48">
         <v>1.3</v>
       </c>
-      <c r="D3" s="49">
-        <v>10</v>
-      </c>
-      <c r="E3" s="49">
+      <c r="D3" s="48">
+        <v>10</v>
+      </c>
+      <c r="E3" s="48">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="47" t="s">
         <v>1099</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="49">
+      <c r="B4" s="47"/>
+      <c r="C4" s="48">
         <v>1.6</v>
       </c>
-      <c r="D4" s="49">
-        <v>10</v>
-      </c>
-      <c r="E4" s="49">
+      <c r="D4" s="48">
+        <v>10</v>
+      </c>
+      <c r="E4" s="48">
         <v>5.5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="47" t="s">
         <v>1100</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49">
+      <c r="B5" s="47"/>
+      <c r="C5" s="48">
         <v>1.8</v>
       </c>
-      <c r="D5" s="49">
-        <v>10</v>
-      </c>
-      <c r="E5" s="49">
+      <c r="D5" s="48">
+        <v>10</v>
+      </c>
+      <c r="E5" s="48">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="47" t="s">
         <v>400</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="49">
+      <c r="B6" s="47"/>
+      <c r="C6" s="48">
         <v>1</v>
       </c>
-      <c r="D6" s="49">
-        <v>10</v>
-      </c>
-      <c r="E6" s="49">
+      <c r="D6" s="48">
+        <v>10</v>
+      </c>
+      <c r="E6" s="48">
         <v>0.5</v>
       </c>
     </row>
@@ -25521,94 +25581,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="46" t="s">
         <v>1106</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="46" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="46" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="46" t="s">
         <v>1083</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="46" t="s">
         <v>1084</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="47" t="s">
         <v>1021</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="49">
+      <c r="B2" s="47"/>
+      <c r="C2" s="48">
         <v>1</v>
       </c>
-      <c r="D2" s="49">
-        <v>10</v>
-      </c>
-      <c r="E2" s="49">
+      <c r="D2" s="48">
+        <v>10</v>
+      </c>
+      <c r="E2" s="48">
         <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="47" t="s">
         <v>1022</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="49">
+      <c r="B3" s="47"/>
+      <c r="C3" s="48">
         <v>1.3</v>
       </c>
-      <c r="D3" s="49">
-        <v>10</v>
-      </c>
-      <c r="E3" s="49">
+      <c r="D3" s="48">
+        <v>10</v>
+      </c>
+      <c r="E3" s="48">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="47" t="s">
         <v>1099</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="49">
+      <c r="B4" s="47"/>
+      <c r="C4" s="48">
         <v>1.6</v>
       </c>
-      <c r="D4" s="49">
-        <v>10</v>
-      </c>
-      <c r="E4" s="49">
+      <c r="D4" s="48">
+        <v>10</v>
+      </c>
+      <c r="E4" s="48">
         <v>5.5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="47" t="s">
         <v>1100</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49">
+      <c r="B5" s="47"/>
+      <c r="C5" s="48">
         <v>1.8</v>
       </c>
-      <c r="D5" s="49">
-        <v>10</v>
-      </c>
-      <c r="E5" s="49">
+      <c r="D5" s="48">
+        <v>10</v>
+      </c>
+      <c r="E5" s="48">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="47" t="s">
         <v>400</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="49">
+      <c r="B6" s="47"/>
+      <c r="C6" s="48">
         <v>1</v>
       </c>
-      <c r="D6" s="49">
-        <v>10</v>
-      </c>
-      <c r="E6" s="49">
+      <c r="D6" s="48">
+        <v>10</v>
+      </c>
+      <c r="E6" s="48">
         <v>0.5</v>
       </c>
     </row>
@@ -25640,94 +25700,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="46" t="s">
         <v>1107</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="46" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="46" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="46" t="s">
         <v>1083</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="46" t="s">
         <v>1084</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="47" t="s">
         <v>1021</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="49">
+      <c r="B2" s="47"/>
+      <c r="C2" s="48">
         <v>1</v>
       </c>
-      <c r="D2" s="49">
-        <v>10</v>
-      </c>
-      <c r="E2" s="49">
+      <c r="D2" s="48">
+        <v>10</v>
+      </c>
+      <c r="E2" s="48">
         <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="47" t="s">
         <v>1022</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="49">
+      <c r="B3" s="47"/>
+      <c r="C3" s="48">
         <v>1.3</v>
       </c>
-      <c r="D3" s="49">
-        <v>10</v>
-      </c>
-      <c r="E3" s="49">
+      <c r="D3" s="48">
+        <v>10</v>
+      </c>
+      <c r="E3" s="48">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="47" t="s">
         <v>1099</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="49">
+      <c r="B4" s="47"/>
+      <c r="C4" s="48">
         <v>1.6</v>
       </c>
-      <c r="D4" s="49">
-        <v>10</v>
-      </c>
-      <c r="E4" s="49">
+      <c r="D4" s="48">
+        <v>10</v>
+      </c>
+      <c r="E4" s="48">
         <v>5.5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="47" t="s">
         <v>1100</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49">
+      <c r="B5" s="47"/>
+      <c r="C5" s="48">
         <v>1.8</v>
       </c>
-      <c r="D5" s="49">
-        <v>10</v>
-      </c>
-      <c r="E5" s="49">
+      <c r="D5" s="48">
+        <v>10</v>
+      </c>
+      <c r="E5" s="48">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="47" t="s">
         <v>400</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="49">
+      <c r="B6" s="47"/>
+      <c r="C6" s="48">
         <v>1</v>
       </c>
-      <c r="D6" s="49">
-        <v>10</v>
-      </c>
-      <c r="E6" s="49">
+      <c r="D6" s="48">
+        <v>10</v>
+      </c>
+      <c r="E6" s="48">
         <v>0.5</v>
       </c>
     </row>
@@ -25759,94 +25819,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="46" t="s">
         <v>1108</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="46" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="46" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="46" t="s">
         <v>1083</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="46" t="s">
         <v>1084</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="47" t="s">
         <v>1021</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="49">
+      <c r="B2" s="47"/>
+      <c r="C2" s="48">
         <v>1</v>
       </c>
-      <c r="D2" s="49">
-        <v>10</v>
-      </c>
-      <c r="E2" s="49">
+      <c r="D2" s="48">
+        <v>10</v>
+      </c>
+      <c r="E2" s="48">
         <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="47" t="s">
         <v>1022</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="49">
+      <c r="B3" s="47"/>
+      <c r="C3" s="48">
         <v>1.3</v>
       </c>
-      <c r="D3" s="49">
-        <v>10</v>
-      </c>
-      <c r="E3" s="49">
+      <c r="D3" s="48">
+        <v>10</v>
+      </c>
+      <c r="E3" s="48">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="47" t="s">
         <v>1099</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="49">
+      <c r="B4" s="47"/>
+      <c r="C4" s="48">
         <v>1.6</v>
       </c>
-      <c r="D4" s="49">
-        <v>10</v>
-      </c>
-      <c r="E4" s="49">
+      <c r="D4" s="48">
+        <v>10</v>
+      </c>
+      <c r="E4" s="48">
         <v>5.5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="47" t="s">
         <v>1100</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49">
+      <c r="B5" s="47"/>
+      <c r="C5" s="48">
         <v>1.8</v>
       </c>
-      <c r="D5" s="49">
-        <v>10</v>
-      </c>
-      <c r="E5" s="49">
+      <c r="D5" s="48">
+        <v>10</v>
+      </c>
+      <c r="E5" s="48">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="47" t="s">
         <v>400</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="49">
+      <c r="B6" s="47"/>
+      <c r="C6" s="48">
         <v>1</v>
       </c>
-      <c r="D6" s="49">
-        <v>10</v>
-      </c>
-      <c r="E6" s="49">
+      <c r="D6" s="48">
+        <v>10</v>
+      </c>
+      <c r="E6" s="48">
         <v>0.5</v>
       </c>
     </row>
@@ -25878,94 +25938,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="46" t="s">
         <v>1109</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="46" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="46" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="46" t="s">
         <v>1083</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="46" t="s">
         <v>1084</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="47" t="s">
         <v>1021</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="49">
+      <c r="B2" s="47"/>
+      <c r="C2" s="48">
         <v>1</v>
       </c>
-      <c r="D2" s="49">
-        <v>10</v>
-      </c>
-      <c r="E2" s="49">
+      <c r="D2" s="48">
+        <v>10</v>
+      </c>
+      <c r="E2" s="48">
         <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="47" t="s">
         <v>1022</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="49">
+      <c r="B3" s="47"/>
+      <c r="C3" s="48">
         <v>1.3</v>
       </c>
-      <c r="D3" s="49">
-        <v>10</v>
-      </c>
-      <c r="E3" s="49">
+      <c r="D3" s="48">
+        <v>10</v>
+      </c>
+      <c r="E3" s="48">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="47" t="s">
         <v>1099</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="49">
+      <c r="B4" s="47"/>
+      <c r="C4" s="48">
         <v>1.6</v>
       </c>
-      <c r="D4" s="49">
-        <v>10</v>
-      </c>
-      <c r="E4" s="49">
+      <c r="D4" s="48">
+        <v>10</v>
+      </c>
+      <c r="E4" s="48">
         <v>5.5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="47" t="s">
         <v>1100</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49">
+      <c r="B5" s="47"/>
+      <c r="C5" s="48">
         <v>1.8</v>
       </c>
-      <c r="D5" s="49">
-        <v>10</v>
-      </c>
-      <c r="E5" s="49">
+      <c r="D5" s="48">
+        <v>10</v>
+      </c>
+      <c r="E5" s="48">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="47" t="s">
         <v>400</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="49">
+      <c r="B6" s="47"/>
+      <c r="C6" s="48">
         <v>1</v>
       </c>
-      <c r="D6" s="49">
-        <v>10</v>
-      </c>
-      <c r="E6" s="49">
+      <c r="D6" s="48">
+        <v>10</v>
+      </c>
+      <c r="E6" s="48">
         <v>0.5</v>
       </c>
     </row>
@@ -25997,79 +26057,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="46" t="s">
         <v>1110</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="46" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="46" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="46" t="s">
         <v>1083</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="46" t="s">
         <v>1084</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="47" t="s">
         <v>594</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="49">
+      <c r="B2" s="47"/>
+      <c r="C2" s="48">
         <v>1</v>
       </c>
-      <c r="D2" s="49">
-        <v>10</v>
-      </c>
-      <c r="E2" s="49">
+      <c r="D2" s="48">
+        <v>10</v>
+      </c>
+      <c r="E2" s="48">
         <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="47" t="s">
         <v>1101</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="49">
+      <c r="B3" s="47"/>
+      <c r="C3" s="48">
         <v>1.3</v>
       </c>
-      <c r="D3" s="49">
-        <v>10</v>
-      </c>
-      <c r="E3" s="49">
+      <c r="D3" s="48">
+        <v>10</v>
+      </c>
+      <c r="E3" s="48">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="47" t="s">
         <v>1031</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="49">
+      <c r="B4" s="47"/>
+      <c r="C4" s="48">
         <v>1.6</v>
       </c>
-      <c r="D4" s="49">
-        <v>10</v>
-      </c>
-      <c r="E4" s="49">
+      <c r="D4" s="48">
+        <v>10</v>
+      </c>
+      <c r="E4" s="48">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="47" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49">
+      <c r="B5" s="47"/>
+      <c r="C5" s="48">
         <v>1</v>
       </c>
-      <c r="D5" s="49">
-        <v>10</v>
-      </c>
-      <c r="E5" s="49">
+      <c r="D5" s="48">
+        <v>10</v>
+      </c>
+      <c r="E5" s="48">
         <v>0.5</v>
       </c>
     </row>
@@ -54685,10 +54745,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -54875,24 +54935,24 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>407</v>
+      <c r="A23" s="49" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B23" s="50" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>406</v>
@@ -54900,7 +54960,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>406</v>
@@ -54908,7 +54968,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>406</v>
@@ -54916,24 +54976,23 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" s="24" t="s">
+      <c r="A29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>406</v>
       </c>
-      <c r="C29" s="15"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="23" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B30" s="24" t="s">
         <v>406</v>
@@ -54942,7 +55001,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="23" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B31" s="24" t="s">
         <v>406</v>
@@ -54951,16 +55010,16 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="23" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C32" s="15"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="23" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B33" s="24" t="s">
         <v>408</v>
@@ -54969,7 +55028,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="23" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B34" s="24" t="s">
         <v>408</v>
@@ -54978,7 +55037,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="23" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B35" s="24" t="s">
         <v>408</v>
@@ -54987,7 +55046,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="23" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B36" s="24" t="s">
         <v>408</v>
@@ -54996,7 +55055,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="23" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B37" s="24" t="s">
         <v>408</v>
@@ -55005,7 +55064,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="23" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B38" s="24" t="s">
         <v>408</v>
@@ -55014,52 +55073,52 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="23" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B39" s="24" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C39" s="15"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B40" s="24" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C40" s="15"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="23" t="s">
-        <v>376</v>
+        <v>56</v>
       </c>
       <c r="B41" s="24" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C41" s="15"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="23" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B42" s="24" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C42" s="15"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="23" t="s">
-        <v>60</v>
+        <v>377</v>
       </c>
       <c r="B43" s="24" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C43" s="15"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="23" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B44" s="24" t="s">
         <v>407</v>
@@ -55068,7 +55127,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B45" s="24" t="s">
         <v>407</v>
@@ -55077,34 +55136,34 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C46" s="15"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="23" t="s">
-        <v>378</v>
+        <v>62</v>
       </c>
       <c r="B47" s="24" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C47" s="15"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="23" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B48" s="24" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C48" s="15"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="23" t="s">
-        <v>66</v>
+        <v>379</v>
       </c>
       <c r="B49" s="24" t="s">
         <v>406</v>
@@ -55112,26 +55171,26 @@
       <c r="C49" s="15"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="36" t="s">
+      <c r="A50" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B50" s="24" t="s">
+        <v>406</v>
+      </c>
+      <c r="C50" s="15"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="36" t="s">
         <v>1020</v>
       </c>
-      <c r="B50" s="37" t="s">
-        <v>406</v>
-      </c>
-      <c r="C50" s="15"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="B51" s="24" t="s">
+      <c r="B51" s="37" t="s">
         <v>406</v>
       </c>
       <c r="C51" s="15"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="23" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B52" s="24" t="s">
         <v>406</v>
@@ -55140,7 +55199,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B53" s="24" t="s">
         <v>406</v>
@@ -55149,7 +55208,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="23" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B54" s="24" t="s">
         <v>406</v>
@@ -55158,16 +55217,16 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="23" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B55" s="24" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C55" s="15"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B56" s="24" t="s">
         <v>408</v>
@@ -55176,7 +55235,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B57" s="24" t="s">
         <v>408</v>
@@ -55185,7 +55244,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="23" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="B58" s="24" t="s">
         <v>408</v>
@@ -55194,43 +55253,43 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="23" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="B59" s="24" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C59" s="15"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B60" s="24" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C60" s="15"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B61" s="24" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C61" s="15"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B62" s="24" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C62" s="15"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B63" s="24" t="s">
         <v>406</v>
@@ -55238,13 +55297,22 @@
       <c r="C63" s="15"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="38" t="s">
+      <c r="A64" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="B64" s="24" t="s">
+        <v>406</v>
+      </c>
+      <c r="C64" s="15"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="38" t="s">
         <v>1064</v>
       </c>
-      <c r="B64" s="45" t="s">
+      <c r="B65" s="45" t="s">
         <v>407</v>
       </c>
-      <c r="C64" s="15"/>
+      <c r="C65" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Actualización table_data: Descripción de condiciones medidas y observadas realizada por Miguel
</commit_message>
<xml_diff>
--- a/data-raw/excel-spreadsheets/table_data.xlsx
+++ b/data-raw/excel-spreadsheets/table_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CNAIM\data-raw\excel-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF323FA6-718E-4106-8E5A-F0A969E6F26F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FCF618-1334-4182-8EEB-1C329EE8C4E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" firstSheet="146" activeTab="159" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -302,7 +302,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6625" uniqueCount="1114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6738" uniqueCount="1214">
   <si>
     <t>Health Index Asset Category</t>
   </si>
@@ -3669,12 +3669,6 @@
     <t>Severamente averiada</t>
   </si>
   <si>
-    <t>Alta (no confirmada)</t>
-  </si>
-  <si>
-    <t>Alta (confirmada)</t>
-  </si>
-  <si>
     <t>Alta</t>
   </si>
   <si>
@@ -3696,9 +3690,6 @@
     <t>Criterios de Condición: Secuencia de Fases</t>
   </si>
   <si>
-    <t>Criterios de Condición: Presencia de Vibraciones</t>
-  </si>
-  <si>
     <t>Criterios de Condición: Pérdidas</t>
   </si>
   <si>
@@ -3712,6 +3703,315 @@
   </si>
   <si>
     <t>Transformador 13.2kV</t>
+  </si>
+  <si>
+    <t>La cubierta de acero del motor no muestra signos de golpes o abolladuras y no hay obstrucciones en sus conductos de ventilación. El motor no muestra signos de daños y el desgaste esperado.</t>
+  </si>
+  <si>
+    <t>El motor presenta golpes con ligeras deformaciones en la estructura del chasis. Estos golpes deben vigilarse para que no comprometan la ventilación y el funcionamiento habitual de la máquina. El motor está contaminado con suciedad de combustible y los elementos de registro del nivel de combustible están contaminados pero registran sus valores correctamente.</t>
+  </si>
+  <si>
+    <t>El motor presenta golpes con ligeras deformaciones en la estructura del chasis. Estos golpes pueden comprometer el funcionamiento debido al contacto con partes internas de la máquina. Excesiva contaminación de combustible y corrosión en el chasis de la máquina obstruyendo los canales de ventilación. Material del chasis corroído, presencia de piezas sueltas sin tornillos de fijación. Elementos de indicación de nivel de fluido, temperatura, presión, etc., no funcionan o indican lecturas erróneas accionando alarmas de forma innecesarias.</t>
+  </si>
+  <si>
+    <t>No hay datos disponibles</t>
+  </si>
+  <si>
+    <t>Rodamientos en buen estado de funcionamiento, sin desgaste considerable</t>
+  </si>
+  <si>
+    <t>Los rodamientos presentan una ligera contaminación previa a una posible corrosión. Mala lubricación de los rodamientos</t>
+  </si>
+  <si>
+    <t>Rodamientos con corrosión, sonidos audibles que indican sustitución inmediata.Rodamientos sin lubricación con suciedad obstruidos.  Rodamientos con grietas que requieren sustitución.</t>
+  </si>
+  <si>
+    <t>Depósito limpio y sin signos de corrosión. Nivel de combustible adecuado. Sin fugas visibles. Líneas y mangueras en buen estado, sin grietas. Sin fugas. Conexiones seguras. Inyectores limpios y en buen estado. Pulverización uniforme del combustible. Sin atascos.</t>
+  </si>
+  <si>
+    <t>Pequeñas zonas de corrosión. Nivel de combustible ligeramente bajo. Pequeñas fugas o goteos. Conexiones ligeramente sueltas. Inyectores parcialmente obstruidos. Pulverización irregular del combustible. Ligeras acumulaciones de suciedad</t>
+  </si>
+  <si>
+    <t>Corrosión significativa. Grandes fugas visibles. Contaminación visible en el combustible (agua, sedimentos). Líneas y mangueras rotas o muy agrietadas. Conexiones sueltas o desconectadas. Inyectores completamente obstruidos o dañados. No hay pulverización de combustible o es muy escasa. Inyectores defectuosos.</t>
+  </si>
+  <si>
+    <t>Aletas del radiador limpias y sin daños. Flujo de aire sin obstrucciones. Nivel de refrigerante adecuado y sin fugas. Funcionamiento suave y sin ruidos extraños en la bomba de agua. Bomba de agua sin fugas. Mangueras en buen estado, sin grietas. El termostato funciona correctamente, abriéndose y cerrándose en función de la temperatura. lectura precisa del sensor de temperatura.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las aletas del radiador están ligeramente dobladas o sucias. Pequeñas obstrucciones del flujo de aire. Nivel de refrigerante ligeramente bajo o pequeñas fugas. Funcionamiento de la bomba de agua con ligeros ruidos o vibraciones. Pequeñas fugas de agua. Flujo de refrigerante ligeramente reducido. Mangueras con pequeñas grietas o signos de desgaste. Termostato abriendo y cerrando ligeramente fuera de posición. </t>
+  </si>
+  <si>
+    <t>Aletas del radiador muy dobladas o dañadas. Obstrucción significativa del flujo de aire. Grandes fugas de refrigerante o nivel de refrigerante extremadamente bajo. Funcionamiento extremadamente ruidoso o no operativo de la bomba de agua. Grandes fugas de agua. Flujo de refrigerante insuficiente o nulo. Mangueras rígidas y quebradizas.</t>
+  </si>
+  <si>
+    <t>Bomba de aceite: Funcionamiento suave sin ruidos extraños. Presión de aceite adecuada. Sin fugas. Líneas y mangueras de aceite: Líneas y mangueras en buen estado, sin grietas. Conexiones seguras y sin fugas. Mangueras flexibles y no rígidas. Cárter de aceite: Nivel de aceite adecuado. Sin signos de contaminación del aceite (agua, sedimentos). Sin fugas.</t>
+  </si>
+  <si>
+    <t>Bomba de aceite: Funcionamiento con ligeros ruidos o vibraciones. Presión de aceite ligeramente baja. Pequeñas fugas de aceite. Líneas y mangueras de aceite: Líneas y mangueras con pequeñas grietas o signos de desgaste. Conexiones ligeramente sueltas o pequeñas fugas. Mangueras ligeramente rígidas. Cárter de aceite: Nivel de aceite ligeramente bajo. Ligera contaminación en el aceite. Pequeñas fugas.</t>
+  </si>
+  <si>
+    <t>Bomba de aceite: Funcionamiento extremadamente ruidoso o no operativo. Presión de aceite insuficiente o nula. Grandes fugas de aceite. Líneas y mangueras de aceite: Líneas y mangueras rotas o con grandes grietas. Conexiones sueltas o grandes fugas. Mangueras rígidas y quebradizas. Cárter de aceite: Nivel de aceite muy bajo o inexistente. Contaminación importante del aceite. Grandes fugas de aceite.</t>
+  </si>
+  <si>
+    <t>Conductos de aire: Los conductos están limpios y en buen estado. Sin grietas ni fugas. Flujo de aire adecuado. Válvula de admisión: Las válvulas están limpias y funcionan correctamente. Apertura y cierre correctos. No hay acumulación de depósitos.</t>
+  </si>
+  <si>
+    <t>Conductos de aire: Conductos con pequeñas grietas o signos de desgaste. Pequeñas fugas. Caudal de aire ligeramente reducido. Válvula de admisión: Válvulas con pequeñas acumulaciones de depósitos. Apertura y cierre ligeramente restringidos. Funcionamiento con ligeros ruidos.</t>
+  </si>
+  <si>
+    <t>Conductos de aire: Conductos gravemente dañados o con grandes grietas. Grandes fugas. Flujo de aire insuficiente. Válvula de admisión: Válvulas muy sucias o dañadas. Apertura y cierre inadecuados. Funcionamiento ruidoso o no operativo.</t>
+  </si>
+  <si>
+    <t>Funcionamiento suave y sin ruidos extraños. Presión de aire adecuada. Sin fugas de aceite ni de aire.</t>
+  </si>
+  <si>
+    <t>Funcionamiento con ligeros ruidos o vibraciones. Presión de aire ligeramente baja. Pequeñas fugas de aceite o aire.</t>
+  </si>
+  <si>
+    <t>Funcionamiento extremadamente ruidoso o no operativo. Presión de aire insuficiente. Grandes fugas de aceite o aire.</t>
+  </si>
+  <si>
+    <t>Superficie lisa sin marcas. Sin signos de desgaste significativo. Lubricación adecuada. Sin acumulación de carbonilla. Juntas de culata en buen estado, sin fugas. Culata bien ajustada y sin deformaciones. No hay signos de compresión excesiva en la culata.</t>
+  </si>
+  <si>
+    <t>Pequeñoas marcas o ligero desgaste. Superficie ligeramente rugosa. Lubricación ligeramente insuficiente. Ligera acumulación de carbonilla. Pequeñas fugas en las juntas. Ajuste ligeramente flojo. Ligeros signos de compresión excesiva.</t>
+  </si>
+  <si>
+    <t>Raspaduras profundas o desgaste grave. Superficie muy rugosa. Falta de lubricación o aceite contaminado. Acumulación importante de depósitos de carbono. Fugas graves o juntas dañadas. Ajuste flojo o inexistente. Compresión excesiva o falta de compresión en la culata.</t>
+  </si>
+  <si>
+    <t>Filtro limpio y en buen estado. Sin obstrucciones. Flujo adecuado a través del filtro.</t>
+  </si>
+  <si>
+    <t>Pequeñas obstrucciones. Caudal ligeramente reducido.</t>
+  </si>
+  <si>
+    <t>Filtro muy sucio o dañado. Obstrucción importante. Caudal insuficiente o nulo en las salidas del filtro.</t>
+  </si>
+  <si>
+    <t>Integridad: Carcasa intacta, sin abolladuras ni daños. Sin corrosión ni óxido visibles. Sellado y protección contra el polvo y el agua: Juntas en buen estado, sin grietas ni desgaste. Sin acumulación de polvo o suciedad en el interior. Carcasa impermeable y sin signos de humedad. Sistema de ventilación y refrigeración: Ventiladores y rejillas de ventilación limpios y sin obstrucciones. El sistema de refrigeración funciona correctamente. Flujo de aire adecuado y ausencia de ruidos anormales. Instalación eléctrica y conexiones: Cableado en buen estado, sin desgaste ni daños. Conexiones eléctricas seguras y sin corrosión. Los componentes eléctricos están bien organizados y protegidos. Datos de la placa de características: Señalización clara y legible.</t>
+  </si>
+  <si>
+    <t>Integridad: Pequeñas abolladuras o golpes. Ligeros signos de corrosión u óxido. Sellado y protección contra el polvo y el agua: Juntas con pequeñas grietas o ligero desgaste. Ligera acumulación de polvo o suciedad. Ligeros signos de humedad. Sistema de ventilación y refrigeración: Ventiladores y rejillas con ligera acumulación de polvo o suciedad. Sistema de refrigeración con rendimiento reducido. Flujo de aire ligeramente restringido, pequeños ruidos o vibraciones. Instalación eléctrica y conexiones: Cableado con ligeros signos de desgaste o daños. Conexiones eléctricas con pequeños puntos de corrosión. Componentes eléctricos ligeramente desorganizados. Datos de la placa de características: Señalización y etiquetas con ligeros signos de desgaste.</t>
+  </si>
+  <si>
+    <t>Integridad: Grandes abolladuras o daños significativos. Corrosión grave u óxido extenso. Sellado y protección contra el polvo y el agua: Juntas rotas o muy desgastadas. Acumulación significativa de polvo o suciedad. Infiltración visible de agua, humedad excesiva o corrosión interna. Sistema de ventilación y refrigeración: Ventiladores y rejillas muy obstruidos. El sistema de refrigeración no funciona. Flujo de aire insuficiente, ruidos fuertes o vibraciones significativas. Instalación y conexiones eléctricas: Cableado muy desgastado o dañado. Conexiones eléctricas con elevada corrosión . Componentes eléctricos desorganizados o expuestos. Datos de la placa de características: Señalización ilegible o ausente.</t>
+  </si>
+  <si>
+    <t>Estado óptimo, sin signos de desgaste, superficies limpias y libres de contaminantes como la corrosión. Aislamiento sin grietas ni decoloración, lo que indica que el aislamiento cumple su función sin problemas.</t>
+  </si>
+  <si>
+    <t>El aislamiento muestra ligeros signos de desgaste o envejecimiento, con pequeñas manchas o suciedad en la superficie, y pequeñas grietas, se trata de un caso de deterioro menor. Desgaste que puede gestionarse con un mantenimiento preventivo.</t>
+  </si>
+  <si>
+    <t>Sistema de aislamiento envejecido, fecha de fabricación posterior a la vida útil del equipo. Humedad, corrosión y aislamiento descolorido.</t>
+  </si>
+  <si>
+    <t>Los cables no muestran cortes ni desgaste, con cubiertas aislantes intactas y bien sujetas sin signos de sobrecalentamiento.</t>
+  </si>
+  <si>
+    <t>Los cables y las cajas de conexiones pueden mostrar ligeros signos de desgaste o envejecimiento, con presencia de suciedad y signos de corrosión. También pueden presentar pequeñas grietas y estar ligeramente desgastados con una ligera decoloración debida al sobrecalentamiento. Esto indica la necesidad de una revisión y posible sustitución a corto plazo.</t>
+  </si>
+  <si>
+    <t>Cables muy desgastados o dañados, con aislamientos desintegrados y cajas de conexiones inutilizadas por la suciedad o la corrosión.Estamos ante un deterioro total que requiere atención urgente para evitar averías graves.</t>
+  </si>
+  <si>
+    <t>Superficie del rotor libre de contaminación. Ejes y cojinetes con alineación correcta. Sin vibraciones debidas a una condición fuera de la condición de diseño. Bobinado sin desgaste del aislamiento ni decoloración por sobrecalentamiento. Sistema de refrigeración del rotor funcionando correctamente.</t>
+  </si>
+  <si>
+    <t>Superficie del rotor con ligeros signos de contaminación ambiental. Ejes y rodamientos con signos  de suciedad, ligeras vibraciones en condiciones habituales de funcionamiento. Devanados con ligeros signos de desgaste del aislamiento, presencia de sobrecalentamiento y olor a quemado de parte de los devanados. Aislamiento ligeramente descolorido. Sistema de ventilación con ligeros defectos.</t>
+  </si>
+  <si>
+    <t>Superficie del rotor con alto nivel de contaminación ambiental, presencia de corrosión, humedad, polvo, entre otros.  Ejes y rodamientos desalineados, niveles de vibración que comprometen la continuidad del funcionamiento de la máquina.  Presencia de ruido audible excesivo del rotor durante su funcionamiento. Bobinado con signos de desgaste del aislamiento, presencia de quemaduras en el bobinado, con funcionamiento del aislamiento poco fiable. Olor excesivo a bobinado quemado. Sistema de ventilación ineficaz.</t>
+  </si>
+  <si>
+    <t>Laminados del núcleo del estator bien apilados, sin signos de deformación, sobrecalentamiento o corrosión. Superficie del estator conforme a las condiciones de diseño de la máquina. Bobinado del estator con aislamiento en buen estado. Ranurado del estator en buen estado. Sistema de ventilación funcionando correctamente.</t>
+  </si>
+  <si>
+    <t>Laminados del núcleo del estator con ligeras deformaciones y signos de contaminación y corrosión. Superficie del estator con ligeras deformaciones y presencia de suciedad. Devanado del estator decolorado. Ranurado del estator con signos de deformaciones.</t>
+  </si>
+  <si>
+    <t>Laminados del núcleo del estator con deformaciones considerables y presencia de contaminación y corrosión. Superficie del estator con deformaciones irreversibles. Devanado del estator con aislamiento defectuoso y presencia de olor de bobinado quemado. Ranurado deficiente.</t>
+  </si>
+  <si>
+    <t>El motor funciona con una eficiencia térmica ≥ 42%, un consumo de combustible dentro del rango nominal (≤ 195 g/kWh) y un funcionamiento estable sin degradación significativa.</t>
+  </si>
+  <si>
+    <t>La eficiencia térmica disminuye hasta el 36-42%, con un mayor consumo de combustible (195-215 g/kWh). Se mantiene la estabilidad operativa, pero es evidente un desgaste clave del sistema.</t>
+  </si>
+  <si>
+    <t>Rendimiento térmico &lt; 36%, consumo excesivo de combustible (&gt; 215 g/kWh), con fluctuaciones de potencia y fallos recurrentes. Pérdida de estabilidad operativa con riesgo de desconexión del sistema.</t>
+  </si>
+  <si>
+    <t>El régimen del motor se mantiene en 514 RPM ±0,5% (o velocidad nominal ±0,5%) en todas las condiciones de carga, sin fluctuaciones significativas.</t>
+  </si>
+  <si>
+    <t>Se producen oscilaciones de alrededor del ±1% de la velocidad nominal, con tiempos de estabilización prolongados durante los cambios de carga.</t>
+  </si>
+  <si>
+    <t>Las variaciones superan el ±3%, lo que afecta a la estabilidad del sistema. Se detectan eventos de sobrevelocidad o caídas repentinas de RPM.</t>
+  </si>
+  <si>
+    <t>El consumo específico de combustible se mantiene dentro de la gama garantizada de 183,4 g/kWh ±5% (173,23 - 192,57 g/kWh). La combustión es eficiente y la relación aire-combustible es óptima.</t>
+  </si>
+  <si>
+    <t>El consumo específico de combustible oscila entre 192,57 - 201,7 g/kWh, con una reducción moderada del rendimiento térmico. Entre las posibles causas se incluyen depósitos en los inyectores, ajustes inadecuados de la mezcla aire-combustible o una ligera pérdida de eficiencia del generador de corriente alterna.</t>
+  </si>
+  <si>
+    <t>El consumo supera los 201,7 g/kWh, lo que indica graves ineficiencias en la combustión o en el sistema de inyección. Las causas potenciales incluyen inyectores obstruidos, combustión incompleta o degradación de componentes clave del sistema de combustible.</t>
+  </si>
+  <si>
+    <t>El sistema de frenado del motor responde dentro de los tiempos de diseño sin retrasos ni fallos. Los componentes mecánicos y neumáticos están en condiciones óptimas.</t>
+  </si>
+  <si>
+    <t>Se observan ligeros retrasos en la activación del freno, aunque dentro de márgenes aceptables. Los componentes de fricción muestran desgaste o hay pérdida parcial de presión en el sistema neumático.</t>
+  </si>
+  <si>
+    <t>El freno no responde en los plazos previstos o presenta fallos intermitentes. Se observan fugas en el sistema neumático, fallos en las válvulas o desgaste grave de los componentes de fricción.</t>
+  </si>
+  <si>
+    <t>≥ 1000 MΩ. Valor típico de máquina nueva o recién secada. Índice de polarización &gt; 2.5. Bajo riesgo dieléctrico.</t>
+  </si>
+  <si>
+    <t>100 – 999 MΩ. Cercano al límite mínimo. Puede indicar humedad, contaminación o envejecimiento parcial. Se recomienda secado o limpieza preventiva.</t>
+  </si>
+  <si>
+    <t>10 – 99 MΩ. Bajo el umbral recomendado. Riesgo elevado de descarga o tracking. Requiere intervención técnica antes de operación sostenida.</t>
+  </si>
+  <si>
+    <t>&lt; 10 MΩ. Condición crítica, alto riesgo de cortocircuito. No se recomienda puesta en marcha hasta recuperación dieléctrica completa.</t>
+  </si>
+  <si>
+    <t>501 – 1000 pC. Patrón bipolar ancho o difuso en fase. Indicios de cavidades internas, degradación de impregnación o inicio de tracking.</t>
+  </si>
+  <si>
+    <t>1001 – 3000 pC. Picos irregulares o alta densidad de PD. Indica tracking severo, delaminación o movimiento mecánico de barras. Riesgo creciente.</t>
+  </si>
+  <si>
+    <t>&gt; 3000 pC. Saturación del patrón o múltiples fuentes de PD. Riesgo inminente de falla dieléctrica. Se recomienda parada y diagnóstico integral.</t>
+  </si>
+  <si>
+    <t>La secuencia de fases es verificada como correcta (R-S-T o equivalente), confirmada por instrumento de secuencia o sistema de sincronización. No se detectan errores de rotación en operación.</t>
+  </si>
+  <si>
+    <t>Se detecta inversión de secuencia de forma esporádica durante pruebas de arranque, sincronización o transferencia de carga. El sistema corrige automáticamente o emite alarmas</t>
+  </si>
+  <si>
+    <t>El sistema detecta secuencia incorrecta (T-S-R), documentada por equipo de medición o rechazo de sincronismo. La inversión produce rotación inversa en motores o bloqueo del sistema de protección</t>
+  </si>
+  <si>
+    <t>La inversión de fases persiste sin intervención, y no existen mecanismos de protección activos. El generador puede dañar equipos acoplados o provocar fallo en sincronismo con red o grupo</t>
+  </si>
+  <si>
+    <t>No se dispone de medición reciente ni registro del control automático de fase. No se puede confirmar el estado actual del sistema.</t>
+  </si>
+  <si>
+    <t>2.9 – 4.5 mm/s. Vibraciones medias. Posible desalineación, asentamiento, o desequilibrio progresivo. Requiere monitoreo frecuente</t>
+  </si>
+  <si>
+    <t>4.6 – 7.1 mm/s. Vibración elevada. Potencial daño a rodamientos o estructura. Requiere análisis dinámico y mantenimiento preventivo.</t>
+  </si>
+  <si>
+    <t>&gt; 7.1 mm/s. Vibraciones severas con riesgo de falla catastrófica. Intervención urgente recomendada. Probables daños en acoplamientos, ejes o rodamientos.</t>
+  </si>
+  <si>
+    <t>No se dispone de medición reciente ni de análisis espectral. Se requiere verificación para clasificar</t>
+  </si>
+  <si>
+    <t>2.59% – 3.0%. Leve aumento de pérdidas por rozamientos, desbalance térmico, escobillas con desgaste o suciedad en sistema de ventilación.</t>
+  </si>
+  <si>
+    <t>3.01% – 3.5%. Disminución sostenida de eficiencia. Probable degradación en devanados o aumento de pérdidas en núcleo o ventilación.</t>
+  </si>
+  <si>
+    <t>&gt; 3.5%. Eficiencia &lt; 96.5%. Riesgo de sobretemperatura, deterioro del aislamiento o fatiga térmica. Evaluación urgente requerida.</t>
+  </si>
+  <si>
+    <t>No se dispone de prueba de rendimiento ni curva de eficiencia medida</t>
+  </si>
+  <si>
+    <t>No se dispone de medición térmica confiable ni de sensores funcionales</t>
+  </si>
+  <si>
+    <t>Excelente</t>
+  </si>
+  <si>
+    <t>Buena</t>
+  </si>
+  <si>
+    <t>Aceptable</t>
+  </si>
+  <si>
+    <t>Deficiente</t>
+  </si>
+  <si>
+    <t>Crítica</t>
+  </si>
+  <si>
+    <t>1000 – 4999 MΩ. Dentro de valores aceptables recomendados por IEEE para máquinas &gt; 1000 V. Sin síntomas de degradación dieléctrica.</t>
+  </si>
+  <si>
+    <t>101 – 500 pC. Patrón estable, unipolar o bipolar estrecho. Indica contaminación leve o envejecimiento superficial sin riesgo inmediato.</t>
+  </si>
+  <si>
+    <t>Muy bajas</t>
+  </si>
+  <si>
+    <t>Bajas</t>
+  </si>
+  <si>
+    <t>Medias</t>
+  </si>
+  <si>
+    <t>Altas</t>
+  </si>
+  <si>
+    <t>Muy altas</t>
+  </si>
+  <si>
+    <t>Correcta</t>
+  </si>
+  <si>
+    <t>Inestable</t>
+  </si>
+  <si>
+    <t>Invertida</t>
+  </si>
+  <si>
+    <t>≤ 100 pC. Patrón unipolar o apenas visible. Descargas superficiales ausentes o mínimas. Sistema de aislamiento en condiciones óptimas.</t>
+  </si>
+  <si>
+    <t>≤ 1.8 mm/s. Vibraciones normales de operación. Medición estable sin picos. Sin indicios de desbalance, desalineación ni aflojamiento.</t>
+  </si>
+  <si>
+    <t>1.9 – 2.8 mm/s. Ligero incremento por desbalance menor, pero dentro de parámetros recomendados por ISO 10816 para generadores montados en bancada rígida.</t>
+  </si>
+  <si>
+    <t>Criterios de Condición: Vibraciones</t>
+  </si>
+  <si>
+    <t>≤ 2.50%. Eficiencia real ≥ 97.5%. Sistema electromagnético y mecánico en estado óptimo. Sin evidencia de pérdidas térmicas o anómalas.</t>
+  </si>
+  <si>
+    <t>2.51% – 2.58%. Dentro de las especificaciones nominales del fabricante. Condición aceptable para operación continua.</t>
+  </si>
+  <si>
+    <t>≤ 110 °C (o &lt; 70 °C de elevación térmica). Temperatura muy por debajo del límite de clase F. Sistema térmico optimizado, sin sobrecarga ni obstrucción de ventilación.</t>
+  </si>
+  <si>
+    <t>141 – 155 °C. Límite superior de clase F alcanzado. Riesgo de envejecimiento acelerado del aislamiento. Requiere acción correctiva preventiva.</t>
+  </si>
+  <si>
+    <t>&gt; 155 °C. Sobrepaso de la clase térmica. Riesgo elevado de falla dieléctrica, deslaminación o colapso del sistema de impregnación. Parada urgente recomendada.</t>
+  </si>
+  <si>
+    <t>111 – 125 °C. Elevación térmica moderada (hasta 80 °C). Dentro del límite de diseño. Devanado operando eficientemente con carga nominal.</t>
+  </si>
+  <si>
+    <t>126 – 140 °C. Cercano al límite térmico (clase F = 155 °C). Puede haber suciedad, reducción de ventilación o carga intermitente elevada.</t>
+  </si>
+  <si>
+    <t>Muy baja</t>
   </si>
 </sst>
 </file>
@@ -3722,7 +4022,7 @@
     <numFmt numFmtId="164" formatCode="0.000000000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3823,6 +4123,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -3935,7 +4240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4016,11 +4321,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4408,7 +4715,7 @@
   </sheetPr>
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -4588,11 +4895,11 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="49" t="s">
+      <c r="A22" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="49" t="s">
-        <v>1113</v>
+      <c r="B22" s="48" t="s">
+        <v>1110</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -8347,14 +8654,14 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="48" t="s">
         <v>177</v>
       </c>
-      <c r="C11" s="49" t="s">
-        <v>1111</v>
+      <c r="C11" s="48" t="s">
+        <v>1108</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -11335,9 +11642,7 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -11374,7 +11679,9 @@
       <c r="A2" s="38" t="s">
         <v>1085</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="38" t="s">
+        <v>1111</v>
+      </c>
       <c r="C2" s="38">
         <v>1</v>
       </c>
@@ -11389,7 +11696,9 @@
       <c r="A3" s="38" t="s">
         <v>1034</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="38" t="s">
+        <v>1112</v>
+      </c>
       <c r="C3" s="38">
         <v>1.4</v>
       </c>
@@ -11404,7 +11713,9 @@
       <c r="A4" s="38" t="s">
         <v>1035</v>
       </c>
-      <c r="B4" s="38"/>
+      <c r="B4" s="38" t="s">
+        <v>1113</v>
+      </c>
       <c r="C4" s="38">
         <v>1.8</v>
       </c>
@@ -11419,7 +11730,9 @@
       <c r="A5" s="38" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="38" t="s">
+        <v>1114</v>
+      </c>
       <c r="C5" s="38">
         <v>1</v>
       </c>
@@ -11443,9 +11756,7 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -11482,7 +11793,9 @@
       <c r="A2" s="38" t="s">
         <v>1085</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="38" t="s">
+        <v>1115</v>
+      </c>
       <c r="C2" s="38">
         <v>1</v>
       </c>
@@ -11497,7 +11810,9 @@
       <c r="A3" s="38" t="s">
         <v>1034</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="38" t="s">
+        <v>1116</v>
+      </c>
       <c r="C3" s="38">
         <v>1.2</v>
       </c>
@@ -11512,7 +11827,9 @@
       <c r="A4" s="38" t="s">
         <v>1035</v>
       </c>
-      <c r="B4" s="38"/>
+      <c r="B4" s="38" t="s">
+        <v>1117</v>
+      </c>
       <c r="C4" s="38">
         <v>1.8</v>
       </c>
@@ -11527,7 +11844,9 @@
       <c r="A5" s="38" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="38" t="s">
+        <v>1114</v>
+      </c>
       <c r="C5" s="38">
         <v>1</v>
       </c>
@@ -11551,9 +11870,7 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E5"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -11590,7 +11907,9 @@
       <c r="A2" s="38" t="s">
         <v>1085</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="38" t="s">
+        <v>1118</v>
+      </c>
       <c r="C2" s="38">
         <v>1</v>
       </c>
@@ -11605,7 +11924,9 @@
       <c r="A3" s="38" t="s">
         <v>1034</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="38" t="s">
+        <v>1119</v>
+      </c>
       <c r="C3" s="38">
         <v>1.2</v>
       </c>
@@ -11620,7 +11941,9 @@
       <c r="A4" s="38" t="s">
         <v>1035</v>
       </c>
-      <c r="B4" s="38"/>
+      <c r="B4" s="38" t="s">
+        <v>1120</v>
+      </c>
       <c r="C4" s="38">
         <v>1.4</v>
       </c>
@@ -11635,7 +11958,9 @@
       <c r="A5" s="38" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="38" t="s">
+        <v>1114</v>
+      </c>
       <c r="C5" s="38">
         <v>1</v>
       </c>
@@ -11782,14 +12107,14 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="48" t="s">
         <v>177</v>
       </c>
-      <c r="C11" s="49" t="s">
-        <v>1112</v>
+      <c r="C11" s="48" t="s">
+        <v>1109</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -12091,9 +12416,7 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E5"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -12130,7 +12453,9 @@
       <c r="A2" s="38" t="s">
         <v>1085</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="38" t="s">
+        <v>1121</v>
+      </c>
       <c r="C2" s="38">
         <v>1</v>
       </c>
@@ -12145,7 +12470,9 @@
       <c r="A3" s="38" t="s">
         <v>1034</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="38" t="s">
+        <v>1122</v>
+      </c>
       <c r="C3" s="38">
         <v>1.2</v>
       </c>
@@ -12160,7 +12487,9 @@
       <c r="A4" s="38" t="s">
         <v>1035</v>
       </c>
-      <c r="B4" s="38"/>
+      <c r="B4" s="38" t="s">
+        <v>1123</v>
+      </c>
       <c r="C4" s="38">
         <v>1.4</v>
       </c>
@@ -12175,7 +12504,9 @@
       <c r="A5" s="38" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="38" t="s">
+        <v>1114</v>
+      </c>
       <c r="C5" s="38">
         <v>1</v>
       </c>
@@ -12199,9 +12530,7 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E5"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -12238,7 +12567,9 @@
       <c r="A2" s="38" t="s">
         <v>1085</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="38" t="s">
+        <v>1124</v>
+      </c>
       <c r="C2" s="38">
         <v>1</v>
       </c>
@@ -12253,7 +12584,9 @@
       <c r="A3" s="38" t="s">
         <v>1034</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="38" t="s">
+        <v>1125</v>
+      </c>
       <c r="C3" s="38">
         <v>1.2</v>
       </c>
@@ -12268,7 +12601,9 @@
       <c r="A4" s="38" t="s">
         <v>1035</v>
       </c>
-      <c r="B4" s="38"/>
+      <c r="B4" s="38" t="s">
+        <v>1126</v>
+      </c>
       <c r="C4" s="38">
         <v>1.4</v>
       </c>
@@ -12283,7 +12618,9 @@
       <c r="A5" s="38" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="38" t="s">
+        <v>1114</v>
+      </c>
       <c r="C5" s="38">
         <v>1</v>
       </c>
@@ -12307,9 +12644,7 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E5"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -12346,7 +12681,9 @@
       <c r="A2" s="38" t="s">
         <v>1085</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="38" t="s">
+        <v>1127</v>
+      </c>
       <c r="C2" s="38">
         <v>1</v>
       </c>
@@ -12361,7 +12698,9 @@
       <c r="A3" s="38" t="s">
         <v>1034</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="38" t="s">
+        <v>1128</v>
+      </c>
       <c r="C3" s="38">
         <v>1.2</v>
       </c>
@@ -12376,7 +12715,9 @@
       <c r="A4" s="38" t="s">
         <v>1035</v>
       </c>
-      <c r="B4" s="38"/>
+      <c r="B4" s="38" t="s">
+        <v>1129</v>
+      </c>
       <c r="C4" s="38">
         <v>1.4</v>
       </c>
@@ -12391,7 +12732,9 @@
       <c r="A5" s="38" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="38" t="s">
+        <v>1114</v>
+      </c>
       <c r="C5" s="38">
         <v>1</v>
       </c>
@@ -12415,9 +12758,7 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E5"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -12454,7 +12795,9 @@
       <c r="A2" s="38" t="s">
         <v>1085</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="38" t="s">
+        <v>1130</v>
+      </c>
       <c r="C2" s="38">
         <v>1</v>
       </c>
@@ -12469,7 +12812,9 @@
       <c r="A3" s="38" t="s">
         <v>1034</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="38" t="s">
+        <v>1131</v>
+      </c>
       <c r="C3" s="38">
         <v>1.2</v>
       </c>
@@ -12484,7 +12829,9 @@
       <c r="A4" s="38" t="s">
         <v>1035</v>
       </c>
-      <c r="B4" s="38"/>
+      <c r="B4" s="38" t="s">
+        <v>1132</v>
+      </c>
       <c r="C4" s="38">
         <v>1.4</v>
       </c>
@@ -12499,7 +12846,9 @@
       <c r="A5" s="38" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="38" t="s">
+        <v>1114</v>
+      </c>
       <c r="C5" s="38">
         <v>1</v>
       </c>
@@ -12523,9 +12872,7 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E5"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -12562,7 +12909,9 @@
       <c r="A2" s="38" t="s">
         <v>1085</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="38" t="s">
+        <v>1133</v>
+      </c>
       <c r="C2" s="38">
         <v>1</v>
       </c>
@@ -12577,7 +12926,9 @@
       <c r="A3" s="38" t="s">
         <v>1034</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="38" t="s">
+        <v>1134</v>
+      </c>
       <c r="C3" s="38">
         <v>1.2</v>
       </c>
@@ -12592,7 +12943,9 @@
       <c r="A4" s="38" t="s">
         <v>1035</v>
       </c>
-      <c r="B4" s="38"/>
+      <c r="B4" s="38" t="s">
+        <v>1135</v>
+      </c>
       <c r="C4" s="38">
         <v>1.4</v>
       </c>
@@ -12607,7 +12960,9 @@
       <c r="A5" s="38" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="38" t="s">
+        <v>1114</v>
+      </c>
       <c r="C5" s="38">
         <v>1</v>
       </c>
@@ -12631,9 +12986,7 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E5"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -12670,7 +13023,9 @@
       <c r="A2" s="38" t="s">
         <v>1085</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="38" t="s">
+        <v>1136</v>
+      </c>
       <c r="C2" s="38">
         <v>1</v>
       </c>
@@ -12685,7 +13040,9 @@
       <c r="A3" s="38" t="s">
         <v>1034</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="38" t="s">
+        <v>1137</v>
+      </c>
       <c r="C3" s="38">
         <v>1.2</v>
       </c>
@@ -12700,7 +13057,9 @@
       <c r="A4" s="38" t="s">
         <v>1035</v>
       </c>
-      <c r="B4" s="38"/>
+      <c r="B4" s="38" t="s">
+        <v>1138</v>
+      </c>
       <c r="C4" s="38">
         <v>1.4</v>
       </c>
@@ -12715,7 +13074,9 @@
       <c r="A5" s="38" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="38" t="s">
+        <v>1114</v>
+      </c>
       <c r="C5" s="38">
         <v>1</v>
       </c>
@@ -12739,9 +13100,7 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E5"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -12778,7 +13137,9 @@
       <c r="A2" s="38" t="s">
         <v>1085</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="38" t="s">
+        <v>1139</v>
+      </c>
       <c r="C2" s="38">
         <v>1</v>
       </c>
@@ -12793,7 +13154,9 @@
       <c r="A3" s="38" t="s">
         <v>1034</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="38" t="s">
+        <v>1140</v>
+      </c>
       <c r="C3" s="38">
         <v>1.2</v>
       </c>
@@ -12808,7 +13171,9 @@
       <c r="A4" s="38" t="s">
         <v>1035</v>
       </c>
-      <c r="B4" s="38"/>
+      <c r="B4" s="38" t="s">
+        <v>1141</v>
+      </c>
       <c r="C4" s="38">
         <v>1.4</v>
       </c>
@@ -12823,7 +13188,9 @@
       <c r="A5" s="38" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="38" t="s">
+        <v>1114</v>
+      </c>
       <c r="C5" s="38">
         <v>1</v>
       </c>
@@ -12847,9 +13214,7 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E5"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -12886,7 +13251,9 @@
       <c r="A2" s="38" t="s">
         <v>1085</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="38" t="s">
+        <v>1142</v>
+      </c>
       <c r="C2" s="38">
         <v>1</v>
       </c>
@@ -12901,7 +13268,9 @@
       <c r="A3" s="38" t="s">
         <v>1034</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="38" t="s">
+        <v>1143</v>
+      </c>
       <c r="C3" s="38">
         <v>1.2</v>
       </c>
@@ -12916,7 +13285,9 @@
       <c r="A4" s="38" t="s">
         <v>1035</v>
       </c>
-      <c r="B4" s="38"/>
+      <c r="B4" s="38" t="s">
+        <v>1144</v>
+      </c>
       <c r="C4" s="38">
         <v>1.4</v>
       </c>
@@ -12931,7 +13302,9 @@
       <c r="A5" s="38" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="38" t="s">
+        <v>1114</v>
+      </c>
       <c r="C5" s="38">
         <v>1</v>
       </c>
@@ -12955,9 +13328,7 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E5"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -12994,7 +13365,9 @@
       <c r="A2" s="38" t="s">
         <v>1085</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="38" t="s">
+        <v>1145</v>
+      </c>
       <c r="C2" s="38">
         <v>1</v>
       </c>
@@ -13009,7 +13382,9 @@
       <c r="A3" s="38" t="s">
         <v>1034</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="38" t="s">
+        <v>1146</v>
+      </c>
       <c r="C3" s="38">
         <v>1.2</v>
       </c>
@@ -13024,7 +13399,9 @@
       <c r="A4" s="38" t="s">
         <v>1035</v>
       </c>
-      <c r="B4" s="38"/>
+      <c r="B4" s="38" t="s">
+        <v>1147</v>
+      </c>
       <c r="C4" s="38">
         <v>1.4</v>
       </c>
@@ -13039,7 +13416,9 @@
       <c r="A5" s="38" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="38" t="s">
+        <v>1114</v>
+      </c>
       <c r="C5" s="38">
         <v>1</v>
       </c>
@@ -13063,9 +13442,7 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E5"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -13102,7 +13479,9 @@
       <c r="A2" s="38" t="s">
         <v>1085</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="38" t="s">
+        <v>1148</v>
+      </c>
       <c r="C2" s="38">
         <v>1</v>
       </c>
@@ -13117,7 +13496,9 @@
       <c r="A3" s="38" t="s">
         <v>1034</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="38" t="s">
+        <v>1149</v>
+      </c>
       <c r="C3" s="38">
         <v>1.2</v>
       </c>
@@ -13132,7 +13513,9 @@
       <c r="A4" s="38" t="s">
         <v>1035</v>
       </c>
-      <c r="B4" s="38"/>
+      <c r="B4" s="38" t="s">
+        <v>1150</v>
+      </c>
       <c r="C4" s="38">
         <v>1.4</v>
       </c>
@@ -13147,7 +13530,9 @@
       <c r="A5" s="38" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="38" t="s">
+        <v>1114</v>
+      </c>
       <c r="C5" s="38">
         <v>1</v>
       </c>
@@ -13809,9 +14194,7 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -13848,7 +14231,9 @@
       <c r="A2" s="38" t="s">
         <v>1085</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="38" t="s">
+        <v>1151</v>
+      </c>
       <c r="C2" s="38">
         <v>1</v>
       </c>
@@ -13863,7 +14248,9 @@
       <c r="A3" s="38" t="s">
         <v>1034</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="38" t="s">
+        <v>1152</v>
+      </c>
       <c r="C3" s="38">
         <v>1.2</v>
       </c>
@@ -13878,7 +14265,9 @@
       <c r="A4" s="38" t="s">
         <v>1035</v>
       </c>
-      <c r="B4" s="38"/>
+      <c r="B4" s="38" t="s">
+        <v>1153</v>
+      </c>
       <c r="C4" s="38">
         <v>1.4</v>
       </c>
@@ -13893,7 +14282,9 @@
       <c r="A5" s="38" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="38" t="s">
+        <v>1114</v>
+      </c>
       <c r="C5" s="38">
         <v>1</v>
       </c>
@@ -16106,22 +16497,22 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="49" t="s">
-        <v>1113</v>
-      </c>
-      <c r="B59" s="49">
+      <c r="A59" s="48" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B59" s="48">
         <v>9297</v>
       </c>
-      <c r="C59" s="49">
+      <c r="C59" s="48">
         <v>4823</v>
       </c>
-      <c r="D59" s="49">
+      <c r="D59" s="48">
         <v>3809</v>
       </c>
-      <c r="E59" s="49">
+      <c r="E59" s="48">
         <v>4343</v>
       </c>
-      <c r="F59" s="49">
+      <c r="F59" s="48">
         <v>22271</v>
       </c>
     </row>
@@ -22374,11 +22765,11 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="49" t="s">
+      <c r="A35" s="48" t="s">
         <v>1076</v>
       </c>
-      <c r="B35" s="49"/>
-      <c r="C35" s="49">
+      <c r="B35" s="48"/>
+      <c r="C35" s="48">
         <v>60</v>
       </c>
     </row>
@@ -25069,7 +25460,9 @@
       <c r="A2" s="47" t="s">
         <v>1088</v>
       </c>
-      <c r="B2" s="47"/>
+      <c r="B2" s="47" t="s">
+        <v>1154</v>
+      </c>
       <c r="C2" s="47">
         <v>1</v>
       </c>
@@ -25084,7 +25477,9 @@
       <c r="A3" s="47" t="s">
         <v>1089</v>
       </c>
-      <c r="B3" s="47"/>
+      <c r="B3" s="47" t="s">
+        <v>1155</v>
+      </c>
       <c r="C3" s="47">
         <v>1.3</v>
       </c>
@@ -25099,7 +25494,9 @@
       <c r="A4" s="47" t="s">
         <v>1090</v>
       </c>
-      <c r="B4" s="47"/>
+      <c r="B4" s="47" t="s">
+        <v>1156</v>
+      </c>
       <c r="C4" s="47">
         <v>1.6</v>
       </c>
@@ -25114,7 +25511,9 @@
       <c r="A5" s="47" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="47"/>
+      <c r="B5" s="47" t="s">
+        <v>1114</v>
+      </c>
       <c r="C5" s="47">
         <v>1</v>
       </c>
@@ -25138,9 +25537,7 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -25154,7 +25551,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="B1" s="46" t="s">
         <v>1081</v>
@@ -25173,7 +25570,9 @@
       <c r="A2" s="47" t="s">
         <v>1091</v>
       </c>
-      <c r="B2" s="47"/>
+      <c r="B2" s="47" t="s">
+        <v>1157</v>
+      </c>
       <c r="C2" s="47">
         <v>1</v>
       </c>
@@ -25188,7 +25587,9 @@
       <c r="A3" s="47" t="s">
         <v>1092</v>
       </c>
-      <c r="B3" s="47"/>
+      <c r="B3" s="47" t="s">
+        <v>1158</v>
+      </c>
       <c r="C3" s="47">
         <v>1.3</v>
       </c>
@@ -25203,7 +25604,9 @@
       <c r="A4" s="47" t="s">
         <v>1093</v>
       </c>
-      <c r="B4" s="47"/>
+      <c r="B4" s="47" t="s">
+        <v>1159</v>
+      </c>
       <c r="C4" s="47">
         <v>1.6</v>
       </c>
@@ -25218,7 +25621,9 @@
       <c r="A5" s="47" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="47"/>
+      <c r="B5" s="47" t="s">
+        <v>1114</v>
+      </c>
       <c r="C5" s="47">
         <v>1</v>
       </c>
@@ -25242,9 +25647,7 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -25258,7 +25661,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="B1" s="46" t="s">
         <v>1081</v>
@@ -25277,7 +25680,9 @@
       <c r="A2" s="47" t="s">
         <v>1088</v>
       </c>
-      <c r="B2" s="47"/>
+      <c r="B2" s="47" t="s">
+        <v>1160</v>
+      </c>
       <c r="C2" s="47">
         <v>1</v>
       </c>
@@ -25292,7 +25697,9 @@
       <c r="A3" s="47" t="s">
         <v>1094</v>
       </c>
-      <c r="B3" s="47"/>
+      <c r="B3" s="47" t="s">
+        <v>1161</v>
+      </c>
       <c r="C3" s="47">
         <v>1.1000000000000001</v>
       </c>
@@ -25307,7 +25714,9 @@
       <c r="A4" s="47" t="s">
         <v>1095</v>
       </c>
-      <c r="B4" s="47"/>
+      <c r="B4" s="47" t="s">
+        <v>1162</v>
+      </c>
       <c r="C4" s="47">
         <v>1.5</v>
       </c>
@@ -25322,7 +25731,9 @@
       <c r="A5" s="47" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="47"/>
+      <c r="B5" s="47" t="s">
+        <v>1114</v>
+      </c>
       <c r="C5" s="47">
         <v>1</v>
       </c>
@@ -25346,9 +25757,7 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E5"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -25362,7 +25771,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="B1" s="46" t="s">
         <v>1081</v>
@@ -25381,7 +25790,9 @@
       <c r="A2" s="47" t="s">
         <v>1096</v>
       </c>
-      <c r="B2" s="47"/>
+      <c r="B2" s="47" t="s">
+        <v>1163</v>
+      </c>
       <c r="C2" s="47">
         <v>1</v>
       </c>
@@ -25396,7 +25807,9 @@
       <c r="A3" s="47" t="s">
         <v>1097</v>
       </c>
-      <c r="B3" s="47"/>
+      <c r="B3" s="47" t="s">
+        <v>1164</v>
+      </c>
       <c r="C3" s="47">
         <v>1.3</v>
       </c>
@@ -25411,7 +25824,9 @@
       <c r="A4" s="47" t="s">
         <v>1098</v>
       </c>
-      <c r="B4" s="47"/>
+      <c r="B4" s="47" t="s">
+        <v>1165</v>
+      </c>
       <c r="C4" s="47">
         <v>1.6</v>
       </c>
@@ -25426,7 +25841,9 @@
       <c r="A5" s="47" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="47"/>
+      <c r="B5" s="47" t="s">
+        <v>1114</v>
+      </c>
       <c r="C5" s="47">
         <v>1</v>
       </c>
@@ -25448,11 +25865,9 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E6"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -25466,7 +25881,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="B1" s="46" t="s">
         <v>1081</v>
@@ -25483,76 +25898,103 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
-        <v>1021</v>
-      </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48">
+        <v>1187</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C2" s="51">
         <v>1</v>
       </c>
-      <c r="D2" s="48">
-        <v>10</v>
-      </c>
-      <c r="E2" s="48">
+      <c r="D2" s="51">
+        <v>1</v>
+      </c>
+      <c r="E2" s="51">
         <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
-        <v>1022</v>
-      </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="48">
+        <v>1188</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C3" s="38">
         <v>1.3</v>
       </c>
-      <c r="D3" s="48">
-        <v>10</v>
-      </c>
-      <c r="E3" s="48">
-        <v>4</v>
+      <c r="D3" s="38">
+        <v>1.3</v>
+      </c>
+      <c r="E3" s="38">
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
-        <v>1099</v>
-      </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="48">
-        <v>1.6</v>
-      </c>
-      <c r="D4" s="48">
-        <v>10</v>
-      </c>
-      <c r="E4" s="48">
-        <v>5.5</v>
+        <v>1189</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C4" s="51">
+        <v>2</v>
+      </c>
+      <c r="D4" s="51">
+        <v>2</v>
+      </c>
+      <c r="E4" s="51">
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
-        <v>1100</v>
-      </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="48">
-        <v>1.8</v>
-      </c>
-      <c r="D5" s="48">
-        <v>10</v>
-      </c>
-      <c r="E5" s="48">
-        <v>8</v>
+        <v>1190</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C5" s="51">
+        <v>4</v>
+      </c>
+      <c r="D5" s="51">
+        <v>4</v>
+      </c>
+      <c r="E5" s="51">
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B6" s="50" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C6" s="51">
+        <v>6</v>
+      </c>
+      <c r="D6" s="51">
+        <v>6</v>
+      </c>
+      <c r="E6" s="51">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="47" t="s">
         <v>400</v>
       </c>
-      <c r="B6" s="47"/>
-      <c r="C6" s="48">
+      <c r="B7" s="47" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C7" s="51">
         <v>1</v>
       </c>
-      <c r="D6" s="48">
-        <v>10</v>
-      </c>
-      <c r="E6" s="48">
+      <c r="D7" s="51">
+        <v>10</v>
+      </c>
+      <c r="E7" s="51">
         <v>0.5</v>
       </c>
     </row>
@@ -25567,11 +26009,9 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E6"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -25585,7 +26025,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="B1" s="46" t="s">
         <v>1081</v>
@@ -25602,76 +26042,103 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
-        <v>1021</v>
-      </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48">
+        <v>1194</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C2" s="52">
         <v>1</v>
       </c>
-      <c r="D2" s="48">
-        <v>10</v>
-      </c>
-      <c r="E2" s="48">
+      <c r="D2" s="52">
+        <v>1</v>
+      </c>
+      <c r="E2" s="52">
         <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
-        <v>1022</v>
-      </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="48">
+        <v>1195</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C3" s="52">
         <v>1.3</v>
       </c>
-      <c r="D3" s="48">
-        <v>10</v>
-      </c>
-      <c r="E3" s="48">
-        <v>4</v>
+      <c r="D3" s="52">
+        <v>1.3</v>
+      </c>
+      <c r="E3" s="52">
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
-        <v>1099</v>
-      </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="48">
-        <v>1.6</v>
-      </c>
-      <c r="D4" s="48">
-        <v>10</v>
-      </c>
-      <c r="E4" s="48">
-        <v>5.5</v>
+        <v>1196</v>
+      </c>
+      <c r="B4" s="52" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C4" s="52">
+        <v>2</v>
+      </c>
+      <c r="D4" s="52">
+        <v>2</v>
+      </c>
+      <c r="E4" s="52">
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
-        <v>1100</v>
-      </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="48">
-        <v>1.8</v>
-      </c>
-      <c r="D5" s="48">
-        <v>10</v>
-      </c>
-      <c r="E5" s="48">
-        <v>8</v>
+        <v>1197</v>
+      </c>
+      <c r="B5" s="52" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C5" s="52">
+        <v>4</v>
+      </c>
+      <c r="D5" s="52">
+        <v>4</v>
+      </c>
+      <c r="E5" s="52">
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B6" s="52" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C6" s="52">
+        <v>6</v>
+      </c>
+      <c r="D6" s="52">
+        <v>6</v>
+      </c>
+      <c r="E6" s="52">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="47" t="s">
         <v>400</v>
       </c>
-      <c r="B6" s="47"/>
-      <c r="C6" s="48">
+      <c r="B7" s="52" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C7" s="52">
         <v>1</v>
       </c>
-      <c r="D6" s="48">
-        <v>10</v>
-      </c>
-      <c r="E6" s="48">
+      <c r="D7" s="52">
+        <v>10</v>
+      </c>
+      <c r="E7" s="52">
         <v>0.5</v>
       </c>
     </row>
@@ -25688,9 +26155,7 @@
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E6"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -25704,7 +26169,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="B1" s="46" t="s">
         <v>1081</v>
@@ -25721,76 +26186,86 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
-        <v>1021</v>
-      </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48">
+        <v>1199</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>1173</v>
+      </c>
+      <c r="C2" s="51">
         <v>1</v>
       </c>
-      <c r="D2" s="48">
-        <v>10</v>
-      </c>
-      <c r="E2" s="48">
+      <c r="D2" s="51">
+        <v>1</v>
+      </c>
+      <c r="E2" s="51">
         <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
-        <v>1022</v>
-      </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="48">
-        <v>1.3</v>
-      </c>
-      <c r="D3" s="48">
-        <v>10</v>
-      </c>
-      <c r="E3" s="48">
-        <v>4</v>
+        <v>1200</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C3" s="51">
+        <v>2</v>
+      </c>
+      <c r="D3" s="51">
+        <v>2</v>
+      </c>
+      <c r="E3" s="51">
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
-        <v>1099</v>
-      </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="48">
-        <v>1.6</v>
-      </c>
-      <c r="D4" s="48">
-        <v>10</v>
-      </c>
-      <c r="E4" s="48">
-        <v>5.5</v>
+        <v>1201</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C4" s="51">
+        <v>4</v>
+      </c>
+      <c r="D4" s="51">
+        <v>4</v>
+      </c>
+      <c r="E4" s="51">
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
-        <v>1100</v>
-      </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="48">
-        <v>1.8</v>
-      </c>
-      <c r="D5" s="48">
-        <v>10</v>
-      </c>
-      <c r="E5" s="48">
-        <v>8</v>
+        <v>1191</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C5" s="51">
+        <v>6</v>
+      </c>
+      <c r="D5" s="51">
+        <v>6</v>
+      </c>
+      <c r="E5" s="51">
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
         <v>400</v>
       </c>
-      <c r="B6" s="47"/>
-      <c r="C6" s="48">
-        <v>1</v>
-      </c>
-      <c r="D6" s="48">
-        <v>10</v>
-      </c>
-      <c r="E6" s="48">
+      <c r="B6" s="47" t="s">
+        <v>1177</v>
+      </c>
+      <c r="C6" s="51">
+        <v>1.5</v>
+      </c>
+      <c r="D6" s="51">
+        <v>10</v>
+      </c>
+      <c r="E6" s="51">
         <v>0.5</v>
       </c>
     </row>
@@ -25805,15 +26280,13 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E6"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.44140625" bestFit="1" customWidth="1"/>
@@ -25823,7 +26296,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>1108</v>
+        <v>1205</v>
       </c>
       <c r="B1" s="46" t="s">
         <v>1081</v>
@@ -25840,76 +26313,103 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
-        <v>1021</v>
-      </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48">
+        <v>1194</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C2" s="52">
         <v>1</v>
       </c>
-      <c r="D2" s="48">
-        <v>10</v>
-      </c>
-      <c r="E2" s="48">
+      <c r="D2" s="52">
+        <v>1</v>
+      </c>
+      <c r="E2" s="52">
         <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
-        <v>1022</v>
-      </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="48">
+        <v>1195</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C3" s="52">
         <v>1.3</v>
       </c>
-      <c r="D3" s="48">
-        <v>10</v>
-      </c>
-      <c r="E3" s="48">
-        <v>4</v>
+      <c r="D3" s="52">
+        <v>1.3</v>
+      </c>
+      <c r="E3" s="52">
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
-        <v>1099</v>
-      </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="48">
-        <v>1.6</v>
-      </c>
-      <c r="D4" s="48">
-        <v>10</v>
-      </c>
-      <c r="E4" s="48">
-        <v>5.5</v>
+        <v>1196</v>
+      </c>
+      <c r="B4" s="52" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C4" s="52">
+        <v>2</v>
+      </c>
+      <c r="D4" s="52">
+        <v>2</v>
+      </c>
+      <c r="E4" s="52">
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
-        <v>1100</v>
-      </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="48">
-        <v>1.8</v>
-      </c>
-      <c r="D5" s="48">
-        <v>10</v>
-      </c>
-      <c r="E5" s="48">
-        <v>8</v>
+        <v>1197</v>
+      </c>
+      <c r="B5" s="52" t="s">
+        <v>1179</v>
+      </c>
+      <c r="C5" s="52">
+        <v>4</v>
+      </c>
+      <c r="D5" s="52">
+        <v>4</v>
+      </c>
+      <c r="E5" s="52">
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B6" s="52" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C6" s="52">
+        <v>6</v>
+      </c>
+      <c r="D6" s="52">
+        <v>6</v>
+      </c>
+      <c r="E6" s="52">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="47" t="s">
         <v>400</v>
       </c>
-      <c r="B6" s="47"/>
-      <c r="C6" s="48">
-        <v>1</v>
-      </c>
-      <c r="D6" s="48">
-        <v>10</v>
-      </c>
-      <c r="E6" s="48">
+      <c r="B7" s="52" t="s">
+        <v>1181</v>
+      </c>
+      <c r="C7" s="52">
+        <v>1.5</v>
+      </c>
+      <c r="D7" s="52">
+        <v>10</v>
+      </c>
+      <c r="E7" s="52">
         <v>0.5</v>
       </c>
     </row>
@@ -25924,11 +26424,9 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E6"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -25942,7 +26440,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>1109</v>
+        <v>1106</v>
       </c>
       <c r="B1" s="46" t="s">
         <v>1081</v>
@@ -25959,76 +26457,103 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
-        <v>1021</v>
-      </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48">
+        <v>1194</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C2" s="52">
         <v>1</v>
       </c>
-      <c r="D2" s="48">
-        <v>10</v>
-      </c>
-      <c r="E2" s="48">
+      <c r="D2" s="52">
+        <v>1</v>
+      </c>
+      <c r="E2" s="52">
         <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
-        <v>1022</v>
-      </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="48">
+        <v>1195</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C3" s="52">
         <v>1.3</v>
       </c>
-      <c r="D3" s="48">
-        <v>10</v>
-      </c>
-      <c r="E3" s="48">
-        <v>4</v>
+      <c r="D3" s="52">
+        <v>1.3</v>
+      </c>
+      <c r="E3" s="52">
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
-        <v>1099</v>
-      </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="48">
-        <v>1.6</v>
-      </c>
-      <c r="D4" s="48">
-        <v>10</v>
-      </c>
-      <c r="E4" s="48">
-        <v>5.5</v>
+        <v>1196</v>
+      </c>
+      <c r="B4" s="52" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C4" s="52">
+        <v>2</v>
+      </c>
+      <c r="D4" s="52">
+        <v>2</v>
+      </c>
+      <c r="E4" s="52">
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
-        <v>1100</v>
-      </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="48">
-        <v>1.8</v>
-      </c>
-      <c r="D5" s="48">
-        <v>10</v>
-      </c>
-      <c r="E5" s="48">
-        <v>8</v>
+        <v>1197</v>
+      </c>
+      <c r="B5" s="52" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C5" s="52">
+        <v>4</v>
+      </c>
+      <c r="D5" s="52">
+        <v>4</v>
+      </c>
+      <c r="E5" s="52">
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B6" s="52" t="s">
+        <v>1184</v>
+      </c>
+      <c r="C6" s="52">
+        <v>6</v>
+      </c>
+      <c r="D6" s="52">
+        <v>6</v>
+      </c>
+      <c r="E6" s="52">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="47" t="s">
         <v>400</v>
       </c>
-      <c r="B6" s="47"/>
-      <c r="C6" s="48">
+      <c r="B7" s="52" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C7" s="52">
         <v>1</v>
       </c>
-      <c r="D6" s="48">
-        <v>10</v>
-      </c>
-      <c r="E6" s="48">
+      <c r="D7" s="52">
+        <v>10</v>
+      </c>
+      <c r="E7" s="52">
         <v>0.5</v>
       </c>
     </row>
@@ -26043,11 +26568,9 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E5"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -26061,7 +26584,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>1110</v>
+        <v>1107</v>
       </c>
       <c r="B1" s="46" t="s">
         <v>1081</v>
@@ -26078,61 +26601,103 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
-        <v>594</v>
-      </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48">
+        <v>1213</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C2" s="52">
         <v>1</v>
       </c>
-      <c r="D2" s="48">
-        <v>10</v>
-      </c>
-      <c r="E2" s="48">
+      <c r="D2" s="52">
+        <v>1</v>
+      </c>
+      <c r="E2" s="52">
         <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
-        <v>1101</v>
-      </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="48">
+        <v>1021</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C3" s="52">
         <v>1.3</v>
       </c>
-      <c r="D3" s="48">
-        <v>10</v>
-      </c>
-      <c r="E3" s="48">
-        <v>4</v>
+      <c r="D3" s="52">
+        <v>1.3</v>
+      </c>
+      <c r="E3" s="52">
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
-        <v>1031</v>
-      </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="48">
-        <v>1.6</v>
-      </c>
-      <c r="D4" s="48">
-        <v>10</v>
-      </c>
-      <c r="E4" s="48">
-        <v>8</v>
+        <v>1022</v>
+      </c>
+      <c r="B4" s="52" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C4" s="52">
+        <v>2</v>
+      </c>
+      <c r="D4" s="52">
+        <v>2</v>
+      </c>
+      <c r="E4" s="52">
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B5" s="52" t="s">
+        <v>1209</v>
+      </c>
+      <c r="C5" s="52">
+        <v>4</v>
+      </c>
+      <c r="D5" s="52">
+        <v>4</v>
+      </c>
+      <c r="E5" s="52">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="47" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B6" s="52" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C6" s="52">
+        <v>6</v>
+      </c>
+      <c r="D6" s="52">
+        <v>6</v>
+      </c>
+      <c r="E6" s="52">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="47" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="48">
+      <c r="B7" s="52" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C7" s="52">
         <v>1</v>
       </c>
-      <c r="D5" s="48">
-        <v>10</v>
-      </c>
-      <c r="E5" s="48">
+      <c r="D7" s="52">
+        <v>10</v>
+      </c>
+      <c r="E7" s="52">
         <v>0.5</v>
       </c>
     </row>
@@ -54938,10 +55503,10 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="49" t="s">
-        <v>1113</v>
-      </c>
-      <c r="B23" s="50" t="s">
+      <c r="A23" s="48" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B23" s="49" t="s">
         <v>406</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización table_data y sysdata: Valores ajustados para las condiciones observadas del alternador
</commit_message>
<xml_diff>
--- a/data-raw/excel-spreadsheets/table_data.xlsx
+++ b/data-raw/excel-spreadsheets/table_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CNAIM\data-raw\excel-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FCF618-1334-4182-8EEB-1C329EE8C4E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FC695A-7111-4AF4-8AB4-51F55C2C71C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" firstSheet="146" activeTab="159" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" firstSheet="213" activeTab="228" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -4240,7 +4240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4326,8 +4326,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14194,7 +14195,7 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -25903,13 +25904,13 @@
       <c r="B2" s="50" t="s">
         <v>1166</v>
       </c>
-      <c r="C2" s="51">
+      <c r="C2" s="52">
         <v>1</v>
       </c>
-      <c r="D2" s="51">
-        <v>1</v>
-      </c>
-      <c r="E2" s="51">
+      <c r="D2" s="52">
+        <v>10</v>
+      </c>
+      <c r="E2" s="52">
         <v>0.5</v>
       </c>
     </row>
@@ -25920,13 +25921,13 @@
       <c r="B3" s="38" t="s">
         <v>1192</v>
       </c>
-      <c r="C3" s="38">
-        <v>1.3</v>
-      </c>
-      <c r="D3" s="38">
-        <v>1.3</v>
-      </c>
-      <c r="E3" s="38">
+      <c r="C3" s="53">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D3" s="53">
+        <v>10</v>
+      </c>
+      <c r="E3" s="53">
         <v>0.5</v>
       </c>
     </row>
@@ -25937,13 +25938,13 @@
       <c r="B4" s="50" t="s">
         <v>1167</v>
       </c>
-      <c r="C4" s="51">
-        <v>2</v>
-      </c>
-      <c r="D4" s="51">
-        <v>2</v>
-      </c>
-      <c r="E4" s="51">
+      <c r="C4" s="52">
+        <v>1.3</v>
+      </c>
+      <c r="D4" s="52">
+        <v>10</v>
+      </c>
+      <c r="E4" s="52">
         <v>0.5</v>
       </c>
     </row>
@@ -25954,14 +25955,14 @@
       <c r="B5" s="50" t="s">
         <v>1168</v>
       </c>
-      <c r="C5" s="51">
-        <v>4</v>
-      </c>
-      <c r="D5" s="51">
-        <v>4</v>
-      </c>
-      <c r="E5" s="51">
-        <v>0.5</v>
+      <c r="C5" s="52">
+        <v>1.5</v>
+      </c>
+      <c r="D5" s="52">
+        <v>10</v>
+      </c>
+      <c r="E5" s="52">
+        <v>5.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -25971,14 +25972,14 @@
       <c r="B6" s="50" t="s">
         <v>1169</v>
       </c>
-      <c r="C6" s="51">
-        <v>6</v>
-      </c>
-      <c r="D6" s="51">
-        <v>6</v>
-      </c>
-      <c r="E6" s="51">
-        <v>0.5</v>
+      <c r="C6" s="52">
+        <v>1.6</v>
+      </c>
+      <c r="D6" s="52">
+        <v>10</v>
+      </c>
+      <c r="E6" s="52">
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -25988,19 +25989,19 @@
       <c r="B7" s="47" t="s">
         <v>1114</v>
       </c>
-      <c r="C7" s="51">
+      <c r="C7" s="52">
         <v>1</v>
       </c>
-      <c r="D7" s="51">
-        <v>10</v>
-      </c>
-      <c r="E7" s="51">
+      <c r="D7" s="52">
+        <v>10</v>
+      </c>
+      <c r="E7" s="52">
         <v>0.5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -26044,14 +26045,14 @@
       <c r="A2" s="47" t="s">
         <v>1194</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="51" t="s">
         <v>1202</v>
       </c>
       <c r="C2" s="52">
         <v>1</v>
       </c>
       <c r="D2" s="52">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E2" s="52">
         <v>0.5</v>
@@ -26061,16 +26062,16 @@
       <c r="A3" s="47" t="s">
         <v>1195</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="51" t="s">
         <v>1193</v>
       </c>
-      <c r="C3" s="52">
-        <v>1.3</v>
-      </c>
-      <c r="D3" s="52">
-        <v>1.3</v>
-      </c>
-      <c r="E3" s="52">
+      <c r="C3" s="53">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D3" s="53">
+        <v>10</v>
+      </c>
+      <c r="E3" s="53">
         <v>0.5</v>
       </c>
     </row>
@@ -26078,14 +26079,14 @@
       <c r="A4" s="47" t="s">
         <v>1196</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="51" t="s">
         <v>1170</v>
       </c>
       <c r="C4" s="52">
-        <v>2</v>
+        <v>1.3</v>
       </c>
       <c r="D4" s="52">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E4" s="52">
         <v>0.5</v>
@@ -26095,41 +26096,41 @@
       <c r="A5" s="47" t="s">
         <v>1197</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="51" t="s">
         <v>1171</v>
       </c>
       <c r="C5" s="52">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="D5" s="52">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E5" s="52">
-        <v>0.5</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
         <v>1198</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="51" t="s">
         <v>1172</v>
       </c>
       <c r="C6" s="52">
-        <v>6</v>
+        <v>1.6</v>
       </c>
       <c r="D6" s="52">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E6" s="52">
-        <v>0.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
         <v>400</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="51" t="s">
         <v>1114</v>
       </c>
       <c r="C7" s="52">
@@ -26191,13 +26192,13 @@
       <c r="B2" s="50" t="s">
         <v>1173</v>
       </c>
-      <c r="C2" s="51">
+      <c r="C2" s="52">
         <v>1</v>
       </c>
-      <c r="D2" s="51">
-        <v>1</v>
-      </c>
-      <c r="E2" s="51">
+      <c r="D2" s="52">
+        <v>10</v>
+      </c>
+      <c r="E2" s="52">
         <v>0.5</v>
       </c>
     </row>
@@ -26208,13 +26209,13 @@
       <c r="B3" s="50" t="s">
         <v>1174</v>
       </c>
-      <c r="C3" s="51">
-        <v>2</v>
-      </c>
-      <c r="D3" s="51">
-        <v>2</v>
-      </c>
-      <c r="E3" s="51">
+      <c r="C3" s="52">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D3" s="52">
+        <v>10</v>
+      </c>
+      <c r="E3" s="52">
         <v>0.5</v>
       </c>
     </row>
@@ -26225,14 +26226,14 @@
       <c r="B4" s="50" t="s">
         <v>1175</v>
       </c>
-      <c r="C4" s="51">
-        <v>4</v>
-      </c>
-      <c r="D4" s="51">
-        <v>4</v>
-      </c>
-      <c r="E4" s="51">
-        <v>0.5</v>
+      <c r="C4" s="52">
+        <v>1.3</v>
+      </c>
+      <c r="D4" s="52">
+        <v>10</v>
+      </c>
+      <c r="E4" s="52">
+        <v>5.5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -26242,14 +26243,14 @@
       <c r="B5" s="50" t="s">
         <v>1176</v>
       </c>
-      <c r="C5" s="51">
-        <v>6</v>
-      </c>
-      <c r="D5" s="51">
-        <v>6</v>
-      </c>
-      <c r="E5" s="51">
-        <v>0.5</v>
+      <c r="C5" s="52">
+        <v>1.5</v>
+      </c>
+      <c r="D5" s="52">
+        <v>10</v>
+      </c>
+      <c r="E5" s="52">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -26259,13 +26260,13 @@
       <c r="B6" s="47" t="s">
         <v>1177</v>
       </c>
-      <c r="C6" s="51">
-        <v>1.5</v>
-      </c>
-      <c r="D6" s="51">
-        <v>10</v>
-      </c>
-      <c r="E6" s="51">
+      <c r="C6" s="52">
+        <v>1</v>
+      </c>
+      <c r="D6" s="52">
+        <v>10</v>
+      </c>
+      <c r="E6" s="52">
         <v>0.5</v>
       </c>
     </row>
@@ -26315,14 +26316,14 @@
       <c r="A2" s="47" t="s">
         <v>1194</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="51" t="s">
         <v>1203</v>
       </c>
       <c r="C2" s="52">
         <v>1</v>
       </c>
       <c r="D2" s="52">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E2" s="52">
         <v>0.5</v>
@@ -26332,16 +26333,16 @@
       <c r="A3" s="47" t="s">
         <v>1195</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="51" t="s">
         <v>1204</v>
       </c>
-      <c r="C3" s="52">
-        <v>1.3</v>
-      </c>
-      <c r="D3" s="52">
-        <v>1.3</v>
-      </c>
-      <c r="E3" s="52">
+      <c r="C3" s="53">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D3" s="53">
+        <v>10</v>
+      </c>
+      <c r="E3" s="53">
         <v>0.5</v>
       </c>
     </row>
@@ -26349,14 +26350,14 @@
       <c r="A4" s="47" t="s">
         <v>1196</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="51" t="s">
         <v>1178</v>
       </c>
       <c r="C4" s="52">
-        <v>2</v>
+        <v>1.3</v>
       </c>
       <c r="D4" s="52">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E4" s="52">
         <v>0.5</v>
@@ -26366,45 +26367,45 @@
       <c r="A5" s="47" t="s">
         <v>1197</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="51" t="s">
         <v>1179</v>
       </c>
       <c r="C5" s="52">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="D5" s="52">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E5" s="52">
-        <v>0.5</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
         <v>1198</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="51" t="s">
         <v>1180</v>
       </c>
       <c r="C6" s="52">
-        <v>6</v>
+        <v>1.6</v>
       </c>
       <c r="D6" s="52">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E6" s="52">
-        <v>0.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
         <v>400</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="51" t="s">
         <v>1181</v>
       </c>
       <c r="C7" s="52">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="D7" s="52">
         <v>10</v>
@@ -26459,14 +26460,14 @@
       <c r="A2" s="47" t="s">
         <v>1194</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="51" t="s">
         <v>1206</v>
       </c>
       <c r="C2" s="52">
         <v>1</v>
       </c>
       <c r="D2" s="52">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E2" s="52">
         <v>0.5</v>
@@ -26476,16 +26477,16 @@
       <c r="A3" s="47" t="s">
         <v>1195</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="51" t="s">
         <v>1207</v>
       </c>
-      <c r="C3" s="52">
-        <v>1.3</v>
-      </c>
-      <c r="D3" s="52">
-        <v>1.3</v>
-      </c>
-      <c r="E3" s="52">
+      <c r="C3" s="53">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D3" s="53">
+        <v>10</v>
+      </c>
+      <c r="E3" s="53">
         <v>0.5</v>
       </c>
     </row>
@@ -26493,14 +26494,14 @@
       <c r="A4" s="47" t="s">
         <v>1196</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="51" t="s">
         <v>1182</v>
       </c>
       <c r="C4" s="52">
-        <v>2</v>
+        <v>1.3</v>
       </c>
       <c r="D4" s="52">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E4" s="52">
         <v>0.5</v>
@@ -26510,41 +26511,41 @@
       <c r="A5" s="47" t="s">
         <v>1197</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="51" t="s">
         <v>1183</v>
       </c>
       <c r="C5" s="52">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="D5" s="52">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E5" s="52">
-        <v>0.5</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
         <v>1198</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="51" t="s">
         <v>1184</v>
       </c>
       <c r="C6" s="52">
-        <v>6</v>
+        <v>1.6</v>
       </c>
       <c r="D6" s="52">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E6" s="52">
-        <v>0.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
         <v>400</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="51" t="s">
         <v>1185</v>
       </c>
       <c r="C7" s="52">
@@ -26570,7 +26571,7 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -26603,14 +26604,14 @@
       <c r="A2" s="47" t="s">
         <v>1213</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="51" t="s">
         <v>1208</v>
       </c>
       <c r="C2" s="52">
         <v>1</v>
       </c>
       <c r="D2" s="52">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E2" s="52">
         <v>0.5</v>
@@ -26620,16 +26621,16 @@
       <c r="A3" s="47" t="s">
         <v>1021</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="51" t="s">
         <v>1211</v>
       </c>
-      <c r="C3" s="52">
-        <v>1.3</v>
-      </c>
-      <c r="D3" s="52">
-        <v>1.3</v>
-      </c>
-      <c r="E3" s="52">
+      <c r="C3" s="53">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D3" s="53">
+        <v>10</v>
+      </c>
+      <c r="E3" s="53">
         <v>0.5</v>
       </c>
     </row>
@@ -26637,14 +26638,14 @@
       <c r="A4" s="47" t="s">
         <v>1022</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="51" t="s">
         <v>1212</v>
       </c>
       <c r="C4" s="52">
-        <v>2</v>
+        <v>1.3</v>
       </c>
       <c r="D4" s="52">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E4" s="52">
         <v>0.5</v>
@@ -26654,41 +26655,41 @@
       <c r="A5" s="47" t="s">
         <v>1099</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="51" t="s">
         <v>1209</v>
       </c>
       <c r="C5" s="52">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="D5" s="52">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E5" s="52">
-        <v>0.5</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
         <v>1031</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="51" t="s">
         <v>1210</v>
       </c>
       <c r="C6" s="52">
-        <v>6</v>
+        <v>1.6</v>
       </c>
       <c r="D6" s="52">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E6" s="52">
-        <v>0.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
         <v>400</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="51" t="s">
         <v>1186</v>
       </c>
       <c r="C7" s="52">

</xml_diff>

<commit_message>
Actualización table_data: tablas para cof GE
</commit_message>
<xml_diff>
--- a/data-raw/excel-spreadsheets/table_data.xlsx
+++ b/data-raw/excel-spreadsheets/table_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CNAIM\data-raw\excel-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FC695A-7111-4AF4-8AB4-51F55C2C71C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FEB926-2A1E-444C-9ACF-2778A1C30013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" firstSheet="213" activeTab="228" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" firstSheet="244" activeTab="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -302,7 +302,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6738" uniqueCount="1214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6779" uniqueCount="1215">
   <si>
     <t>Health Index Asset Category</t>
   </si>
@@ -4013,14 +4013,18 @@
   <si>
     <t>Muy baja</t>
   </si>
+  <si>
+    <t>CMR equivalent</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000000000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -4240,7 +4244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4329,6 +4333,8 @@
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4716,8 +4722,8 @@
   </sheetPr>
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="A55" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22433,8 +22439,8 @@
   </sheetPr>
   <dimension ref="A1:C148"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E120" sqref="E120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26571,7 +26577,7 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -29457,7 +29463,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29532,8 +29538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-CF00-000000000000}">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30421,10 +30427,13 @@
 
 <file path=xl/worksheets/sheet245.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-D000-000000000000}">
-  <dimension ref="A1:H62"/>
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView topLeftCell="A52" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32047,6 +32056,32 @@
         <v>263015</v>
       </c>
     </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63" s="38" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B63" s="38">
+        <v>45</v>
+      </c>
+      <c r="C63" s="38">
+        <v>50</v>
+      </c>
+      <c r="D63" s="38">
+        <v>5</v>
+      </c>
+      <c r="E63" s="38">
+        <v>39863</v>
+      </c>
+      <c r="F63" s="38">
+        <v>99657</v>
+      </c>
+      <c r="G63" s="38">
+        <v>398629</v>
+      </c>
+      <c r="H63" s="38">
+        <v>87698</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -32055,15 +32090,18 @@
 
 <file path=xl/worksheets/sheet246.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-D100-000000000000}">
-  <dimension ref="A1:F72"/>
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54:B56"/>
+    <sheetView topLeftCell="A64" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.88671875" customWidth="1"/>
+    <col min="1" max="1" width="28.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46" customWidth="1"/>
     <col min="3" max="4" width="6.109375" customWidth="1"/>
     <col min="5" max="5" width="20.33203125" customWidth="1"/>
@@ -33121,6 +33159,64 @@
       <c r="D72" s="5"/>
       <c r="F72">
         <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="38" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B73" s="38" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C73" s="38">
+        <v>0</v>
+      </c>
+      <c r="D73" s="38">
+        <v>10</v>
+      </c>
+      <c r="E73" s="38" t="s">
+        <v>758</v>
+      </c>
+      <c r="F73" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="38" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B74" s="38" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C74" s="38">
+        <v>10</v>
+      </c>
+      <c r="D74" s="38">
+        <v>20</v>
+      </c>
+      <c r="E74" s="38" t="s">
+        <v>758</v>
+      </c>
+      <c r="F74" s="38">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="38" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B75" s="38" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C75" s="38">
+        <v>20</v>
+      </c>
+      <c r="D75" s="38"/>
+      <c r="E75" s="38" t="s">
+        <v>758</v>
+      </c>
+      <c r="F75" s="38">
+        <v>1.25</v>
       </c>
     </row>
   </sheetData>
@@ -33263,10 +33359,13 @@
 
 <file path=xl/worksheets/sheet248.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-D300-000000000000}">
-  <dimension ref="A1:D9"/>
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33402,6 +33501,20 @@
       </c>
       <c r="D9">
         <v>1.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="38" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B10" s="38">
+        <v>1</v>
+      </c>
+      <c r="C10" s="38">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D10" s="38">
+        <v>1.35</v>
       </c>
     </row>
   </sheetData>
@@ -33758,9 +33871,12 @@
 
 <file path=xl/worksheets/sheet251.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-D400-000000000000}">
-  <dimension ref="A1:E62"/>
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A49" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
@@ -34826,6 +34942,23 @@
       </c>
       <c r="E62">
         <v>36171</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="38" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B63" s="38">
+        <v>2.6027400000000001E-4</v>
+      </c>
+      <c r="C63" s="38">
+        <v>1.15E-4</v>
+      </c>
+      <c r="D63" s="38">
+        <v>1.9606160000000001E-3</v>
+      </c>
+      <c r="E63" s="38">
+        <v>23502</v>
       </c>
     </row>
   </sheetData>
@@ -35021,10 +35154,13 @@
 
 <file path=xl/worksheets/sheet255.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-D900-000000000000}">
-  <dimension ref="A1:Q26"/>
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23:Q26"/>
+    <sheetView topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36417,6 +36553,59 @@
         <v>96</v>
       </c>
     </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27" s="38" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B27" s="38">
+        <v>50</v>
+      </c>
+      <c r="C27" s="38">
+        <v>250</v>
+      </c>
+      <c r="D27" s="38">
+        <v>2500</v>
+      </c>
+      <c r="E27" s="38">
+        <v>0</v>
+      </c>
+      <c r="F27" s="38">
+        <v>0</v>
+      </c>
+      <c r="G27" s="38">
+        <v>0</v>
+      </c>
+      <c r="H27" s="38">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="I27" s="38">
+        <v>2E-3</v>
+      </c>
+      <c r="J27" s="38">
+        <v>0.02</v>
+      </c>
+      <c r="K27" s="38">
+        <v>0.2</v>
+      </c>
+      <c r="L27" s="38">
+        <v>3</v>
+      </c>
+      <c r="M27" s="38">
+        <v>30</v>
+      </c>
+      <c r="N27" s="38">
+        <v>50</v>
+      </c>
+      <c r="O27" s="38">
+        <v>40</v>
+      </c>
+      <c r="P27" s="38">
+        <v>10</v>
+      </c>
+      <c r="Q27" s="54">
+        <v>17048</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -36427,9 +36616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-DA00-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -36533,15 +36720,18 @@
 
 <file path=xl/worksheets/sheet257.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-DB00-000000000000}">
-  <dimension ref="A1:F42"/>
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView topLeftCell="A37" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="6.109375" customWidth="1"/>
     <col min="5" max="5" width="57" customWidth="1"/>
@@ -37265,6 +37455,58 @@
         <v>2.5</v>
       </c>
     </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="38" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38">
+        <v>0</v>
+      </c>
+      <c r="D43" s="38">
+        <v>10</v>
+      </c>
+      <c r="E43" s="38" t="s">
+        <v>822</v>
+      </c>
+      <c r="F43" s="38">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="38" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38">
+        <v>10</v>
+      </c>
+      <c r="D44" s="38">
+        <v>20</v>
+      </c>
+      <c r="E44" s="38" t="s">
+        <v>822</v>
+      </c>
+      <c r="F44" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="38" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B45" s="38"/>
+      <c r="C45" s="38">
+        <v>20</v>
+      </c>
+      <c r="D45" s="38"/>
+      <c r="E45" s="38" t="s">
+        <v>822</v>
+      </c>
+      <c r="F45" s="38">
+        <v>1.6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -37273,10 +37515,13 @@
 
 <file path=xl/worksheets/sheet258.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-DC00-000000000000}">
-  <dimension ref="A1:G10"/>
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37515,6 +37760,29 @@
         <v>0.5</v>
       </c>
       <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="38" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B11" s="38">
+        <v>0.8</v>
+      </c>
+      <c r="C11" s="38">
+        <v>1</v>
+      </c>
+      <c r="D11" s="38">
+        <v>1.5</v>
+      </c>
+      <c r="E11" s="38">
+        <v>2.5</v>
+      </c>
+      <c r="F11" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="G11" s="38">
         <v>1</v>
       </c>
     </row>
@@ -38106,10 +38374,13 @@
 
 <file path=xl/worksheets/sheet262.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-E000-000000000000}">
-  <dimension ref="A1:K41"/>
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView topLeftCell="A34" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39557,6 +39828,38 @@
         <v>230441</v>
       </c>
     </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="38" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B42" s="38">
+        <v>15</v>
+      </c>
+      <c r="C42" s="38">
+        <v>100</v>
+      </c>
+      <c r="D42" s="38">
+        <v>100</v>
+      </c>
+      <c r="E42" s="38">
+        <v>80</v>
+      </c>
+      <c r="F42" s="38">
+        <v>0</v>
+      </c>
+      <c r="G42" s="38">
+        <v>2</v>
+      </c>
+      <c r="H42" s="38">
+        <v>400</v>
+      </c>
+      <c r="I42" s="38">
+        <v>0.05</v>
+      </c>
+      <c r="J42" s="38">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -39565,15 +39868,18 @@
 
 <file path=xl/worksheets/sheet263.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D6C426-89EE-49AA-9C90-5B5D8351FDF2}">
-  <dimension ref="A1:E63"/>
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.88671875" customWidth="1"/>
     <col min="3" max="3" width="18.109375" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" customWidth="1"/>
@@ -40651,6 +40957,23 @@
         <v>1411803.68</v>
       </c>
     </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="38" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B64" s="38">
+        <v>110031.29</v>
+      </c>
+      <c r="C64" s="38">
+        <v>157187.56</v>
+      </c>
+      <c r="D64" s="38">
+        <v>235781.34</v>
+      </c>
+      <c r="E64" s="38">
+        <v>392968.9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -40659,15 +40982,18 @@
 
 <file path=xl/worksheets/sheet264.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB50D737-0212-40DC-B856-D8A5EC742BF6}">
-  <dimension ref="A1:F63"/>
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.88671875" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="5" width="10.6640625" customWidth="1"/>
@@ -41934,6 +42260,26 @@
         <v>9.7467999999999999E-2</v>
       </c>
     </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="38" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B64" s="38">
+        <v>1.2939000000000001E-2</v>
+      </c>
+      <c r="C64" s="38">
+        <v>1.4855999999999999E-2</v>
+      </c>
+      <c r="D64" s="38">
+        <v>3.4062000000000002E-2</v>
+      </c>
+      <c r="E64" s="38">
+        <v>5.5164999999999999E-2</v>
+      </c>
+      <c r="F64" s="38">
+        <v>9.7467999999999999E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -41941,10 +42287,13 @@
 
 <file path=xl/worksheets/sheet265.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317B802B-6900-474F-B2EC-A070196B70EF}">
-  <dimension ref="A1:G249"/>
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:G253"/>
   <sheetViews>
-    <sheetView topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="A197" sqref="A197"/>
+    <sheetView topLeftCell="A241" workbookViewId="0">
+      <selection activeCell="A253" sqref="A253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -47680,6 +48029,98 @@
         <v>137606</v>
       </c>
     </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A250" s="38" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B250" s="38" t="s">
+        <v>165</v>
+      </c>
+      <c r="C250" s="38">
+        <v>1424</v>
+      </c>
+      <c r="D250" s="38">
+        <v>1635</v>
+      </c>
+      <c r="E250" s="38">
+        <v>3748</v>
+      </c>
+      <c r="F250" s="38">
+        <v>6070</v>
+      </c>
+      <c r="G250" s="38">
+        <v>10725</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A251" s="38" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B251" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="C251" s="38">
+        <v>2034</v>
+      </c>
+      <c r="D251" s="38">
+        <v>2335</v>
+      </c>
+      <c r="E251" s="38">
+        <v>5354</v>
+      </c>
+      <c r="F251" s="38">
+        <v>8671</v>
+      </c>
+      <c r="G251" s="38">
+        <v>15321</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A252" s="38" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B252" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="C252" s="38">
+        <v>3051</v>
+      </c>
+      <c r="D252" s="38">
+        <v>3503</v>
+      </c>
+      <c r="E252" s="38">
+        <v>8031</v>
+      </c>
+      <c r="F252" s="38">
+        <v>13007</v>
+      </c>
+      <c r="G252" s="38">
+        <v>22981</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A253" s="38" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B253" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="C253" s="38">
+        <v>5085</v>
+      </c>
+      <c r="D253" s="38">
+        <v>5838</v>
+      </c>
+      <c r="E253" s="38">
+        <v>13385</v>
+      </c>
+      <c r="F253" s="38">
+        <v>21678</v>
+      </c>
+      <c r="G253" s="38">
+        <v>38302</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -47687,10 +48128,13 @@
 
 <file path=xl/worksheets/sheet266.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F99DD3C9-B330-4E74-8D65-7C1404034804}">
-  <dimension ref="A1:C63"/>
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -47698,9 +48142,10 @@
     <col min="1" max="1" width="37.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="73.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
@@ -47711,7 +48156,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -47722,7 +48167,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -47730,7 +48175,7 @@
         <v>3.9964920000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -47738,7 +48183,7 @@
         <v>3.9964920000000001E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -47746,7 +48191,7 @@
         <v>3.9964920000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -47754,7 +48199,7 @@
         <v>3.9964920000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -47762,7 +48207,7 @@
         <v>3.9964920000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -47770,7 +48215,7 @@
         <v>4.3598100000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -47778,7 +48223,7 @@
         <v>3.9964920000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -47788,8 +48233,9 @@
       <c r="C10" t="s">
         <v>996</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E10" s="55"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -47800,7 +48246,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -47808,7 +48254,7 @@
         <v>3.9964920000000001E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -47816,7 +48262,7 @@
         <v>4.3598100000000001E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -47824,7 +48270,7 @@
         <v>4.3598100000000001E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -47832,7 +48278,7 @@
         <v>4.3598100000000001E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -48269,6 +48715,15 @@
       <c r="C63" t="s">
         <v>1000</v>
       </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="38" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B64" s="38">
+        <v>0.11989476363991854</v>
+      </c>
+      <c r="C64" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -48277,10 +48732,13 @@
 
 <file path=xl/worksheets/sheet267.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1590256-6A55-46CA-A90D-5C856B0A45CE}">
-  <dimension ref="A1:F63"/>
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -49553,6 +50011,26 @@
         <v>4.7271000000000001</v>
       </c>
     </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="38" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B64" s="38">
+        <v>0.25109999999999999</v>
+      </c>
+      <c r="C64" s="38">
+        <v>0.90749999999999997</v>
+      </c>
+      <c r="D64" s="38">
+        <v>1.8915</v>
+      </c>
+      <c r="E64" s="38">
+        <v>3.1021000000000001</v>
+      </c>
+      <c r="F64" s="38">
+        <v>4.7271000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -49560,10 +50038,13 @@
 
 <file path=xl/worksheets/sheet268.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59BC7345-7AB9-4B72-8350-23628CD4A363}">
-  <dimension ref="A1:G249"/>
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:G253"/>
   <sheetViews>
-    <sheetView topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="A194" sqref="A194:A197"/>
+    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="A250" sqref="A250:A253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -55302,6 +55783,98 @@
       </c>
       <c r="G249">
         <v>6673737</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A250" s="38" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B250" s="38" t="s">
+        <v>165</v>
+      </c>
+      <c r="C250" s="38">
+        <v>27629</v>
+      </c>
+      <c r="D250" s="38">
+        <v>99853</v>
+      </c>
+      <c r="E250" s="38">
+        <v>208124</v>
+      </c>
+      <c r="F250" s="38">
+        <v>341328</v>
+      </c>
+      <c r="G250" s="38">
+        <v>520129</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A251" s="38" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B251" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="C251" s="38">
+        <v>39470</v>
+      </c>
+      <c r="D251" s="38">
+        <v>142648</v>
+      </c>
+      <c r="E251" s="38">
+        <v>297320</v>
+      </c>
+      <c r="F251" s="38">
+        <v>487612</v>
+      </c>
+      <c r="G251" s="38">
+        <v>743041</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A252" s="38" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B252" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="C252" s="38">
+        <v>59205</v>
+      </c>
+      <c r="D252" s="38">
+        <v>213972</v>
+      </c>
+      <c r="E252" s="38">
+        <v>445980</v>
+      </c>
+      <c r="F252" s="38">
+        <v>731417</v>
+      </c>
+      <c r="G252" s="38">
+        <v>1114562</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A253" s="38" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B253" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="C253" s="38">
+        <v>98674</v>
+      </c>
+      <c r="D253" s="38">
+        <v>356619</v>
+      </c>
+      <c r="E253" s="38">
+        <v>743301</v>
+      </c>
+      <c r="F253" s="38">
+        <v>1219029</v>
+      </c>
+      <c r="G253" s="38">
+        <v>1857603</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización table_data: Indicación de tablas a modificar por Miguel
</commit_message>
<xml_diff>
--- a/data-raw/excel-spreadsheets/table_data.xlsx
+++ b/data-raw/excel-spreadsheets/table_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CNAIM\data-raw\excel-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FEB926-2A1E-444C-9ACF-2778A1C30013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAEB59E-19F8-430D-88DC-E26F46EDAB16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" firstSheet="244" activeTab="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" firstSheet="83" activeTab="83" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -302,7 +302,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6779" uniqueCount="1215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6819" uniqueCount="1217">
   <si>
     <t>Health Index Asset Category</t>
   </si>
@@ -4016,6 +4016,12 @@
   <si>
     <t>CMR equivalent</t>
   </si>
+  <si>
+    <t>Estado como nuevo</t>
+  </si>
+  <si>
+    <t>Ligeramente deteriorado</t>
+  </si>
 </sst>
 </file>
 
@@ -4026,7 +4032,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -4132,6 +4138,13 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -4331,10 +4344,10 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -18677,10 +18690,13 @@
 
 <file path=xl/worksheets/sheet188.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-AC00-000000000000}">
-  <dimension ref="A1:E6"/>
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection sqref="A1:E6"/>
+      <selection activeCell="A7" sqref="A7:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18795,6 +18811,91 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>586</v>
+      </c>
+      <c r="C7" s="48">
+        <v>1</v>
+      </c>
+      <c r="D7" s="48">
+        <v>10</v>
+      </c>
+      <c r="E7" s="48">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="48" t="s">
+        <v>561</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>583</v>
+      </c>
+      <c r="C8" s="48">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D8" s="48">
+        <v>10</v>
+      </c>
+      <c r="E8" s="48">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="48" t="s">
+        <v>563</v>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>584</v>
+      </c>
+      <c r="C9" s="48">
+        <v>1.3</v>
+      </c>
+      <c r="D9" s="48">
+        <v>10</v>
+      </c>
+      <c r="E9" s="48">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="48" t="s">
+        <v>565</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>585</v>
+      </c>
+      <c r="C10" s="48">
+        <v>1.5</v>
+      </c>
+      <c r="D10" s="48">
+        <v>10</v>
+      </c>
+      <c r="E10" s="48">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="48" t="s">
+        <v>400</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>456</v>
+      </c>
+      <c r="C11" s="48">
+        <v>1</v>
+      </c>
+      <c r="D11" s="48">
+        <v>10</v>
+      </c>
+      <c r="E11" s="48">
+        <v>0.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -18803,10 +18904,13 @@
 
 <file path=xl/worksheets/sheet189.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-AD00-000000000000}">
-  <dimension ref="A1:E5"/>
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection sqref="A1:E5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18901,6 +19005,74 @@
         <v>10</v>
       </c>
       <c r="E5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="48" t="s">
+        <v>594</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>595</v>
+      </c>
+      <c r="C6" s="48">
+        <v>1</v>
+      </c>
+      <c r="D6" s="48">
+        <v>10</v>
+      </c>
+      <c r="E6" s="48">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="48" t="s">
+        <v>596</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>597</v>
+      </c>
+      <c r="C7" s="48">
+        <v>1.2</v>
+      </c>
+      <c r="D7" s="48">
+        <v>10</v>
+      </c>
+      <c r="E7" s="48">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="48" t="s">
+        <v>598</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>599</v>
+      </c>
+      <c r="C8" s="48">
+        <v>1.4</v>
+      </c>
+      <c r="D8" s="48">
+        <v>10</v>
+      </c>
+      <c r="E8" s="48">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="48" t="s">
+        <v>400</v>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>456</v>
+      </c>
+      <c r="C9" s="48">
+        <v>1</v>
+      </c>
+      <c r="D9" s="48">
+        <v>10</v>
+      </c>
+      <c r="E9" s="48">
         <v>0.5</v>
       </c>
     </row>
@@ -25910,13 +26082,13 @@
       <c r="B2" s="50" t="s">
         <v>1166</v>
       </c>
-      <c r="C2" s="52">
+      <c r="C2" s="54">
         <v>1</v>
       </c>
-      <c r="D2" s="52">
-        <v>10</v>
-      </c>
-      <c r="E2" s="52">
+      <c r="D2" s="54">
+        <v>10</v>
+      </c>
+      <c r="E2" s="54">
         <v>0.5</v>
       </c>
     </row>
@@ -25927,13 +26099,13 @@
       <c r="B3" s="38" t="s">
         <v>1192</v>
       </c>
-      <c r="C3" s="53">
+      <c r="C3" s="55">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D3" s="53">
-        <v>10</v>
-      </c>
-      <c r="E3" s="53">
+      <c r="D3" s="55">
+        <v>10</v>
+      </c>
+      <c r="E3" s="55">
         <v>0.5</v>
       </c>
     </row>
@@ -25944,13 +26116,13 @@
       <c r="B4" s="50" t="s">
         <v>1167</v>
       </c>
-      <c r="C4" s="52">
+      <c r="C4" s="54">
         <v>1.3</v>
       </c>
-      <c r="D4" s="52">
-        <v>10</v>
-      </c>
-      <c r="E4" s="52">
+      <c r="D4" s="54">
+        <v>10</v>
+      </c>
+      <c r="E4" s="54">
         <v>0.5</v>
       </c>
     </row>
@@ -25961,13 +26133,13 @@
       <c r="B5" s="50" t="s">
         <v>1168</v>
       </c>
-      <c r="C5" s="52">
+      <c r="C5" s="54">
         <v>1.5</v>
       </c>
-      <c r="D5" s="52">
-        <v>10</v>
-      </c>
-      <c r="E5" s="52">
+      <c r="D5" s="54">
+        <v>10</v>
+      </c>
+      <c r="E5" s="54">
         <v>5.5</v>
       </c>
     </row>
@@ -25978,13 +26150,13 @@
       <c r="B6" s="50" t="s">
         <v>1169</v>
       </c>
-      <c r="C6" s="52">
+      <c r="C6" s="54">
         <v>1.6</v>
       </c>
-      <c r="D6" s="52">
-        <v>10</v>
-      </c>
-      <c r="E6" s="52">
+      <c r="D6" s="54">
+        <v>10</v>
+      </c>
+      <c r="E6" s="54">
         <v>8</v>
       </c>
     </row>
@@ -25995,13 +26167,13 @@
       <c r="B7" s="47" t="s">
         <v>1114</v>
       </c>
-      <c r="C7" s="52">
+      <c r="C7" s="54">
         <v>1</v>
       </c>
-      <c r="D7" s="52">
-        <v>10</v>
-      </c>
-      <c r="E7" s="52">
+      <c r="D7" s="54">
+        <v>10</v>
+      </c>
+      <c r="E7" s="54">
         <v>0.5</v>
       </c>
     </row>
@@ -26054,13 +26226,13 @@
       <c r="B2" s="51" t="s">
         <v>1202</v>
       </c>
-      <c r="C2" s="52">
+      <c r="C2" s="54">
         <v>1</v>
       </c>
-      <c r="D2" s="52">
-        <v>10</v>
-      </c>
-      <c r="E2" s="52">
+      <c r="D2" s="54">
+        <v>10</v>
+      </c>
+      <c r="E2" s="54">
         <v>0.5</v>
       </c>
     </row>
@@ -26071,13 +26243,13 @@
       <c r="B3" s="51" t="s">
         <v>1193</v>
       </c>
-      <c r="C3" s="53">
+      <c r="C3" s="55">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D3" s="53">
-        <v>10</v>
-      </c>
-      <c r="E3" s="53">
+      <c r="D3" s="55">
+        <v>10</v>
+      </c>
+      <c r="E3" s="55">
         <v>0.5</v>
       </c>
     </row>
@@ -26088,13 +26260,13 @@
       <c r="B4" s="51" t="s">
         <v>1170</v>
       </c>
-      <c r="C4" s="52">
+      <c r="C4" s="54">
         <v>1.3</v>
       </c>
-      <c r="D4" s="52">
-        <v>10</v>
-      </c>
-      <c r="E4" s="52">
+      <c r="D4" s="54">
+        <v>10</v>
+      </c>
+      <c r="E4" s="54">
         <v>0.5</v>
       </c>
     </row>
@@ -26105,13 +26277,13 @@
       <c r="B5" s="51" t="s">
         <v>1171</v>
       </c>
-      <c r="C5" s="52">
+      <c r="C5" s="54">
         <v>1.5</v>
       </c>
-      <c r="D5" s="52">
-        <v>10</v>
-      </c>
-      <c r="E5" s="52">
+      <c r="D5" s="54">
+        <v>10</v>
+      </c>
+      <c r="E5" s="54">
         <v>5.5</v>
       </c>
     </row>
@@ -26122,13 +26294,13 @@
       <c r="B6" s="51" t="s">
         <v>1172</v>
       </c>
-      <c r="C6" s="52">
+      <c r="C6" s="54">
         <v>1.6</v>
       </c>
-      <c r="D6" s="52">
-        <v>10</v>
-      </c>
-      <c r="E6" s="52">
+      <c r="D6" s="54">
+        <v>10</v>
+      </c>
+      <c r="E6" s="54">
         <v>8</v>
       </c>
     </row>
@@ -26139,13 +26311,13 @@
       <c r="B7" s="51" t="s">
         <v>1114</v>
       </c>
-      <c r="C7" s="52">
+      <c r="C7" s="54">
         <v>1</v>
       </c>
-      <c r="D7" s="52">
-        <v>10</v>
-      </c>
-      <c r="E7" s="52">
+      <c r="D7" s="54">
+        <v>10</v>
+      </c>
+      <c r="E7" s="54">
         <v>0.5</v>
       </c>
     </row>
@@ -26198,13 +26370,13 @@
       <c r="B2" s="50" t="s">
         <v>1173</v>
       </c>
-      <c r="C2" s="52">
+      <c r="C2" s="54">
         <v>1</v>
       </c>
-      <c r="D2" s="52">
-        <v>10</v>
-      </c>
-      <c r="E2" s="52">
+      <c r="D2" s="54">
+        <v>10</v>
+      </c>
+      <c r="E2" s="54">
         <v>0.5</v>
       </c>
     </row>
@@ -26215,13 +26387,13 @@
       <c r="B3" s="50" t="s">
         <v>1174</v>
       </c>
-      <c r="C3" s="52">
+      <c r="C3" s="54">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D3" s="52">
-        <v>10</v>
-      </c>
-      <c r="E3" s="52">
+      <c r="D3" s="54">
+        <v>10</v>
+      </c>
+      <c r="E3" s="54">
         <v>0.5</v>
       </c>
     </row>
@@ -26232,13 +26404,13 @@
       <c r="B4" s="50" t="s">
         <v>1175</v>
       </c>
-      <c r="C4" s="52">
+      <c r="C4" s="54">
         <v>1.3</v>
       </c>
-      <c r="D4" s="52">
-        <v>10</v>
-      </c>
-      <c r="E4" s="52">
+      <c r="D4" s="54">
+        <v>10</v>
+      </c>
+      <c r="E4" s="54">
         <v>5.5</v>
       </c>
     </row>
@@ -26249,13 +26421,13 @@
       <c r="B5" s="50" t="s">
         <v>1176</v>
       </c>
-      <c r="C5" s="52">
+      <c r="C5" s="54">
         <v>1.5</v>
       </c>
-      <c r="D5" s="52">
-        <v>10</v>
-      </c>
-      <c r="E5" s="52">
+      <c r="D5" s="54">
+        <v>10</v>
+      </c>
+      <c r="E5" s="54">
         <v>8</v>
       </c>
     </row>
@@ -26266,13 +26438,13 @@
       <c r="B6" s="47" t="s">
         <v>1177</v>
       </c>
-      <c r="C6" s="52">
+      <c r="C6" s="54">
         <v>1</v>
       </c>
-      <c r="D6" s="52">
-        <v>10</v>
-      </c>
-      <c r="E6" s="52">
+      <c r="D6" s="54">
+        <v>10</v>
+      </c>
+      <c r="E6" s="54">
         <v>0.5</v>
       </c>
     </row>
@@ -26325,13 +26497,13 @@
       <c r="B2" s="51" t="s">
         <v>1203</v>
       </c>
-      <c r="C2" s="52">
+      <c r="C2" s="54">
         <v>1</v>
       </c>
-      <c r="D2" s="52">
-        <v>10</v>
-      </c>
-      <c r="E2" s="52">
+      <c r="D2" s="54">
+        <v>10</v>
+      </c>
+      <c r="E2" s="54">
         <v>0.5</v>
       </c>
     </row>
@@ -26342,13 +26514,13 @@
       <c r="B3" s="51" t="s">
         <v>1204</v>
       </c>
-      <c r="C3" s="53">
+      <c r="C3" s="55">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D3" s="53">
-        <v>10</v>
-      </c>
-      <c r="E3" s="53">
+      <c r="D3" s="55">
+        <v>10</v>
+      </c>
+      <c r="E3" s="55">
         <v>0.5</v>
       </c>
     </row>
@@ -26359,13 +26531,13 @@
       <c r="B4" s="51" t="s">
         <v>1178</v>
       </c>
-      <c r="C4" s="52">
+      <c r="C4" s="54">
         <v>1.3</v>
       </c>
-      <c r="D4" s="52">
-        <v>10</v>
-      </c>
-      <c r="E4" s="52">
+      <c r="D4" s="54">
+        <v>10</v>
+      </c>
+      <c r="E4" s="54">
         <v>0.5</v>
       </c>
     </row>
@@ -26376,13 +26548,13 @@
       <c r="B5" s="51" t="s">
         <v>1179</v>
       </c>
-      <c r="C5" s="52">
+      <c r="C5" s="54">
         <v>1.5</v>
       </c>
-      <c r="D5" s="52">
-        <v>10</v>
-      </c>
-      <c r="E5" s="52">
+      <c r="D5" s="54">
+        <v>10</v>
+      </c>
+      <c r="E5" s="54">
         <v>5.5</v>
       </c>
     </row>
@@ -26393,13 +26565,13 @@
       <c r="B6" s="51" t="s">
         <v>1180</v>
       </c>
-      <c r="C6" s="52">
+      <c r="C6" s="54">
         <v>1.6</v>
       </c>
-      <c r="D6" s="52">
-        <v>10</v>
-      </c>
-      <c r="E6" s="52">
+      <c r="D6" s="54">
+        <v>10</v>
+      </c>
+      <c r="E6" s="54">
         <v>8</v>
       </c>
     </row>
@@ -26410,13 +26582,13 @@
       <c r="B7" s="51" t="s">
         <v>1181</v>
       </c>
-      <c r="C7" s="52">
+      <c r="C7" s="54">
         <v>1</v>
       </c>
-      <c r="D7" s="52">
-        <v>10</v>
-      </c>
-      <c r="E7" s="52">
+      <c r="D7" s="54">
+        <v>10</v>
+      </c>
+      <c r="E7" s="54">
         <v>0.5</v>
       </c>
     </row>
@@ -26469,13 +26641,13 @@
       <c r="B2" s="51" t="s">
         <v>1206</v>
       </c>
-      <c r="C2" s="52">
+      <c r="C2" s="54">
         <v>1</v>
       </c>
-      <c r="D2" s="52">
-        <v>10</v>
-      </c>
-      <c r="E2" s="52">
+      <c r="D2" s="54">
+        <v>10</v>
+      </c>
+      <c r="E2" s="54">
         <v>0.5</v>
       </c>
     </row>
@@ -26486,13 +26658,13 @@
       <c r="B3" s="51" t="s">
         <v>1207</v>
       </c>
-      <c r="C3" s="53">
+      <c r="C3" s="55">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D3" s="53">
-        <v>10</v>
-      </c>
-      <c r="E3" s="53">
+      <c r="D3" s="55">
+        <v>10</v>
+      </c>
+      <c r="E3" s="55">
         <v>0.5</v>
       </c>
     </row>
@@ -26503,13 +26675,13 @@
       <c r="B4" s="51" t="s">
         <v>1182</v>
       </c>
-      <c r="C4" s="52">
+      <c r="C4" s="54">
         <v>1.3</v>
       </c>
-      <c r="D4" s="52">
-        <v>10</v>
-      </c>
-      <c r="E4" s="52">
+      <c r="D4" s="54">
+        <v>10</v>
+      </c>
+      <c r="E4" s="54">
         <v>0.5</v>
       </c>
     </row>
@@ -26520,13 +26692,13 @@
       <c r="B5" s="51" t="s">
         <v>1183</v>
       </c>
-      <c r="C5" s="52">
+      <c r="C5" s="54">
         <v>1.5</v>
       </c>
-      <c r="D5" s="52">
-        <v>10</v>
-      </c>
-      <c r="E5" s="52">
+      <c r="D5" s="54">
+        <v>10</v>
+      </c>
+      <c r="E5" s="54">
         <v>5.5</v>
       </c>
     </row>
@@ -26537,13 +26709,13 @@
       <c r="B6" s="51" t="s">
         <v>1184</v>
       </c>
-      <c r="C6" s="52">
+      <c r="C6" s="54">
         <v>1.6</v>
       </c>
-      <c r="D6" s="52">
-        <v>10</v>
-      </c>
-      <c r="E6" s="52">
+      <c r="D6" s="54">
+        <v>10</v>
+      </c>
+      <c r="E6" s="54">
         <v>8</v>
       </c>
     </row>
@@ -26554,13 +26726,13 @@
       <c r="B7" s="51" t="s">
         <v>1185</v>
       </c>
-      <c r="C7" s="52">
+      <c r="C7" s="54">
         <v>1</v>
       </c>
-      <c r="D7" s="52">
-        <v>10</v>
-      </c>
-      <c r="E7" s="52">
+      <c r="D7" s="54">
+        <v>10</v>
+      </c>
+      <c r="E7" s="54">
         <v>0.5</v>
       </c>
     </row>
@@ -26613,13 +26785,13 @@
       <c r="B2" s="51" t="s">
         <v>1208</v>
       </c>
-      <c r="C2" s="52">
+      <c r="C2" s="54">
         <v>1</v>
       </c>
-      <c r="D2" s="52">
-        <v>10</v>
-      </c>
-      <c r="E2" s="52">
+      <c r="D2" s="54">
+        <v>10</v>
+      </c>
+      <c r="E2" s="54">
         <v>0.5</v>
       </c>
     </row>
@@ -26630,13 +26802,13 @@
       <c r="B3" s="51" t="s">
         <v>1211</v>
       </c>
-      <c r="C3" s="53">
+      <c r="C3" s="55">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D3" s="53">
-        <v>10</v>
-      </c>
-      <c r="E3" s="53">
+      <c r="D3" s="55">
+        <v>10</v>
+      </c>
+      <c r="E3" s="55">
         <v>0.5</v>
       </c>
     </row>
@@ -26647,13 +26819,13 @@
       <c r="B4" s="51" t="s">
         <v>1212</v>
       </c>
-      <c r="C4" s="52">
+      <c r="C4" s="54">
         <v>1.3</v>
       </c>
-      <c r="D4" s="52">
-        <v>10</v>
-      </c>
-      <c r="E4" s="52">
+      <c r="D4" s="54">
+        <v>10</v>
+      </c>
+      <c r="E4" s="54">
         <v>0.5</v>
       </c>
     </row>
@@ -26664,13 +26836,13 @@
       <c r="B5" s="51" t="s">
         <v>1209</v>
       </c>
-      <c r="C5" s="52">
+      <c r="C5" s="54">
         <v>1.5</v>
       </c>
-      <c r="D5" s="52">
-        <v>10</v>
-      </c>
-      <c r="E5" s="52">
+      <c r="D5" s="54">
+        <v>10</v>
+      </c>
+      <c r="E5" s="54">
         <v>5.5</v>
       </c>
     </row>
@@ -26681,13 +26853,13 @@
       <c r="B6" s="51" t="s">
         <v>1210</v>
       </c>
-      <c r="C6" s="52">
+      <c r="C6" s="54">
         <v>1.6</v>
       </c>
-      <c r="D6" s="52">
-        <v>10</v>
-      </c>
-      <c r="E6" s="52">
+      <c r="D6" s="54">
+        <v>10</v>
+      </c>
+      <c r="E6" s="54">
         <v>8</v>
       </c>
     </row>
@@ -26698,13 +26870,13 @@
       <c r="B7" s="51" t="s">
         <v>1186</v>
       </c>
-      <c r="C7" s="52">
+      <c r="C7" s="54">
         <v>1</v>
       </c>
-      <c r="D7" s="52">
-        <v>10</v>
-      </c>
-      <c r="E7" s="52">
+      <c r="D7" s="54">
+        <v>10</v>
+      </c>
+      <c r="E7" s="54">
         <v>0.5</v>
       </c>
     </row>
@@ -30432,8 +30604,8 @@
   </sheetPr>
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView topLeftCell="A49" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36602,7 +36774,7 @@
       <c r="P27" s="38">
         <v>10</v>
       </c>
-      <c r="Q27" s="54">
+      <c r="Q27" s="52">
         <v>17048</v>
       </c>
     </row>
@@ -48233,7 +48405,7 @@
       <c r="C10" t="s">
         <v>996</v>
       </c>
-      <c r="E10" s="55"/>
+      <c r="E10" s="53"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -50043,7 +50215,7 @@
   </sheetPr>
   <dimension ref="A1:G253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
+    <sheetView topLeftCell="A241" workbookViewId="0">
       <selection activeCell="A250" sqref="A250:A253"/>
     </sheetView>
   </sheetViews>
@@ -63665,10 +63837,13 @@
 
 <file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5200-000000000000}">
-  <dimension ref="A1:E7"/>
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -63800,6 +63975,108 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="48" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C8" s="48">
+        <v>0.9</v>
+      </c>
+      <c r="D8" s="48">
+        <v>10</v>
+      </c>
+      <c r="E8" s="48">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="48" t="s">
+        <v>869</v>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>921</v>
+      </c>
+      <c r="C9" s="48">
+        <v>1</v>
+      </c>
+      <c r="D9" s="48">
+        <v>10</v>
+      </c>
+      <c r="E9" s="48">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="48" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>922</v>
+      </c>
+      <c r="C10" s="48">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D10" s="48">
+        <v>10</v>
+      </c>
+      <c r="E10" s="48">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="48" t="s">
+        <v>452</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>923</v>
+      </c>
+      <c r="C11" s="48">
+        <v>1.25</v>
+      </c>
+      <c r="D11" s="48">
+        <v>10</v>
+      </c>
+      <c r="E11" s="48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="48" t="s">
+        <v>454</v>
+      </c>
+      <c r="B12" s="48" t="s">
+        <v>924</v>
+      </c>
+      <c r="C12" s="48">
+        <v>1.4</v>
+      </c>
+      <c r="D12" s="48">
+        <v>10</v>
+      </c>
+      <c r="E12" s="48">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="48" t="s">
+        <v>400</v>
+      </c>
+      <c r="B13" s="48" t="s">
+        <v>456</v>
+      </c>
+      <c r="C13" s="48">
+        <v>1</v>
+      </c>
+      <c r="D13" s="48">
+        <v>10</v>
+      </c>
+      <c r="E13" s="48">
+        <v>0.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -63808,10 +64085,13 @@
 
 <file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5300-000000000000}">
-  <dimension ref="A1:E6"/>
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection sqref="A1:E6"/>
+      <selection activeCell="A7" sqref="A7:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -63923,6 +64203,91 @@
         <v>10</v>
       </c>
       <c r="E6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="48" t="s">
+        <v>896</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>919</v>
+      </c>
+      <c r="C7" s="48">
+        <v>1</v>
+      </c>
+      <c r="D7" s="48">
+        <v>10</v>
+      </c>
+      <c r="E7" s="48">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="48" t="s">
+        <v>897</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>914</v>
+      </c>
+      <c r="C8" s="48">
+        <v>1</v>
+      </c>
+      <c r="D8" s="48">
+        <v>10</v>
+      </c>
+      <c r="E8" s="48">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="48" t="s">
+        <v>452</v>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>900</v>
+      </c>
+      <c r="C9" s="48">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D9" s="48">
+        <v>10</v>
+      </c>
+      <c r="E9" s="48">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="48" t="s">
+        <v>454</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>901</v>
+      </c>
+      <c r="C10" s="48">
+        <v>1.3</v>
+      </c>
+      <c r="D10" s="48">
+        <v>10</v>
+      </c>
+      <c r="E10" s="48">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="48" t="s">
+        <v>400</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>456</v>
+      </c>
+      <c r="C11" s="48">
+        <v>1</v>
+      </c>
+      <c r="D11" s="48">
+        <v>10</v>
+      </c>
+      <c r="E11" s="48">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización de cof y cof financiero. Actualización de table_data y sysdata (tipos para cálculo de cof)
</commit_message>
<xml_diff>
--- a/data-raw/excel-spreadsheets/table_data.xlsx
+++ b/data-raw/excel-spreadsheets/table_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CNAIM\data-raw\excel-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAEB59E-19F8-430D-88DC-E26F46EDAB16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D710000E-7358-44C9-B4D0-EF0EEA813F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" firstSheet="83" activeTab="83" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" firstSheet="233" activeTab="244" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -302,7 +302,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6819" uniqueCount="1217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6822" uniqueCount="1217">
   <si>
     <t>Health Index Asset Category</t>
   </si>
@@ -4014,13 +4014,13 @@
     <t>Muy baja</t>
   </si>
   <si>
-    <t>CMR equivalent</t>
-  </si>
-  <si>
     <t>Estado como nuevo</t>
   </si>
   <si>
     <t>Ligeramente deteriorado</t>
+  </si>
+  <si>
+    <t>13.8kV</t>
   </si>
 </sst>
 </file>
@@ -30604,8 +30604,8 @@
   </sheetPr>
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32256,7 +32256,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -32267,8 +32267,8 @@
   </sheetPr>
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73"/>
+    <sheetView topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33338,7 +33338,7 @@
         <v>1064</v>
       </c>
       <c r="B73" s="38" t="s">
-        <v>1214</v>
+        <v>1216</v>
       </c>
       <c r="C73" s="38">
         <v>0</v>
@@ -33358,7 +33358,7 @@
         <v>1064</v>
       </c>
       <c r="B74" s="38" t="s">
-        <v>1214</v>
+        <v>1216</v>
       </c>
       <c r="C74" s="38">
         <v>10</v>
@@ -33378,7 +33378,7 @@
         <v>1064</v>
       </c>
       <c r="B75" s="38" t="s">
-        <v>1214</v>
+        <v>1216</v>
       </c>
       <c r="C75" s="38">
         <v>20</v>
@@ -36897,8 +36897,8 @@
   </sheetPr>
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView topLeftCell="A31" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37631,7 +37631,9 @@
       <c r="A43" s="38" t="s">
         <v>1064</v>
       </c>
-      <c r="B43" s="38"/>
+      <c r="B43" s="38" t="s">
+        <v>1216</v>
+      </c>
       <c r="C43" s="38">
         <v>0</v>
       </c>
@@ -37649,7 +37651,9 @@
       <c r="A44" s="38" t="s">
         <v>1064</v>
       </c>
-      <c r="B44" s="38"/>
+      <c r="B44" s="38" t="s">
+        <v>1216</v>
+      </c>
       <c r="C44" s="38">
         <v>10</v>
       </c>
@@ -37667,7 +37671,9 @@
       <c r="A45" s="38" t="s">
         <v>1064</v>
       </c>
-      <c r="B45" s="38"/>
+      <c r="B45" s="38" t="s">
+        <v>1216</v>
+      </c>
       <c r="C45" s="38">
         <v>20</v>
       </c>
@@ -63842,7 +63848,7 @@
   </sheetPr>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A8" sqref="A8:E13"/>
     </sheetView>
   </sheetViews>
@@ -63980,7 +63986,7 @@
         <v>1048</v>
       </c>
       <c r="B8" s="48" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="C8" s="48">
         <v>0.9</v>
@@ -64011,7 +64017,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="48" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B10" s="48" t="s">
         <v>922</v>

</xml_diff>

<commit_message>
Actualización tablas y cof seguridad GE
</commit_message>
<xml_diff>
--- a/data-raw/excel-spreadsheets/table_data.xlsx
+++ b/data-raw/excel-spreadsheets/table_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CNAIM\data-raw\excel-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D710000E-7358-44C9-B4D0-EF0EEA813F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA844A6E-01F5-4022-A7A0-15C57E872C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" firstSheet="233" activeTab="244" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" firstSheet="233" activeTab="252" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -265,22 +265,23 @@
     <sheet name="223" sheetId="215" r:id="rId250"/>
     <sheet name="224" sheetId="213" r:id="rId251"/>
     <sheet name="225" sheetId="216" r:id="rId252"/>
-    <sheet name="226" sheetId="217" r:id="rId253"/>
-    <sheet name="227" sheetId="248" r:id="rId254"/>
-    <sheet name="228" sheetId="218" r:id="rId255"/>
-    <sheet name="229" sheetId="219" r:id="rId256"/>
-    <sheet name="230" sheetId="220" r:id="rId257"/>
-    <sheet name="231" sheetId="221" r:id="rId258"/>
-    <sheet name="232" sheetId="222" r:id="rId259"/>
-    <sheet name="233" sheetId="223" r:id="rId260"/>
-    <sheet name="234" sheetId="224" r:id="rId261"/>
-    <sheet name="235" sheetId="225" r:id="rId262"/>
-    <sheet name="236" sheetId="249" r:id="rId263"/>
-    <sheet name="237" sheetId="250" r:id="rId264"/>
-    <sheet name="238" sheetId="251" r:id="rId265"/>
-    <sheet name="239" sheetId="252" r:id="rId266"/>
-    <sheet name="240" sheetId="253" r:id="rId267"/>
-    <sheet name="241" sheetId="254" r:id="rId268"/>
+    <sheet name="225A" sheetId="280" r:id="rId253"/>
+    <sheet name="226" sheetId="217" r:id="rId254"/>
+    <sheet name="227" sheetId="248" r:id="rId255"/>
+    <sheet name="228" sheetId="218" r:id="rId256"/>
+    <sheet name="229" sheetId="219" r:id="rId257"/>
+    <sheet name="230" sheetId="220" r:id="rId258"/>
+    <sheet name="231" sheetId="221" r:id="rId259"/>
+    <sheet name="232" sheetId="222" r:id="rId260"/>
+    <sheet name="233" sheetId="223" r:id="rId261"/>
+    <sheet name="234" sheetId="224" r:id="rId262"/>
+    <sheet name="235" sheetId="225" r:id="rId263"/>
+    <sheet name="236" sheetId="249" r:id="rId264"/>
+    <sheet name="237" sheetId="250" r:id="rId265"/>
+    <sheet name="238" sheetId="251" r:id="rId266"/>
+    <sheet name="239" sheetId="252" r:id="rId267"/>
+    <sheet name="240" sheetId="253" r:id="rId268"/>
+    <sheet name="241" sheetId="254" r:id="rId269"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -302,7 +303,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6822" uniqueCount="1217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6833" uniqueCount="1225">
   <si>
     <t>Health Index Asset Category</t>
   </si>
@@ -4021,6 +4022,30 @@
   </si>
   <si>
     <t>13.8kV</t>
+  </si>
+  <si>
+    <t>Factor de consecuencia de seguridad - Generadores</t>
+  </si>
+  <si>
+    <t>CALIFICACIÓN DE RIESGO DE UBICACIÓN</t>
+  </si>
+  <si>
+    <t>Bajo</t>
+  </si>
+  <si>
+    <t>Alto</t>
+  </si>
+  <si>
+    <t>Medio (Default)</t>
+  </si>
+  <si>
+    <t>CALIFICACIÓN DE RIESGO DE TIPO: Bajo</t>
+  </si>
+  <si>
+    <t>CALIFICACIÓN DE RIESGO DE TIPO: Medio (Default)</t>
+  </si>
+  <si>
+    <t>CALIFICACIÓN DE RIESGO DE TIPO: Alto</t>
   </si>
 </sst>
 </file>
@@ -30604,7 +30629,7 @@
   </sheetPr>
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A49" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
@@ -35143,9 +35168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-D700-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -35232,6 +35255,101 @@
 </file>
 
 <file path=xl/worksheets/sheet253.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA55BD2-31C1-4539-94DB-4CE4A51B9489}">
+  <sheetPr>
+    <tabColor theme="5"/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="34.88671875" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="33" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" customWidth="1"/>
+    <col min="7" max="1025" width="8.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="43" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>1222</v>
+      </c>
+      <c r="D1" s="43" t="s">
+        <v>1223</v>
+      </c>
+      <c r="E1" s="43" t="s">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="43" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C2" s="43">
+        <v>0.7</v>
+      </c>
+      <c r="D2" s="43">
+        <v>0.9</v>
+      </c>
+      <c r="E2" s="43">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="43" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C3" s="43">
+        <v>0.9</v>
+      </c>
+      <c r="D3" s="43">
+        <v>1</v>
+      </c>
+      <c r="E3" s="43">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="43" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C4" s="43">
+        <v>1.2</v>
+      </c>
+      <c r="D4" s="43">
+        <v>1.4</v>
+      </c>
+      <c r="E4" s="43">
+        <v>1.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet254.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-D800-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -35276,7 +35394,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet254.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet255.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6958CC5-9DF2-4A0E-9B47-F65C1C375716}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -35324,7 +35442,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet255.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet256.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-D900-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -36784,7 +36902,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet256.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet257.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-DA00-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -36890,7 +37008,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet257.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet258.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-DB00-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -37691,7 +37809,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet258.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet259.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-DC00-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -37962,51 +38080,6 @@
       </c>
       <c r="G11" s="38">
         <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet259.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-DD00-000000000000}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" customWidth="1"/>
-    <col min="3" max="1025" width="8.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>833</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>965</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>834</v>
-      </c>
-      <c r="B2">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>835</v>
-      </c>
-      <c r="B3">
-        <v>18.55</v>
       </c>
     </row>
   </sheetData>
@@ -38119,6 +38192,51 @@
 </file>
 
 <file path=xl/worksheets/sheet260.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-DD00-000000000000}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="3" max="1025" width="8.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>834</v>
+      </c>
+      <c r="B2">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>835</v>
+      </c>
+      <c r="B3">
+        <v>18.55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet261.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-DE00-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
@@ -38431,7 +38549,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet261.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet262.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-DF00-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -38550,7 +38668,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet262.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet263.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-E000-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -40044,7 +40162,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet263.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet264.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D6C426-89EE-49AA-9C90-5B5D8351FDF2}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -41158,7 +41276,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet264.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet265.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB50D737-0212-40DC-B856-D8A5EC742BF6}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -42463,7 +42581,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet265.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet266.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317B802B-6900-474F-B2EC-A070196B70EF}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -48304,7 +48422,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet266.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet267.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F99DD3C9-B330-4E74-8D65-7C1404034804}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -48908,7 +49026,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet267.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet268.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1590256-6A55-46CA-A90D-5C856B0A45CE}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -50214,7 +50332,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet268.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet269.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59BC7345-7AB9-4B72-8350-23628CD4A363}">
   <sheetPr>
     <tabColor theme="7"/>

</xml_diff>

<commit_message>
Actualización de pof de transformadores de distribución y tablas
</commit_message>
<xml_diff>
--- a/data-raw/excel-spreadsheets/table_data.xlsx
+++ b/data-raw/excel-spreadsheets/table_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CNAIM\data-raw\excel-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70D5098-0F85-4BC0-BEAE-08F393A58477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9CFFFA-3C3B-48DC-B2FC-F7FB6AC2A72C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" firstSheet="246" activeTab="268" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" firstSheet="164" activeTab="188" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -303,7 +303,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6867" uniqueCount="1248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6867" uniqueCount="1245">
   <si>
     <t>Health Index Asset Category</t>
   </si>
@@ -4048,9 +4048,6 @@
     <t>CALIFICACIÓN DE RIESGO DE TIPO: Alto</t>
   </si>
   <si>
-    <t>Deterioro especifico/menor</t>
-  </si>
-  <si>
     <t>El transformador puede presentar signos de envejecimiento o marcas (por ejemplo, rayaduras superficiales, musgo o líquenes que pueden eliminarse con un cepillado). Esto no tiene un impacto significativo en la probabilidad de falla del equipo</t>
   </si>
   <si>
@@ -4087,34 +4084,28 @@
     <t>Se registran niveles moderados de descargas parciales (por ejemplo, resultado “ámbar” en un dispositivo de medición TEV o valores entre el 10 % y el 30 % de lo recomendado por el fabricante).</t>
   </si>
   <si>
-    <t>Alta (no confirmada)</t>
-  </si>
-  <si>
     <t>Niveles elevados de descargas parciales que indican la posible presencia de un defecto en la planta o el equipo, lo cual requiere una investigación más detallada (por ejemplo, resultado “rojo” en un dispositivo de medición TEV o valores por encima de lo recomendado por el fabricante).</t>
   </si>
   <si>
-    <t>Alta (Confirmida)</t>
-  </si>
-  <si>
     <t>Descargas parciales elevadas. Se ha confirmado que la fuente de descarga parcial constituye una posible causa de falla.</t>
   </si>
   <si>
     <t>Temperatura normalmente esperada para la carga del transformador.</t>
   </si>
   <si>
-    <t>Moderamente elevada</t>
-  </si>
-  <si>
     <t>Temperatura ligeramente superior a la normalmente esperada para la carga del transformador.</t>
   </si>
   <si>
-    <t>Severamente elevada</t>
-  </si>
-  <si>
     <t>Temperatura significativamente superior a la normalmente esperada para la carga del transformador.</t>
   </si>
   <si>
     <t>Transformador 13.2 kV</t>
+  </si>
+  <si>
+    <t>Moderamente Alta</t>
+  </si>
+  <si>
+    <t>Muy Alta</t>
   </si>
 </sst>
 </file>
@@ -18801,9 +18792,7 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:E11"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -18922,7 +18911,7 @@
         <v>1021</v>
       </c>
       <c r="B7" s="57" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="C7" s="56">
         <v>1</v>
@@ -18939,7 +18928,7 @@
         <v>1022</v>
       </c>
       <c r="B8" s="57" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="C8" s="56">
         <v>1.1000000000000001</v>
@@ -18953,10 +18942,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="56" t="s">
-        <v>1238</v>
+        <v>1023</v>
       </c>
       <c r="B9" s="57" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="C9" s="56">
         <v>1.3</v>
@@ -18970,10 +18959,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="56" t="s">
-        <v>1240</v>
+        <v>1024</v>
       </c>
       <c r="B10" s="56" t="s">
-        <v>1241</v>
+        <v>1238</v>
       </c>
       <c r="C10" s="56">
         <v>1.5</v>
@@ -19015,8 +19004,8 @@
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:E9"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19119,7 +19108,7 @@
         <v>594</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>1242</v>
+        <v>1239</v>
       </c>
       <c r="C6" s="48">
         <v>1</v>
@@ -19136,7 +19125,7 @@
         <v>1243</v>
       </c>
       <c r="B7" s="48" t="s">
-        <v>1244</v>
+        <v>1240</v>
       </c>
       <c r="C7" s="48">
         <v>1.2</v>
@@ -19150,10 +19139,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="48" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="B8" s="48" t="s">
-        <v>1246</v>
+        <v>1241</v>
       </c>
       <c r="C8" s="48">
         <v>1.4</v>
@@ -35217,7 +35206,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="48" t="s">
-        <v>1247</v>
+        <v>1242</v>
       </c>
       <c r="B58" s="59">
         <v>2.6027400000000001E-5</v>
@@ -50724,7 +50713,7 @@
   </sheetPr>
   <dimension ref="A1:G257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -64591,10 +64580,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="56" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B9" s="56" t="s">
         <v>1225</v>
-      </c>
-      <c r="B9" s="56" t="s">
-        <v>1226</v>
       </c>
       <c r="C9" s="56">
         <v>1</v>
@@ -64611,7 +64600,7 @@
         <v>1215</v>
       </c>
       <c r="B10" s="57" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="C10" s="56">
         <v>1.1000000000000001</v>
@@ -64628,7 +64617,7 @@
         <v>1034</v>
       </c>
       <c r="B11" s="57" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="C11" s="56">
         <v>1.25</v>
@@ -64645,7 +64634,7 @@
         <v>1035</v>
       </c>
       <c r="B12" s="57" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="C12" s="56">
         <v>1.4</v>
@@ -64676,7 +64665,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -64803,10 +64792,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="56" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B7" s="56" t="s">
         <v>1230</v>
-      </c>
-      <c r="B7" s="56" t="s">
-        <v>1231</v>
       </c>
       <c r="C7" s="56">
         <v>1</v>
@@ -64820,10 +64809,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="56" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B8" s="57" t="s">
         <v>1232</v>
-      </c>
-      <c r="B8" s="57" t="s">
-        <v>1233</v>
       </c>
       <c r="C8" s="56">
         <v>1</v>
@@ -64840,7 +64829,7 @@
         <v>1034</v>
       </c>
       <c r="B9" s="57" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="C9" s="56">
         <v>1.1000000000000001</v>
@@ -64857,7 +64846,7 @@
         <v>1035</v>
       </c>
       <c r="B10" s="57" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="C10" s="56">
         <v>1.3</v>

</xml_diff>

<commit_message>
Actualización tablas y pof trafos dist
</commit_message>
<xml_diff>
--- a/data-raw/excel-spreadsheets/table_data.xlsx
+++ b/data-raw/excel-spreadsheets/table_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CNAIM\data-raw\excel-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9CFFFA-3C3B-48DC-B2FC-F7FB6AC2A72C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6BA514-A39E-49A1-86F9-DD1B6B24785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" firstSheet="164" activeTab="188" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -303,7 +303,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6867" uniqueCount="1245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6867" uniqueCount="1244">
   <si>
     <t>Health Index Asset Category</t>
   </si>
@@ -3599,9 +3599,6 @@
   </si>
   <si>
     <t>Max % Utilisation under normal operating conditions (Generador)</t>
-  </si>
-  <si>
-    <t>Transformador 13.2kV (GM)</t>
   </si>
   <si>
     <t>1. Cubierta, 2. Aislamiento, 3. Cables y de la caja de terminales, 4. Rotor, 5. Estator</t>
@@ -4832,7 +4829,7 @@
   </sheetPr>
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
@@ -5016,7 +5013,7 @@
         <v>26</v>
       </c>
       <c r="B22" s="48" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -8778,7 +8775,7 @@
         <v>177</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -9053,7 +9050,7 @@
         <v>1067</v>
       </c>
       <c r="C36" s="38" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -9064,7 +9061,7 @@
         <v>1068</v>
       </c>
       <c r="C37" s="38" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
   </sheetData>
@@ -10225,7 +10222,7 @@
   </sheetPr>
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -11775,29 +11772,29 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B1" s="43" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1" s="43" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="D1" s="43" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="E1" s="43" t="s">
         <v>1083</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>1084</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="38" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="C2" s="38">
         <v>1</v>
@@ -11814,7 +11811,7 @@
         <v>1034</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="C3" s="38">
         <v>1.4</v>
@@ -11831,7 +11828,7 @@
         <v>1035</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="C4" s="38">
         <v>1.8</v>
@@ -11848,7 +11845,7 @@
         <v>400</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C5" s="38">
         <v>1</v>
@@ -11889,29 +11886,29 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B1" s="43" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1" s="43" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="D1" s="43" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="E1" s="43" t="s">
         <v>1083</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>1084</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="38" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="C2" s="38">
         <v>1</v>
@@ -11928,7 +11925,7 @@
         <v>1034</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="C3" s="38">
         <v>1.2</v>
@@ -11945,7 +11942,7 @@
         <v>1035</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="C4" s="38">
         <v>1.8</v>
@@ -11962,7 +11959,7 @@
         <v>400</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C5" s="38">
         <v>1</v>
@@ -12003,29 +12000,29 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B1" s="43" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1" s="43" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="D1" s="43" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="E1" s="43" t="s">
         <v>1083</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>1084</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="38" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="C2" s="38">
         <v>1</v>
@@ -12042,7 +12039,7 @@
         <v>1034</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="C3" s="38">
         <v>1.2</v>
@@ -12059,7 +12056,7 @@
         <v>1035</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="C4" s="38">
         <v>1.4</v>
@@ -12076,7 +12073,7 @@
         <v>400</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C5" s="38">
         <v>1</v>
@@ -12231,7 +12228,7 @@
         <v>177</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -12506,7 +12503,7 @@
         <v>1067</v>
       </c>
       <c r="C36" s="38" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -12517,7 +12514,7 @@
         <v>1068</v>
       </c>
       <c r="C37" s="38" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
   </sheetData>
@@ -12549,29 +12546,29 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B1" s="43" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1" s="43" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="D1" s="43" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="E1" s="43" t="s">
         <v>1083</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>1084</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="38" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="C2" s="38">
         <v>1</v>
@@ -12588,7 +12585,7 @@
         <v>1034</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="C3" s="38">
         <v>1.2</v>
@@ -12605,7 +12602,7 @@
         <v>1035</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="C4" s="38">
         <v>1.4</v>
@@ -12622,7 +12619,7 @@
         <v>400</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C5" s="38">
         <v>1</v>
@@ -12663,29 +12660,29 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B1" s="43" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1" s="43" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="D1" s="43" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="E1" s="43" t="s">
         <v>1083</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>1084</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="38" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C2" s="38">
         <v>1</v>
@@ -12702,7 +12699,7 @@
         <v>1034</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C3" s="38">
         <v>1.2</v>
@@ -12719,7 +12716,7 @@
         <v>1035</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="C4" s="38">
         <v>1.4</v>
@@ -12736,7 +12733,7 @@
         <v>400</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C5" s="38">
         <v>1</v>
@@ -12777,29 +12774,29 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B1" s="43" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1" s="43" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="D1" s="43" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="E1" s="43" t="s">
         <v>1083</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>1084</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="38" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C2" s="38">
         <v>1</v>
@@ -12816,7 +12813,7 @@
         <v>1034</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="C3" s="38">
         <v>1.2</v>
@@ -12833,7 +12830,7 @@
         <v>1035</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="C4" s="38">
         <v>1.4</v>
@@ -12850,7 +12847,7 @@
         <v>400</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C5" s="38">
         <v>1</v>
@@ -12891,29 +12888,29 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B1" s="43" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1" s="43" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="D1" s="43" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="E1" s="43" t="s">
         <v>1083</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>1084</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="38" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="C2" s="38">
         <v>1</v>
@@ -12930,7 +12927,7 @@
         <v>1034</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="C3" s="38">
         <v>1.2</v>
@@ -12947,7 +12944,7 @@
         <v>1035</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="C4" s="38">
         <v>1.4</v>
@@ -12964,7 +12961,7 @@
         <v>400</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C5" s="38">
         <v>1</v>
@@ -13005,29 +13002,29 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B1" s="43" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1" s="43" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="D1" s="43" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="E1" s="43" t="s">
         <v>1083</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>1084</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="38" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="C2" s="38">
         <v>1</v>
@@ -13044,7 +13041,7 @@
         <v>1034</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="C3" s="38">
         <v>1.2</v>
@@ -13061,7 +13058,7 @@
         <v>1035</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="C4" s="38">
         <v>1.4</v>
@@ -13078,7 +13075,7 @@
         <v>400</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C5" s="38">
         <v>1</v>
@@ -13119,29 +13116,29 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B1" s="43" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1" s="43" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="D1" s="43" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="E1" s="43" t="s">
         <v>1083</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>1084</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="38" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="C2" s="38">
         <v>1</v>
@@ -13158,7 +13155,7 @@
         <v>1034</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="C3" s="38">
         <v>1.2</v>
@@ -13175,7 +13172,7 @@
         <v>1035</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="C4" s="38">
         <v>1.4</v>
@@ -13192,7 +13189,7 @@
         <v>400</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C5" s="38">
         <v>1</v>
@@ -13233,29 +13230,29 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B1" s="43" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1" s="43" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="D1" s="43" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="E1" s="43" t="s">
         <v>1083</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>1084</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="38" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="C2" s="38">
         <v>1</v>
@@ -13272,7 +13269,7 @@
         <v>1034</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="C3" s="38">
         <v>1.2</v>
@@ -13289,7 +13286,7 @@
         <v>1035</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="C4" s="38">
         <v>1.4</v>
@@ -13306,7 +13303,7 @@
         <v>400</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C5" s="38">
         <v>1</v>
@@ -13347,29 +13344,29 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B1" s="43" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1" s="43" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="D1" s="43" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="E1" s="43" t="s">
         <v>1083</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>1084</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="38" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="C2" s="38">
         <v>1</v>
@@ -13386,7 +13383,7 @@
         <v>1034</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="C3" s="38">
         <v>1.2</v>
@@ -13403,7 +13400,7 @@
         <v>1035</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C4" s="38">
         <v>1.4</v>
@@ -13420,7 +13417,7 @@
         <v>400</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C5" s="38">
         <v>1</v>
@@ -13461,29 +13458,29 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B1" s="43" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1" s="43" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="D1" s="43" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="E1" s="43" t="s">
         <v>1083</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>1084</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="38" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="C2" s="38">
         <v>1</v>
@@ -13500,7 +13497,7 @@
         <v>1034</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="C3" s="38">
         <v>1.2</v>
@@ -13517,7 +13514,7 @@
         <v>1035</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="C4" s="38">
         <v>1.4</v>
@@ -13534,7 +13531,7 @@
         <v>400</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C5" s="38">
         <v>1</v>
@@ -13575,29 +13572,29 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B1" s="43" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1" s="43" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="D1" s="43" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="E1" s="43" t="s">
         <v>1083</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>1084</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="38" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="C2" s="38">
         <v>1</v>
@@ -13614,7 +13611,7 @@
         <v>1034</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="C3" s="38">
         <v>1.2</v>
@@ -13631,7 +13628,7 @@
         <v>1035</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="C4" s="38">
         <v>1.4</v>
@@ -13648,7 +13645,7 @@
         <v>400</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C5" s="38">
         <v>1</v>
@@ -14327,29 +14324,29 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B1" s="43" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1" s="43" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="D1" s="43" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="E1" s="43" t="s">
         <v>1083</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>1084</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="38" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="C2" s="38">
         <v>1</v>
@@ -14366,7 +14363,7 @@
         <v>1034</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="C3" s="38">
         <v>1.2</v>
@@ -14383,7 +14380,7 @@
         <v>1035</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="C4" s="38">
         <v>1.4</v>
@@ -14400,7 +14397,7 @@
         <v>400</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C5" s="38">
         <v>1</v>
@@ -16615,7 +16612,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="48" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B59" s="48">
         <v>9297</v>
@@ -18911,7 +18908,7 @@
         <v>1021</v>
       </c>
       <c r="B7" s="57" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="C7" s="56">
         <v>1</v>
@@ -18928,7 +18925,7 @@
         <v>1022</v>
       </c>
       <c r="B8" s="57" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="C8" s="56">
         <v>1.1000000000000001</v>
@@ -18945,7 +18942,7 @@
         <v>1023</v>
       </c>
       <c r="B9" s="57" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="C9" s="56">
         <v>1.3</v>
@@ -18962,7 +18959,7 @@
         <v>1024</v>
       </c>
       <c r="B10" s="56" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="C10" s="56">
         <v>1.5</v>
@@ -18979,7 +18976,7 @@
         <v>400</v>
       </c>
       <c r="B11" s="56" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C11" s="56">
         <v>1</v>
@@ -19004,7 +19001,7 @@
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -19108,7 +19105,7 @@
         <v>594</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="C6" s="48">
         <v>1</v>
@@ -19122,10 +19119,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="48" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="B7" s="48" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="C7" s="48">
         <v>1.2</v>
@@ -19139,10 +19136,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="48" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="B8" s="48" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="C8" s="48">
         <v>1.4</v>
@@ -19159,7 +19156,7 @@
         <v>400</v>
       </c>
       <c r="B9" s="48" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C9" s="48">
         <v>1</v>
@@ -20681,7 +20678,7 @@
   </sheetPr>
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -22706,8 +22703,8 @@
   </sheetPr>
   <dimension ref="A1:C148"/>
   <sheetViews>
-    <sheetView topLeftCell="A136" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E120" sqref="E120"/>
+    <sheetView topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23040,7 +23037,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="48" t="s">
-        <v>1076</v>
+        <v>1109</v>
       </c>
       <c r="B35" s="48"/>
       <c r="C35" s="48">
@@ -25715,27 +25712,27 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="B1" s="46" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1" s="46" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="D1" s="46" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="E1" s="46" t="s">
         <v>1083</v>
-      </c>
-      <c r="E1" s="46" t="s">
-        <v>1084</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="C2" s="47">
         <v>1</v>
@@ -25749,10 +25746,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="C3" s="47">
         <v>1.3</v>
@@ -25766,10 +25763,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="C4" s="47">
         <v>1.6</v>
@@ -25786,7 +25783,7 @@
         <v>400</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C5" s="47">
         <v>1</v>
@@ -25825,27 +25822,27 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="B1" s="46" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1" s="46" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="D1" s="46" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="E1" s="46" t="s">
         <v>1083</v>
-      </c>
-      <c r="E1" s="46" t="s">
-        <v>1084</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="C2" s="47">
         <v>1</v>
@@ -25859,10 +25856,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="C3" s="47">
         <v>1.3</v>
@@ -25876,10 +25873,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="C4" s="47">
         <v>1.6</v>
@@ -25896,7 +25893,7 @@
         <v>400</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C5" s="47">
         <v>1</v>
@@ -25935,27 +25932,27 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="B1" s="46" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1" s="46" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="D1" s="46" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="E1" s="46" t="s">
         <v>1083</v>
-      </c>
-      <c r="E1" s="46" t="s">
-        <v>1084</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="C2" s="47">
         <v>1</v>
@@ -25969,10 +25966,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="C3" s="47">
         <v>1.1000000000000001</v>
@@ -25986,10 +25983,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="C4" s="47">
         <v>1.5</v>
@@ -26006,7 +26003,7 @@
         <v>400</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C5" s="47">
         <v>1</v>
@@ -26045,27 +26042,27 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B1" s="46" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1" s="46" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="D1" s="46" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="E1" s="46" t="s">
         <v>1083</v>
-      </c>
-      <c r="E1" s="46" t="s">
-        <v>1084</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="C2" s="47">
         <v>1</v>
@@ -26079,10 +26076,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="C3" s="47">
         <v>1.3</v>
@@ -26096,10 +26093,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="C4" s="47">
         <v>1.6</v>
@@ -26116,7 +26113,7 @@
         <v>400</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C5" s="47">
         <v>1</v>
@@ -26155,27 +26152,27 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B1" s="46" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1" s="46" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="D1" s="46" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="E1" s="46" t="s">
         <v>1083</v>
-      </c>
-      <c r="E1" s="46" t="s">
-        <v>1084</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="C2" s="54">
         <v>1</v>
@@ -26189,10 +26186,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="C3" s="55">
         <v>1.1000000000000001</v>
@@ -26206,10 +26203,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="C4" s="54">
         <v>1.3</v>
@@ -26223,10 +26220,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="C5" s="54">
         <v>1.5</v>
@@ -26240,10 +26237,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="C6" s="54">
         <v>1.6</v>
@@ -26260,7 +26257,7 @@
         <v>400</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C7" s="54">
         <v>1</v>
@@ -26299,27 +26296,27 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="B1" s="46" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1" s="46" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="D1" s="46" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="E1" s="46" t="s">
         <v>1083</v>
-      </c>
-      <c r="E1" s="46" t="s">
-        <v>1084</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="C2" s="54">
         <v>1</v>
@@ -26333,10 +26330,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="B3" s="51" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="C3" s="55">
         <v>1.1000000000000001</v>
@@ -26350,10 +26347,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="B4" s="51" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="C4" s="54">
         <v>1.3</v>
@@ -26367,10 +26364,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="C5" s="54">
         <v>1.5</v>
@@ -26384,10 +26381,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C6" s="54">
         <v>1.6</v>
@@ -26404,7 +26401,7 @@
         <v>400</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C7" s="54">
         <v>1</v>
@@ -26443,27 +26440,27 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="B1" s="46" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1" s="46" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="D1" s="46" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="E1" s="46" t="s">
         <v>1083</v>
-      </c>
-      <c r="E1" s="46" t="s">
-        <v>1084</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="C2" s="54">
         <v>1</v>
@@ -26477,10 +26474,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="C3" s="54">
         <v>1.1000000000000001</v>
@@ -26494,10 +26491,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="C4" s="54">
         <v>1.3</v>
@@ -26511,10 +26508,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="C5" s="54">
         <v>1.5</v>
@@ -26531,7 +26528,7 @@
         <v>400</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="C6" s="54">
         <v>1</v>
@@ -26570,27 +26567,27 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="B1" s="46" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1" s="46" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="D1" s="46" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="E1" s="46" t="s">
         <v>1083</v>
-      </c>
-      <c r="E1" s="46" t="s">
-        <v>1084</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="C2" s="54">
         <v>1</v>
@@ -26604,10 +26601,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="B3" s="51" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="C3" s="55">
         <v>1.1000000000000001</v>
@@ -26621,10 +26618,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="B4" s="51" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C4" s="54">
         <v>1.3</v>
@@ -26638,10 +26635,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C5" s="54">
         <v>1.5</v>
@@ -26655,10 +26652,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="C6" s="54">
         <v>1.6</v>
@@ -26675,7 +26672,7 @@
         <v>400</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="C7" s="54">
         <v>1</v>
@@ -26714,27 +26711,27 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="B1" s="46" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1" s="46" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="D1" s="46" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="E1" s="46" t="s">
         <v>1083</v>
-      </c>
-      <c r="E1" s="46" t="s">
-        <v>1084</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="C2" s="54">
         <v>1</v>
@@ -26748,10 +26745,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="B3" s="51" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="C3" s="55">
         <v>1.1000000000000001</v>
@@ -26765,10 +26762,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="B4" s="51" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="C4" s="54">
         <v>1.3</v>
@@ -26782,10 +26779,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C5" s="54">
         <v>1.5</v>
@@ -26799,10 +26796,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="C6" s="54">
         <v>1.6</v>
@@ -26819,7 +26816,7 @@
         <v>400</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="C7" s="54">
         <v>1</v>
@@ -26858,27 +26855,27 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="B1" s="46" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1" s="46" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="D1" s="46" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="E1" s="46" t="s">
         <v>1083</v>
-      </c>
-      <c r="E1" s="46" t="s">
-        <v>1084</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="C2" s="54">
         <v>1</v>
@@ -26895,7 +26892,7 @@
         <v>1021</v>
       </c>
       <c r="B3" s="51" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="C3" s="55">
         <v>1.1000000000000001</v>
@@ -26912,7 +26909,7 @@
         <v>1022</v>
       </c>
       <c r="B4" s="51" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="C4" s="54">
         <v>1.3</v>
@@ -26926,10 +26923,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="C5" s="54">
         <v>1.5</v>
@@ -26946,7 +26943,7 @@
         <v>1031</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="C6" s="54">
         <v>1.6</v>
@@ -26963,7 +26960,7 @@
         <v>400</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="C7" s="54">
         <v>1</v>
@@ -32195,7 +32192,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="48" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B58" s="48">
         <v>15</v>
@@ -32847,7 +32844,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="48" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B39" s="48"/>
       <c r="C39" s="58">
@@ -32865,7 +32862,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="48" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B40" s="48"/>
       <c r="C40" s="48">
@@ -32883,7 +32880,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="48" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B41" s="48"/>
       <c r="C41" s="48">
@@ -33511,7 +33508,7 @@
         <v>1064</v>
       </c>
       <c r="B76" s="38" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="C76" s="38">
         <v>0</v>
@@ -33531,7 +33528,7 @@
         <v>1064</v>
       </c>
       <c r="B77" s="38" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="C77" s="38">
         <v>10</v>
@@ -33551,7 +33548,7 @@
         <v>1064</v>
       </c>
       <c r="B78" s="38" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="C78" s="38">
         <v>20</v>
@@ -35206,7 +35203,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="48" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="B58" s="59">
         <v>2.6027400000000001E-5</v>
@@ -35442,27 +35439,27 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="B1" s="43" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="C1" s="43" t="s">
+        <v>1221</v>
+      </c>
+      <c r="D1" s="43" t="s">
         <v>1222</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="E1" s="43" t="s">
         <v>1223</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>1224</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B2" s="43" t="s">
         <v>1218</v>
-      </c>
-      <c r="B2" s="43" t="s">
-        <v>1219</v>
       </c>
       <c r="C2" s="43">
         <v>0.7</v>
@@ -35476,10 +35473,10 @@
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="43" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="B3" s="43" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="C3" s="43">
         <v>0.9</v>
@@ -35493,10 +35490,10 @@
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="43" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="B4" s="43" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="C4" s="43">
         <v>1.2</v>
@@ -37265,7 +37262,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="48" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B5" s="48"/>
       <c r="C5" s="58">
@@ -37283,7 +37280,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="48" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B6" s="48"/>
       <c r="C6" s="48">
@@ -37301,7 +37298,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="48" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B7" s="48"/>
       <c r="C7" s="48">
@@ -37967,7 +37964,7 @@
         <v>1064</v>
       </c>
       <c r="B46" s="38" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="C46" s="38">
         <v>0</v>
@@ -37987,7 +37984,7 @@
         <v>1064</v>
       </c>
       <c r="B47" s="38" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="C47" s="38">
         <v>10</v>
@@ -38007,7 +38004,7 @@
         <v>1064</v>
       </c>
       <c r="B48" s="38" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="C48" s="38">
         <v>20</v>
@@ -40775,7 +40772,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="48" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B23" s="48">
         <v>15589.91</v>
@@ -41972,7 +41969,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="48" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B23" s="48">
         <v>2.2230000000000001E-3</v>
@@ -44809,7 +44806,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="48" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B86" s="48" t="s">
         <v>165</v>
@@ -44832,7 +44829,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="48" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B87" s="48" t="s">
         <v>167</v>
@@ -44855,7 +44852,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="48" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B88" s="48" t="s">
         <v>168</v>
@@ -44878,7 +44875,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="48" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B89" s="48" t="s">
         <v>169</v>
@@ -48978,7 +48975,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="48" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B23" s="48">
         <v>3.9964920000000001E-2</v>
@@ -49843,7 +49840,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="48" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B23" s="48">
         <v>4.3099999999999999E-2</v>
@@ -52683,7 +52680,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="48" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B86" s="48" t="s">
         <v>165</v>
@@ -52706,7 +52703,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="48" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B87" s="48" t="s">
         <v>167</v>
@@ -52729,7 +52726,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="48" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B88" s="48" t="s">
         <v>168</v>
@@ -52752,7 +52749,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="48" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B89" s="48" t="s">
         <v>169</v>
@@ -56649,7 +56646,7 @@
   </sheetPr>
   <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -56838,7 +56835,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="48" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B23" s="49" t="s">
         <v>406</v>
@@ -64566,7 +64563,7 @@
         <v>1048</v>
       </c>
       <c r="B8" s="56" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="C8" s="56">
         <v>0.9</v>
@@ -64580,10 +64577,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="56" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B9" s="56" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="C9" s="56">
         <v>1</v>
@@ -64597,10 +64594,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="56" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="B10" s="57" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="C10" s="56">
         <v>1.1000000000000001</v>
@@ -64617,7 +64614,7 @@
         <v>1034</v>
       </c>
       <c r="B11" s="57" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="C11" s="56">
         <v>1.25</v>
@@ -64634,7 +64631,7 @@
         <v>1035</v>
       </c>
       <c r="B12" s="57" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="C12" s="56">
         <v>1.4</v>
@@ -64651,7 +64648,7 @@
         <v>400</v>
       </c>
       <c r="B13" s="56" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C13" s="56">
         <v>1</v>
@@ -64792,10 +64789,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="56" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B7" s="56" t="s">
         <v>1229</v>
-      </c>
-      <c r="B7" s="56" t="s">
-        <v>1230</v>
       </c>
       <c r="C7" s="56">
         <v>1</v>
@@ -64809,10 +64806,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="56" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B8" s="57" t="s">
         <v>1231</v>
-      </c>
-      <c r="B8" s="57" t="s">
-        <v>1232</v>
       </c>
       <c r="C8" s="56">
         <v>1</v>
@@ -64829,7 +64826,7 @@
         <v>1034</v>
       </c>
       <c r="B9" s="57" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C9" s="56">
         <v>1.1000000000000001</v>
@@ -64846,7 +64843,7 @@
         <v>1035</v>
       </c>
       <c r="B10" s="57" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="C10" s="56">
         <v>1.3</v>
@@ -64863,7 +64860,7 @@
         <v>400</v>
       </c>
       <c r="B11" s="56" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C11" s="56">
         <v>1</v>

</xml_diff>